<commit_message>
Update code - add text to image
</commit_message>
<xml_diff>
--- a/Historical Figures List.xlsx
+++ b/Historical Figures List.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:H26"/>
+  <dimension ref="A1:I81"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -474,6 +474,11 @@
           <t>Youtube_Video_Posted</t>
         </is>
       </c>
+      <c r="I1" s="1" t="inlineStr">
+        <is>
+          <t>Prompt</t>
+        </is>
+      </c>
     </row>
     <row r="2">
       <c r="A2" t="n">
@@ -514,6 +519,11 @@
           <t>Yes</t>
         </is>
       </c>
+      <c r="I2" t="inlineStr">
+        <is>
+          <t>Generate 10 pretty long and interesting facts about Albert Einstein</t>
+        </is>
+      </c>
     </row>
     <row r="3">
       <c r="A3" t="n">
@@ -554,6 +564,11 @@
           <t>No</t>
         </is>
       </c>
+      <c r="I3" t="inlineStr">
+        <is>
+          <t>Generate 10 pretty long and interesting facts about Marie Curie</t>
+        </is>
+      </c>
     </row>
     <row r="4">
       <c r="A4" t="n">
@@ -594,6 +609,11 @@
           <t>No</t>
         </is>
       </c>
+      <c r="I4" t="inlineStr">
+        <is>
+          <t>Generate 10 pretty long and interesting facts about Leonardo da Vinci</t>
+        </is>
+      </c>
     </row>
     <row r="5">
       <c r="A5" t="n">
@@ -611,12 +631,12 @@
       </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t>No</t>
+          <t>Yes</t>
         </is>
       </c>
       <c r="E5" t="inlineStr">
         <is>
-          <t>No</t>
+          <t>Yes</t>
         </is>
       </c>
       <c r="F5" t="inlineStr">
@@ -632,6 +652,11 @@
       <c r="H5" t="inlineStr">
         <is>
           <t>No</t>
+        </is>
+      </c>
+      <c r="I5" t="inlineStr">
+        <is>
+          <t>Generate 10 pretty long and interesting facts about Mahatma Gandhi</t>
         </is>
       </c>
     </row>
@@ -651,12 +676,12 @@
       </c>
       <c r="D6" t="inlineStr">
         <is>
-          <t>No</t>
+          <t>Yes</t>
         </is>
       </c>
       <c r="E6" t="inlineStr">
         <is>
-          <t>No</t>
+          <t>Yes</t>
         </is>
       </c>
       <c r="F6" t="inlineStr">
@@ -672,6 +697,11 @@
       <c r="H6" t="inlineStr">
         <is>
           <t>No</t>
+        </is>
+      </c>
+      <c r="I6" t="inlineStr">
+        <is>
+          <t>Generate 10 pretty long and interesting facts about Rosa Parks</t>
         </is>
       </c>
     </row>
@@ -691,12 +721,12 @@
       </c>
       <c r="D7" t="inlineStr">
         <is>
-          <t>No</t>
+          <t>Yes</t>
         </is>
       </c>
       <c r="E7" t="inlineStr">
         <is>
-          <t>No</t>
+          <t>Yes</t>
         </is>
       </c>
       <c r="F7" t="inlineStr">
@@ -712,6 +742,11 @@
       <c r="H7" t="inlineStr">
         <is>
           <t>No</t>
+        </is>
+      </c>
+      <c r="I7" t="inlineStr">
+        <is>
+          <t>Generate 10 pretty long and interesting facts about Isaac Newton</t>
         </is>
       </c>
     </row>
@@ -731,12 +766,12 @@
       </c>
       <c r="D8" t="inlineStr">
         <is>
-          <t>No</t>
+          <t>Yes</t>
         </is>
       </c>
       <c r="E8" t="inlineStr">
         <is>
-          <t>No</t>
+          <t>Yes</t>
         </is>
       </c>
       <c r="F8" t="inlineStr">
@@ -752,6 +787,11 @@
       <c r="H8" t="inlineStr">
         <is>
           <t>No</t>
+        </is>
+      </c>
+      <c r="I8" t="inlineStr">
+        <is>
+          <t>Generate 10 pretty long and interesting facts about Cleopatra</t>
         </is>
       </c>
     </row>
@@ -771,27 +811,32 @@
       </c>
       <c r="D9" t="inlineStr">
         <is>
-          <t>No</t>
+          <t>Yes</t>
         </is>
       </c>
       <c r="E9" t="inlineStr">
         <is>
-          <t>No</t>
+          <t>Yes</t>
         </is>
       </c>
       <c r="F9" t="inlineStr">
         <is>
-          <t>No</t>
+          <t>Yes</t>
         </is>
       </c>
       <c r="G9" t="inlineStr">
         <is>
-          <t>No</t>
+          <t>Yes</t>
         </is>
       </c>
       <c r="H9" t="inlineStr">
         <is>
           <t>No</t>
+        </is>
+      </c>
+      <c r="I9" t="inlineStr">
+        <is>
+          <t>Generate 10 pretty long and interesting facts about Nelson Mandela</t>
         </is>
       </c>
     </row>
@@ -811,12 +856,12 @@
       </c>
       <c r="D10" t="inlineStr">
         <is>
-          <t>No</t>
+          <t>Yes</t>
         </is>
       </c>
       <c r="E10" t="inlineStr">
         <is>
-          <t>No</t>
+          <t>Yes</t>
         </is>
       </c>
       <c r="F10" t="inlineStr">
@@ -832,6 +877,11 @@
       <c r="H10" t="inlineStr">
         <is>
           <t>No</t>
+        </is>
+      </c>
+      <c r="I10" t="inlineStr">
+        <is>
+          <t>Generate 10 pretty long and interesting facts about William Shakespeare</t>
         </is>
       </c>
     </row>
@@ -851,12 +901,12 @@
       </c>
       <c r="D11" t="inlineStr">
         <is>
-          <t>No</t>
+          <t>Yes</t>
         </is>
       </c>
       <c r="E11" t="inlineStr">
         <is>
-          <t>No</t>
+          <t>Yes</t>
         </is>
       </c>
       <c r="F11" t="inlineStr">
@@ -872,6 +922,11 @@
       <c r="H11" t="inlineStr">
         <is>
           <t>No</t>
+        </is>
+      </c>
+      <c r="I11" t="inlineStr">
+        <is>
+          <t>Generate 10 pretty long and interesting facts about Amelia Earhart</t>
         </is>
       </c>
     </row>
@@ -891,12 +946,12 @@
       </c>
       <c r="D12" t="inlineStr">
         <is>
-          <t>No</t>
+          <t>Yes</t>
         </is>
       </c>
       <c r="E12" t="inlineStr">
         <is>
-          <t>No</t>
+          <t>Yes</t>
         </is>
       </c>
       <c r="F12" t="inlineStr">
@@ -912,6 +967,11 @@
       <c r="H12" t="inlineStr">
         <is>
           <t>No</t>
+        </is>
+      </c>
+      <c r="I12" t="inlineStr">
+        <is>
+          <t>Generate 10 pretty long and interesting facts about Galileo Galilei</t>
         </is>
       </c>
     </row>
@@ -954,19 +1014,24 @@
           <t>No</t>
         </is>
       </c>
+      <c r="I13" t="inlineStr">
+        <is>
+          <t>Generate 10 pretty long and interesting facts about Joan of Arc</t>
+        </is>
+      </c>
     </row>
     <row r="14">
       <c r="A14" t="n">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>Leonardo da Vinci</t>
+          <t>Alexander the Great</t>
         </is>
       </c>
       <c r="C14" t="inlineStr">
         <is>
-          <t>Polymath genius, excelling in art, science, and engineering.</t>
+          <t>Ancient Greek military genius, conquered vast territories.</t>
         </is>
       </c>
       <c r="D14" t="inlineStr">
@@ -976,7 +1041,7 @@
       </c>
       <c r="E14" t="inlineStr">
         <is>
-          <t>Yes</t>
+          <t>No</t>
         </is>
       </c>
       <c r="F14" t="inlineStr">
@@ -992,21 +1057,26 @@
       <c r="H14" t="inlineStr">
         <is>
           <t>No</t>
+        </is>
+      </c>
+      <c r="I14" t="inlineStr">
+        <is>
+          <t>Generate 10 pretty long and interesting facts about Alexander the Great</t>
         </is>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="n">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>Alexander the Great</t>
+          <t>Thomas Edison</t>
         </is>
       </c>
       <c r="C15" t="inlineStr">
         <is>
-          <t>Ancient Greek military genius, conquered vast territories.</t>
+          <t>Inventor and businessman, held over a thousand patents.</t>
         </is>
       </c>
       <c r="D15" t="inlineStr">
@@ -1032,21 +1102,26 @@
       <c r="H15" t="inlineStr">
         <is>
           <t>No</t>
+        </is>
+      </c>
+      <c r="I15" t="inlineStr">
+        <is>
+          <t>Generate 10 pretty long and interesting facts about Thomas Edison</t>
         </is>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="n">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="B16" t="inlineStr">
         <is>
-          <t>Thomas Edison</t>
+          <t>Martin Luther King Jr.</t>
         </is>
       </c>
       <c r="C16" t="inlineStr">
         <is>
-          <t>Inventor and businessman, held over a thousand patents.</t>
+          <t>Leader of the civil rights movement in the United States.</t>
         </is>
       </c>
       <c r="D16" t="inlineStr">
@@ -1072,21 +1147,26 @@
       <c r="H16" t="inlineStr">
         <is>
           <t>No</t>
+        </is>
+      </c>
+      <c r="I16" t="inlineStr">
+        <is>
+          <t>Generate 10 pretty long and interesting facts about Martin Luther King Jr.</t>
         </is>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="n">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="B17" t="inlineStr">
         <is>
-          <t>Martin Luther King Jr.</t>
+          <t>Marie Antoinette</t>
         </is>
       </c>
       <c r="C17" t="inlineStr">
         <is>
-          <t>Leader of the civil rights movement in the United States.</t>
+          <t>Queen consort of France during the French Revolution.</t>
         </is>
       </c>
       <c r="D17" t="inlineStr">
@@ -1112,21 +1192,26 @@
       <c r="H17" t="inlineStr">
         <is>
           <t>No</t>
+        </is>
+      </c>
+      <c r="I17" t="inlineStr">
+        <is>
+          <t>Generate 10 pretty long and interesting facts about Marie Antoinette</t>
         </is>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="n">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="B18" t="inlineStr">
         <is>
-          <t>Marie Antoinette</t>
+          <t>Winston Churchill</t>
         </is>
       </c>
       <c r="C18" t="inlineStr">
         <is>
-          <t>Queen consort of France during the French Revolution.</t>
+          <t>British Prime Minister during World War II.</t>
         </is>
       </c>
       <c r="D18" t="inlineStr">
@@ -1152,21 +1237,26 @@
       <c r="H18" t="inlineStr">
         <is>
           <t>No</t>
+        </is>
+      </c>
+      <c r="I18" t="inlineStr">
+        <is>
+          <t>Generate 10 pretty long and interesting facts about Winston Churchill</t>
         </is>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="n">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="B19" t="inlineStr">
         <is>
-          <t>Winston Churchill</t>
+          <t>Socrates</t>
         </is>
       </c>
       <c r="C19" t="inlineStr">
         <is>
-          <t>British Prime Minister during World War II.</t>
+          <t>Greek philosopher, known for his Socratic method of questioning.</t>
         </is>
       </c>
       <c r="D19" t="inlineStr">
@@ -1192,21 +1282,26 @@
       <c r="H19" t="inlineStr">
         <is>
           <t>No</t>
+        </is>
+      </c>
+      <c r="I19" t="inlineStr">
+        <is>
+          <t>Generate 10 pretty long and interesting facts about Socrates</t>
         </is>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="n">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="B20" t="inlineStr">
         <is>
-          <t>Socrates</t>
+          <t>Frida Kahlo</t>
         </is>
       </c>
       <c r="C20" t="inlineStr">
         <is>
-          <t>Greek philosopher, known for his Socratic method of questioning.</t>
+          <t>Renowned Mexican painter and feminist icon.</t>
         </is>
       </c>
       <c r="D20" t="inlineStr">
@@ -1232,21 +1327,26 @@
       <c r="H20" t="inlineStr">
         <is>
           <t>No</t>
+        </is>
+      </c>
+      <c r="I20" t="inlineStr">
+        <is>
+          <t>Generate 10 pretty long and interesting facts about Frida Kahlo</t>
         </is>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="n">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="B21" t="inlineStr">
         <is>
-          <t>Frida Kahlo</t>
+          <t>Genghis Khan</t>
         </is>
       </c>
       <c r="C21" t="inlineStr">
         <is>
-          <t>Renowned Mexican painter and feminist icon.</t>
+          <t>Founder and emperor of the Mongol Empire.</t>
         </is>
       </c>
       <c r="D21" t="inlineStr">
@@ -1272,21 +1372,26 @@
       <c r="H21" t="inlineStr">
         <is>
           <t>No</t>
+        </is>
+      </c>
+      <c r="I21" t="inlineStr">
+        <is>
+          <t>Generate 10 pretty long and interesting facts about Genghis Khan</t>
         </is>
       </c>
     </row>
     <row r="22">
       <c r="A22" t="n">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="B22" t="inlineStr">
         <is>
-          <t>Genghis Khan</t>
+          <t>Rosa Luxemburg</t>
         </is>
       </c>
       <c r="C22" t="inlineStr">
         <is>
-          <t>Founder and emperor of the Mongol Empire.</t>
+          <t>Marxist theorist and revolutionary socialist.</t>
         </is>
       </c>
       <c r="D22" t="inlineStr">
@@ -1312,21 +1417,26 @@
       <c r="H22" t="inlineStr">
         <is>
           <t>No</t>
+        </is>
+      </c>
+      <c r="I22" t="inlineStr">
+        <is>
+          <t>Generate 10 pretty long and interesting facts about Rosa Luxemburg</t>
         </is>
       </c>
     </row>
     <row r="23">
       <c r="A23" t="n">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="B23" t="inlineStr">
         <is>
-          <t>Rosa Luxemburg</t>
+          <t>Hatshepsut</t>
         </is>
       </c>
       <c r="C23" t="inlineStr">
         <is>
-          <t>Marxist theorist and revolutionary socialist.</t>
+          <t>Ancient Egyptian queen, one of the longest-reigning female pharaohs.</t>
         </is>
       </c>
       <c r="D23" t="inlineStr">
@@ -1352,21 +1462,26 @@
       <c r="H23" t="inlineStr">
         <is>
           <t>No</t>
+        </is>
+      </c>
+      <c r="I23" t="inlineStr">
+        <is>
+          <t>Generate 10 pretty long and interesting facts about Hatshepsut</t>
         </is>
       </c>
     </row>
     <row r="24">
       <c r="A24" t="n">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="B24" t="inlineStr">
         <is>
-          <t>Hatshepsut</t>
+          <t>Nikola Tesla</t>
         </is>
       </c>
       <c r="C24" t="inlineStr">
         <is>
-          <t>Ancient Egyptian queen, one of the longest-reigning female pharaohs.</t>
+          <t>Electrical engineer and inventor, known for AC power system.</t>
         </is>
       </c>
       <c r="D24" t="inlineStr">
@@ -1392,21 +1507,26 @@
       <c r="H24" t="inlineStr">
         <is>
           <t>No</t>
+        </is>
+      </c>
+      <c r="I24" t="inlineStr">
+        <is>
+          <t>Generate 10 pretty long and interesting facts about Nikola Tesla</t>
         </is>
       </c>
     </row>
     <row r="25">
       <c r="A25" t="n">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="B25" t="inlineStr">
         <is>
-          <t>Nikola Tesla</t>
+          <t>Confucius</t>
         </is>
       </c>
       <c r="C25" t="inlineStr">
         <is>
-          <t>Electrical engineer and inventor, known for AC power system.</t>
+          <t>Chinese philosopher, influential figure in Eastern thought.</t>
         </is>
       </c>
       <c r="D25" t="inlineStr">
@@ -1432,21 +1552,26 @@
       <c r="H25" t="inlineStr">
         <is>
           <t>No</t>
+        </is>
+      </c>
+      <c r="I25" t="inlineStr">
+        <is>
+          <t>Generate 10 pretty long and interesting facts about Confucius</t>
         </is>
       </c>
     </row>
     <row r="26">
       <c r="A26" t="n">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="B26" t="inlineStr">
         <is>
-          <t>Confucius</t>
+          <t>Queen Elizabeth I</t>
         </is>
       </c>
       <c r="C26" t="inlineStr">
         <is>
-          <t>Chinese philosopher, influential figure in Eastern thought.</t>
+          <t>Queen of England during the Elizabethan era, known for her strong leadership and support of the arts and exploration.</t>
         </is>
       </c>
       <c r="D26" t="inlineStr">
@@ -1472,6 +1597,2486 @@
       <c r="H26" t="inlineStr">
         <is>
           <t>No</t>
+        </is>
+      </c>
+      <c r="I26" t="inlineStr">
+        <is>
+          <t>Generate 10 pretty long and interesting facts about Queen Elizabeth I</t>
+        </is>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" t="n">
+        <v>27</v>
+      </c>
+      <c r="B27" t="inlineStr">
+        <is>
+          <t>Karl Marx</t>
+        </is>
+      </c>
+      <c r="C27" t="inlineStr">
+        <is>
+          <t>German philosopher, economist, and author of "The Communist Manifesto" and "Das Kapital," influential in the development of socialist and communist theories.</t>
+        </is>
+      </c>
+      <c r="D27" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="E27" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="F27" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="G27" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="H27" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="I27" t="inlineStr">
+        <is>
+          <t>Generate 10 pretty long and interesting facts about Karl Marx</t>
+        </is>
+      </c>
+    </row>
+    <row r="28">
+      <c r="A28" t="n">
+        <v>28</v>
+      </c>
+      <c r="B28" t="inlineStr">
+        <is>
+          <t>Abraham Lincoln</t>
+        </is>
+      </c>
+      <c r="C28" t="inlineStr">
+        <is>
+          <t>16th President of the United States, known for his leadership during the American Civil War and the abolition of slavery through the Emancipation Proclamation.</t>
+        </is>
+      </c>
+      <c r="D28" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="E28" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="F28" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="G28" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="H28" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="I28" t="inlineStr">
+        <is>
+          <t>Generate 10 pretty long and interesting facts about Abraham Lincoln</t>
+        </is>
+      </c>
+    </row>
+    <row r="29">
+      <c r="A29" t="n">
+        <v>29</v>
+      </c>
+      <c r="B29" t="inlineStr">
+        <is>
+          <t>Aristotle</t>
+        </is>
+      </c>
+      <c r="C29" t="inlineStr">
+        <is>
+          <t>Ancient Greek philosopher and polymath, known for his contributions to logic, ethics, politics, biology, and numerous other fields of study.</t>
+        </is>
+      </c>
+      <c r="D29" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="E29" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="F29" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="G29" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="H29" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="I29" t="inlineStr">
+        <is>
+          <t>Generate 10 pretty long and interesting facts about Aristotle</t>
+        </is>
+      </c>
+    </row>
+    <row r="30">
+      <c r="A30" t="n">
+        <v>32</v>
+      </c>
+      <c r="B30" t="inlineStr">
+        <is>
+          <t>George Washington</t>
+        </is>
+      </c>
+      <c r="C30" t="inlineStr">
+        <is>
+          <t>Founding Father and the first President of the United States, instrumental in leading the American Revolutionary War and shaping the early American government.</t>
+        </is>
+      </c>
+      <c r="D30" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="E30" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="F30" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="G30" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="H30" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="I30" t="inlineStr">
+        <is>
+          <t>Generate 10 pretty long and interesting facts about George Washington</t>
+        </is>
+      </c>
+    </row>
+    <row r="31">
+      <c r="A31" t="n">
+        <v>34</v>
+      </c>
+      <c r="B31" t="inlineStr">
+        <is>
+          <t>Julius Caesar</t>
+        </is>
+      </c>
+      <c r="C31" t="inlineStr">
+        <is>
+          <t>Roman military and political leader, played a critical role in the transformation of the Roman Republic into the Roman Empire and left a lasting impact on Roman history.</t>
+        </is>
+      </c>
+      <c r="D31" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="E31" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="F31" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="G31" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="H31" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="I31" t="inlineStr">
+        <is>
+          <t>Generate 10 pretty long and interesting facts about Julius Caesar</t>
+        </is>
+      </c>
+    </row>
+    <row r="32">
+      <c r="A32" t="n">
+        <v>35</v>
+      </c>
+      <c r="B32" t="inlineStr">
+        <is>
+          <t>Alan Turing</t>
+        </is>
+      </c>
+      <c r="C32" t="inlineStr">
+        <is>
+          <t>Considered to be the father of theoretical computer science and artificial intelligence.</t>
+        </is>
+      </c>
+      <c r="D32" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="E32" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="F32" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="G32" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="H32" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="I32" t="inlineStr">
+        <is>
+          <t>Generate 10 pretty long and interesting facts about Alan Turing</t>
+        </is>
+      </c>
+    </row>
+    <row r="33">
+      <c r="A33" t="n">
+        <v>36</v>
+      </c>
+      <c r="B33" t="inlineStr">
+        <is>
+          <t>Benjamin Franklin</t>
+        </is>
+      </c>
+      <c r="C33" t="inlineStr">
+        <is>
+          <t>One of the Founding Fathers of the United States, he was a major contributor to the American Revolution.</t>
+        </is>
+      </c>
+      <c r="D33" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="E33" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="F33" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="G33" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="H33" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="I33" t="inlineStr">
+        <is>
+          <t>Generate 10 pretty long and interesting facts about Benjamin Franklin</t>
+        </is>
+      </c>
+    </row>
+    <row r="34">
+      <c r="A34" t="n">
+        <v>37</v>
+      </c>
+      <c r="B34" t="inlineStr">
+        <is>
+          <t>Charles Darwin</t>
+        </is>
+      </c>
+      <c r="C34" t="inlineStr">
+        <is>
+          <t>Developed the theory of evolution by natural selection, which is one of the most important scientific theories of all time.</t>
+        </is>
+      </c>
+      <c r="D34" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="E34" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="F34" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="G34" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="H34" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="I34" t="inlineStr">
+        <is>
+          <t>Generate 10 pretty long and interesting facts about Charles Darwin</t>
+        </is>
+      </c>
+    </row>
+    <row r="35">
+      <c r="A35" t="n">
+        <v>38</v>
+      </c>
+      <c r="B35" t="inlineStr">
+        <is>
+          <t>Christopher Columbus</t>
+        </is>
+      </c>
+      <c r="C35" t="inlineStr">
+        <is>
+          <t>Discovered the Americas in 1492, which had a profound impact on world history.</t>
+        </is>
+      </c>
+      <c r="D35" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="E35" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="F35" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="G35" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="H35" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="I35" t="inlineStr">
+        <is>
+          <t>Generate 10 pretty long and interesting facts about Christopher Columbus</t>
+        </is>
+      </c>
+    </row>
+    <row r="36">
+      <c r="A36" t="n">
+        <v>40</v>
+      </c>
+      <c r="B36" t="inlineStr">
+        <is>
+          <t>Eleanor Roosevelt</t>
+        </is>
+      </c>
+      <c r="C36" t="inlineStr">
+        <is>
+          <t>First Lady of the United States from 1933 to 1945, she was a leading advocate for human rights.</t>
+        </is>
+      </c>
+      <c r="D36" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="E36" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="F36" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="G36" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="H36" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="I36" t="inlineStr">
+        <is>
+          <t>Generate 10 pretty long and interesting facts about Eleanor Roosevelt</t>
+        </is>
+      </c>
+    </row>
+    <row r="37">
+      <c r="A37" t="n">
+        <v>42</v>
+      </c>
+      <c r="B37" t="inlineStr">
+        <is>
+          <t>Stephen Hawking</t>
+        </is>
+      </c>
+      <c r="C37" t="inlineStr">
+        <is>
+          <t>Developed theories about black holes and the Big Bang.</t>
+        </is>
+      </c>
+      <c r="D37" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="E37" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="F37" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="G37" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="H37" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="I37" t="inlineStr">
+        <is>
+          <t>Generate 10 pretty long and interesting facts about Stephen Hawking</t>
+        </is>
+      </c>
+    </row>
+    <row r="38">
+      <c r="A38" t="n">
+        <v>43</v>
+      </c>
+      <c r="B38" t="inlineStr">
+        <is>
+          <t>Jane Austen</t>
+        </is>
+      </c>
+      <c r="C38" t="inlineStr">
+        <is>
+          <t>One of the most celebrated novelists in English literature.</t>
+        </is>
+      </c>
+      <c r="D38" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="E38" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="F38" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="G38" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="H38" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="I38" t="inlineStr">
+        <is>
+          <t>Generate 10 pretty long and interesting facts about Jane Austen</t>
+        </is>
+      </c>
+    </row>
+    <row r="39">
+      <c r="A39" t="n">
+        <v>45</v>
+      </c>
+      <c r="B39" t="inlineStr">
+        <is>
+          <t>Martin Luther</t>
+        </is>
+      </c>
+      <c r="C39" t="inlineStr">
+        <is>
+          <t>Started the Protestant Reformation, which had a profound impact on Christianity.</t>
+        </is>
+      </c>
+      <c r="D39" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="E39" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="F39" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="G39" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="H39" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="I39" t="inlineStr">
+        <is>
+          <t>Generate 10 pretty long and interesting facts about Martin Luther</t>
+        </is>
+      </c>
+    </row>
+    <row r="40">
+      <c r="A40" t="n">
+        <v>47</v>
+      </c>
+      <c r="B40" t="inlineStr">
+        <is>
+          <t>Plato</t>
+        </is>
+      </c>
+      <c r="C40" t="inlineStr">
+        <is>
+          <t>One of the most influential philosophers in Western history.</t>
+        </is>
+      </c>
+      <c r="D40" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="E40" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="F40" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="G40" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="H40" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="I40" t="inlineStr">
+        <is>
+          <t>Generate 10 pretty long and interesting facts about Plato</t>
+        </is>
+      </c>
+    </row>
+    <row r="41">
+      <c r="A41" t="n">
+        <v>48</v>
+      </c>
+      <c r="B41" t="inlineStr">
+        <is>
+          <t>Pythagoras</t>
+        </is>
+      </c>
+      <c r="C41" t="inlineStr">
+        <is>
+          <t>Developed the Pythagorean theorem, which is one of the most important mathematical theorems of all time.</t>
+        </is>
+      </c>
+      <c r="D41" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="E41" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="F41" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="G41" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="H41" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="I41" t="inlineStr">
+        <is>
+          <t>Generate 10 pretty long and interesting facts about Pythagoras</t>
+        </is>
+      </c>
+    </row>
+    <row r="42">
+      <c r="A42" t="n">
+        <v>50</v>
+      </c>
+      <c r="B42" t="inlineStr">
+        <is>
+          <t>Theodore Roosevelt</t>
+        </is>
+      </c>
+      <c r="C42" t="inlineStr">
+        <is>
+          <t>26th President of the United States, he was a leading advocate for environmental protection.</t>
+        </is>
+      </c>
+      <c r="D42" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="E42" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="F42" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="G42" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="H42" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="I42" t="inlineStr">
+        <is>
+          <t>Generate 10 pretty long and interesting facts about Theodore Roosevelt</t>
+        </is>
+      </c>
+    </row>
+    <row r="43">
+      <c r="A43" t="n">
+        <v>51</v>
+      </c>
+      <c r="B43" t="inlineStr">
+        <is>
+          <t>Thomas Jefferson</t>
+        </is>
+      </c>
+      <c r="C43" t="inlineStr">
+        <is>
+          <t>3rd President of the United States, he was a major contributor to the Declaration of Independence.</t>
+        </is>
+      </c>
+      <c r="D43" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="E43" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="F43" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="G43" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="H43" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="I43" t="inlineStr">
+        <is>
+          <t>Generate 10 pretty long and interesting facts about Thomas Jefferson</t>
+        </is>
+      </c>
+    </row>
+    <row r="44">
+      <c r="A44" t="n">
+        <v>52</v>
+      </c>
+      <c r="B44" t="inlineStr">
+        <is>
+          <t>Tupac Shakur</t>
+        </is>
+      </c>
+      <c r="C44" t="inlineStr">
+        <is>
+          <t>One of the most influential rappers of all time, he was also a successful actor.</t>
+        </is>
+      </c>
+      <c r="D44" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="E44" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="F44" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="G44" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="H44" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="I44" t="inlineStr">
+        <is>
+          <t>Generate 10 pretty long and interesting facts about Tupac Shakur</t>
+        </is>
+      </c>
+    </row>
+    <row r="45">
+      <c r="A45" t="n">
+        <v>53</v>
+      </c>
+      <c r="B45" t="inlineStr">
+        <is>
+          <t>Voltaire</t>
+        </is>
+      </c>
+      <c r="C45" t="inlineStr">
+        <is>
+          <t>One of the most important Enlightenment thinkers, he was a leading advocate for freedom of speech and religious tolerance.</t>
+        </is>
+      </c>
+      <c r="D45" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="E45" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="F45" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="G45" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="H45" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="I45" t="inlineStr">
+        <is>
+          <t>Generate 10 pretty long and interesting facts about Voltaire</t>
+        </is>
+      </c>
+    </row>
+    <row r="46">
+      <c r="A46" t="n">
+        <v>55</v>
+      </c>
+      <c r="B46" t="inlineStr">
+        <is>
+          <t>Harriet Tubman</t>
+        </is>
+      </c>
+      <c r="C46" t="inlineStr">
+        <is>
+          <t>Fought for the abolition of slavery and helped to lead hundreds of slaves to freedom on the Underground Railroad.</t>
+        </is>
+      </c>
+      <c r="D46" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="E46" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="F46" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="G46" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="H46" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="I46" t="inlineStr">
+        <is>
+          <t>Generate 10 pretty long and interesting facts about Harriet Tubman</t>
+        </is>
+      </c>
+    </row>
+    <row r="47">
+      <c r="A47" t="n">
+        <v>56</v>
+      </c>
+      <c r="B47" t="inlineStr">
+        <is>
+          <t>Jimi Hendrix</t>
+        </is>
+      </c>
+      <c r="C47" t="inlineStr">
+        <is>
+          <t>One of the most influential guitarists of all time, he was known for his innovative playing style.</t>
+        </is>
+      </c>
+      <c r="D47" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="E47" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="F47" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="G47" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="H47" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="I47" t="inlineStr">
+        <is>
+          <t>Generate 10 pretty long and interesting facts about Jimi Hendrix</t>
+        </is>
+      </c>
+    </row>
+    <row r="48">
+      <c r="A48" t="n">
+        <v>57</v>
+      </c>
+      <c r="B48" t="inlineStr">
+        <is>
+          <t>Muhammad Ali</t>
+        </is>
+      </c>
+      <c r="C48" t="inlineStr">
+        <is>
+          <t>One of the most successful boxers of all time, he was also a vocal advocate for civil rights.</t>
+        </is>
+      </c>
+      <c r="D48" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="E48" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="F48" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="G48" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="H48" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="I48" t="inlineStr">
+        <is>
+          <t>Generate 10 pretty long and interesting facts about Muhammad Ali</t>
+        </is>
+      </c>
+    </row>
+    <row r="49">
+      <c r="A49" t="n">
+        <v>58</v>
+      </c>
+      <c r="B49" t="inlineStr">
+        <is>
+          <t>Mother Teresa</t>
+        </is>
+      </c>
+      <c r="C49" t="inlineStr">
+        <is>
+          <t>Founded the Missionaries of Charity, a Roman Catholic organization that provides care for the poor and sick.</t>
+        </is>
+      </c>
+      <c r="D49" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="E49" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="F49" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="G49" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="H49" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="I49" t="inlineStr">
+        <is>
+          <t>Generate 10 pretty long and interesting facts about Mother Teresa</t>
+        </is>
+      </c>
+    </row>
+    <row r="50">
+      <c r="A50" t="n">
+        <v>60</v>
+      </c>
+      <c r="B50" t="inlineStr">
+        <is>
+          <t>Neil Armstrong</t>
+        </is>
+      </c>
+      <c r="C50" t="inlineStr">
+        <is>
+          <t>First person to walk on the moon.</t>
+        </is>
+      </c>
+      <c r="D50" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="E50" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="F50" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="G50" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="H50" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="I50" t="inlineStr">
+        <is>
+          <t>Generate 10 pretty long and interesting facts about Neil Armstrong</t>
+        </is>
+      </c>
+    </row>
+    <row r="51">
+      <c r="A51" t="n">
+        <v>61</v>
+      </c>
+      <c r="B51" t="inlineStr">
+        <is>
+          <t>Oprah Winfrey</t>
+        </is>
+      </c>
+      <c r="C51" t="inlineStr">
+        <is>
+          <t>One of the most successful talk show hosts of all time, she is also a successful actress and producer.</t>
+        </is>
+      </c>
+      <c r="D51" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="E51" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="F51" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="G51" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="H51" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="I51" t="inlineStr">
+        <is>
+          <t>Generate 10 pretty long and interesting facts about Oprah Winfrey</t>
+        </is>
+      </c>
+    </row>
+    <row r="52">
+      <c r="A52" t="n">
+        <v>62</v>
+      </c>
+      <c r="B52" t="inlineStr">
+        <is>
+          <t>Pablo Picasso</t>
+        </is>
+      </c>
+      <c r="C52" t="inlineStr">
+        <is>
+          <t>One of the most influential artists of the 20th century, he was known for his Cubist paintings.</t>
+        </is>
+      </c>
+      <c r="D52" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="E52" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="F52" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="G52" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="H52" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="I52" t="inlineStr">
+        <is>
+          <t>Generate 10 pretty long and interesting facts about Pablo Picasso</t>
+        </is>
+      </c>
+    </row>
+    <row r="53">
+      <c r="A53" t="n">
+        <v>63</v>
+      </c>
+      <c r="B53" t="inlineStr">
+        <is>
+          <t>Queen Nefertiti</t>
+        </is>
+      </c>
+      <c r="C53" t="inlineStr">
+        <is>
+          <t>One of the most famous queens of ancient Egypt, she was known for her beauty and her political influence.</t>
+        </is>
+      </c>
+      <c r="D53" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="E53" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="F53" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="G53" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="H53" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="I53" t="inlineStr">
+        <is>
+          <t>Generate 10 pretty long and interesting facts about Queen Nefertiti</t>
+        </is>
+      </c>
+    </row>
+    <row r="54">
+      <c r="A54" t="n">
+        <v>64</v>
+      </c>
+      <c r="B54" t="inlineStr">
+        <is>
+          <t>Rembrandt van Rijn</t>
+        </is>
+      </c>
+      <c r="C54" t="inlineStr">
+        <is>
+          <t>One of the most important painters of the Dutch Golden Age, he was known for his realistic and dramatic paintings.</t>
+        </is>
+      </c>
+      <c r="D54" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="E54" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="F54" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="G54" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="H54" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="I54" t="inlineStr">
+        <is>
+          <t>Generate 10 pretty long and interesting facts about Rembrandt van Rijn</t>
+        </is>
+      </c>
+    </row>
+    <row r="55">
+      <c r="A55" t="n">
+        <v>65</v>
+      </c>
+      <c r="B55" t="inlineStr">
+        <is>
+          <t>Steve Jobs</t>
+        </is>
+      </c>
+      <c r="C55" t="inlineStr">
+        <is>
+          <t>Co-founder of Apple Inc., he was one of the most influential figures in the technology industry.</t>
+        </is>
+      </c>
+      <c r="D55" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="E55" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="F55" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="G55" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="H55" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="I55" t="inlineStr">
+        <is>
+          <t>Generate 10 pretty long and interesting facts about Steve Jobs</t>
+        </is>
+      </c>
+    </row>
+    <row r="56">
+      <c r="A56" t="n">
+        <v>66</v>
+      </c>
+      <c r="B56" t="inlineStr">
+        <is>
+          <t>Susan B. Anthony</t>
+        </is>
+      </c>
+      <c r="C56" t="inlineStr">
+        <is>
+          <t>Fought for women's suffrage and other women's rights.</t>
+        </is>
+      </c>
+      <c r="D56" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="E56" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="F56" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="G56" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="H56" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="I56" t="inlineStr">
+        <is>
+          <t>Generate 10 pretty long and interesting facts about Susan B. Anthony</t>
+        </is>
+      </c>
+    </row>
+    <row r="57">
+      <c r="A57" t="n">
+        <v>67</v>
+      </c>
+      <c r="B57" t="inlineStr">
+        <is>
+          <t>Tina Fey</t>
+        </is>
+      </c>
+      <c r="C57" t="inlineStr">
+        <is>
+          <t>One of the most successful comedians of all time, she is also a successful actress and writer.</t>
+        </is>
+      </c>
+      <c r="D57" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="E57" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="F57" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="G57" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="H57" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="I57" t="inlineStr">
+        <is>
+          <t>Generate 10 pretty long and interesting facts about Tina Fey</t>
+        </is>
+      </c>
+    </row>
+    <row r="58">
+      <c r="A58" t="n">
+        <v>68</v>
+      </c>
+      <c r="B58" t="inlineStr">
+        <is>
+          <t>Vincent van Gogh</t>
+        </is>
+      </c>
+      <c r="C58" t="inlineStr">
+        <is>
+          <t>One of the most influential painters of the Post-Impressionist movement, he was known for his expressive and colorful paintings.</t>
+        </is>
+      </c>
+      <c r="D58" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="E58" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="F58" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="G58" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="H58" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="I58" t="inlineStr">
+        <is>
+          <t>Generate 10 pretty long and interesting facts about Vincent van Gogh</t>
+        </is>
+      </c>
+    </row>
+    <row r="59">
+      <c r="A59" t="n">
+        <v>69</v>
+      </c>
+      <c r="B59" t="inlineStr">
+        <is>
+          <t>W.E.B. Du Bois</t>
+        </is>
+      </c>
+      <c r="C59" t="inlineStr">
+        <is>
+          <t>One of the most important figures in the American civil rights movement, he was a scholar, writer, and activist.</t>
+        </is>
+      </c>
+      <c r="D59" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="E59" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="F59" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="G59" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="H59" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="I59" t="inlineStr">
+        <is>
+          <t>Generate 10 pretty long and interesting facts about W.E.B. Du Bois</t>
+        </is>
+      </c>
+    </row>
+    <row r="60">
+      <c r="A60" t="n">
+        <v>70</v>
+      </c>
+      <c r="B60" t="inlineStr">
+        <is>
+          <t>Walt Disney</t>
+        </is>
+      </c>
+      <c r="C60" t="inlineStr">
+        <is>
+          <t>One of the most influential figures in the entertainment industry, he was the founder of The Walt Disney Company.</t>
+        </is>
+      </c>
+      <c r="D60" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="E60" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="F60" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="G60" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="H60" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="I60" t="inlineStr">
+        <is>
+          <t>Generate 10 pretty long and interesting facts about Walt Disney</t>
+        </is>
+      </c>
+    </row>
+    <row r="61">
+      <c r="A61" t="n">
+        <v>71</v>
+      </c>
+      <c r="B61" t="inlineStr">
+        <is>
+          <t>Wilhelmina Drucker</t>
+        </is>
+      </c>
+      <c r="C61" t="inlineStr">
+        <is>
+          <t>One of the first women to be elected to the German parliament, she was a leading figure in the women's suffrage movement.</t>
+        </is>
+      </c>
+      <c r="D61" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="E61" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="F61" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="G61" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="H61" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="I61" t="inlineStr">
+        <is>
+          <t>Generate 10 pretty long and interesting facts about Wilhelmina Drucker</t>
+        </is>
+      </c>
+    </row>
+    <row r="62">
+      <c r="A62" t="n">
+        <v>72</v>
+      </c>
+      <c r="B62" t="inlineStr">
+        <is>
+          <t>Xenophon</t>
+        </is>
+      </c>
+      <c r="C62" t="inlineStr">
+        <is>
+          <t>A Greek historian and soldier, he wrote about the Peloponnesian War and the Anabasis.</t>
+        </is>
+      </c>
+      <c r="D62" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="E62" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="F62" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="G62" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="H62" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="I62" t="inlineStr">
+        <is>
+          <t>Generate 10 pretty long and interesting facts about Xenophon</t>
+        </is>
+      </c>
+    </row>
+    <row r="63">
+      <c r="A63" t="n">
+        <v>73</v>
+      </c>
+      <c r="B63" t="inlineStr">
+        <is>
+          <t>Yoko Ono</t>
+        </is>
+      </c>
+      <c r="C63" t="inlineStr">
+        <is>
+          <t>One of the most influential artists of the 20th century, she is also a peace activist and the widow of John Lennon.</t>
+        </is>
+      </c>
+      <c r="D63" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="E63" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="F63" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="G63" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="H63" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="I63" t="inlineStr">
+        <is>
+          <t>Generate 10 pretty long and interesting facts about Yoko Ono</t>
+        </is>
+      </c>
+    </row>
+    <row r="64">
+      <c r="A64" t="n">
+        <v>74</v>
+      </c>
+      <c r="B64" t="inlineStr">
+        <is>
+          <t>Yuri Gagarin</t>
+        </is>
+      </c>
+      <c r="C64" t="inlineStr">
+        <is>
+          <t>First person to travel into space.</t>
+        </is>
+      </c>
+      <c r="D64" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="E64" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="F64" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="G64" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="H64" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="I64" t="inlineStr">
+        <is>
+          <t>Generate 10 pretty long and interesting facts about Yuri Gagarin</t>
+        </is>
+      </c>
+    </row>
+    <row r="65">
+      <c r="A65" t="n">
+        <v>75</v>
+      </c>
+      <c r="B65" t="inlineStr">
+        <is>
+          <t>Aung San Suu Kyi</t>
+        </is>
+      </c>
+      <c r="C65" t="inlineStr">
+        <is>
+          <t>Led the pro-democracy movement in Myanmar and was awarded the Nobel Peace Prize.</t>
+        </is>
+      </c>
+      <c r="D65" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="E65" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="F65" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="G65" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="H65" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="I65" t="inlineStr">
+        <is>
+          <t>Generate 10 pretty long and interesting facts about Aung San Suu Kyi</t>
+        </is>
+      </c>
+    </row>
+    <row r="66">
+      <c r="A66" t="n">
+        <v>76</v>
+      </c>
+      <c r="B66" t="inlineStr">
+        <is>
+          <t>Bill Gates</t>
+        </is>
+      </c>
+      <c r="C66" t="inlineStr">
+        <is>
+          <t>Co-founder of Microsoft, he is one of the richest people in the world and has dedicated his wealth to philanthropy.</t>
+        </is>
+      </c>
+      <c r="D66" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="E66" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="F66" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="G66" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="H66" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="I66" t="inlineStr">
+        <is>
+          <t>Generate 10 pretty long and interesting facts about Bill Gates</t>
+        </is>
+      </c>
+    </row>
+    <row r="67">
+      <c r="A67" t="n">
+        <v>77</v>
+      </c>
+      <c r="B67" t="inlineStr">
+        <is>
+          <t>Charles Dickens</t>
+        </is>
+      </c>
+      <c r="C67" t="inlineStr">
+        <is>
+          <t>One of the most popular novelists of the 19th century, he wrote about the lives of the poor and working class.</t>
+        </is>
+      </c>
+      <c r="D67" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="E67" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="F67" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="G67" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="H67" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="I67" t="inlineStr">
+        <is>
+          <t>Generate 10 pretty long and interesting facts about Charles Dickens</t>
+        </is>
+      </c>
+    </row>
+    <row r="68">
+      <c r="A68" t="n">
+        <v>78</v>
+      </c>
+      <c r="B68" t="inlineStr">
+        <is>
+          <t>Chen Guangcheng</t>
+        </is>
+      </c>
+      <c r="C68" t="inlineStr">
+        <is>
+          <t>Fought for the rights of people with disabilities in China and was imprisoned for his activism.</t>
+        </is>
+      </c>
+      <c r="D68" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="E68" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="F68" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="G68" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="H68" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="I68" t="inlineStr">
+        <is>
+          <t>Generate 10 pretty long and interesting facts about Chen Guangcheng</t>
+        </is>
+      </c>
+    </row>
+    <row r="69">
+      <c r="A69" t="n">
+        <v>79</v>
+      </c>
+      <c r="B69" t="inlineStr">
+        <is>
+          <t>Daenerys Targaryen</t>
+        </is>
+      </c>
+      <c r="C69" t="inlineStr">
+        <is>
+          <t>A fictional character in the "Game of Thrones" series, she is a powerful and inspiring leader.</t>
+        </is>
+      </c>
+      <c r="D69" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="E69" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="F69" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="G69" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="H69" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="I69" t="inlineStr">
+        <is>
+          <t>Generate 10 pretty long and interesting facts about Daenerys Targaryen</t>
+        </is>
+      </c>
+    </row>
+    <row r="70">
+      <c r="A70" t="n">
+        <v>80</v>
+      </c>
+      <c r="B70" t="inlineStr">
+        <is>
+          <t>Elon Musk</t>
+        </is>
+      </c>
+      <c r="C70" t="inlineStr">
+        <is>
+          <t>Co-founder of Tesla and SpaceX, he is one of the most innovative entrepreneurs of our time.</t>
+        </is>
+      </c>
+      <c r="D70" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="E70" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="F70" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="G70" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="H70" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="I70" t="inlineStr">
+        <is>
+          <t>Generate 10 pretty long and interesting facts about Elon Musk</t>
+        </is>
+      </c>
+    </row>
+    <row r="71">
+      <c r="A71" t="n">
+        <v>83</v>
+      </c>
+      <c r="B71" t="inlineStr">
+        <is>
+          <t>George Orwell</t>
+        </is>
+      </c>
+      <c r="C71" t="inlineStr">
+        <is>
+          <t>One of the most important writers of the 20th century, he wrote about the dangers of totalitarianism.</t>
+        </is>
+      </c>
+      <c r="D71" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="E71" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="F71" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="G71" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="H71" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="I71" t="inlineStr">
+        <is>
+          <t>Generate 10 pretty long and interesting facts about George Orwell</t>
+        </is>
+      </c>
+    </row>
+    <row r="72">
+      <c r="A72" t="n">
+        <v>84</v>
+      </c>
+      <c r="B72" t="inlineStr">
+        <is>
+          <t>Harvey Milk</t>
+        </is>
+      </c>
+      <c r="C72" t="inlineStr">
+        <is>
+          <t>One of the first openly gay elected officials in the United States, he was a leading figure in the gay rights movement.</t>
+        </is>
+      </c>
+      <c r="D72" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="E72" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="F72" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="G72" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="H72" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="I72" t="inlineStr">
+        <is>
+          <t>Generate 10 pretty long and interesting facts about Harvey Milk</t>
+        </is>
+      </c>
+    </row>
+    <row r="73">
+      <c r="A73" t="n">
+        <v>85</v>
+      </c>
+      <c r="B73" t="inlineStr">
+        <is>
+          <t>Jackie Robinson</t>
+        </is>
+      </c>
+      <c r="C73" t="inlineStr">
+        <is>
+          <t>One of the first African Americans to play Major League Baseball, he broke the color barrier and inspired a generation of athletes.</t>
+        </is>
+      </c>
+      <c r="D73" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="E73" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="F73" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="G73" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="H73" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="I73" t="inlineStr">
+        <is>
+          <t>Generate 10 pretty long and interesting facts about Jackie Robinson</t>
+        </is>
+      </c>
+    </row>
+    <row r="74">
+      <c r="A74" t="n">
+        <v>86</v>
+      </c>
+      <c r="B74" t="inlineStr">
+        <is>
+          <t>Jacqueline Kennedy Onassis</t>
+        </is>
+      </c>
+      <c r="C74" t="inlineStr">
+        <is>
+          <t>One of the most popular First Ladies of the 20th century, she was also a successful author.</t>
+        </is>
+      </c>
+      <c r="D74" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="E74" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="F74" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="G74" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="H74" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="I74" t="inlineStr">
+        <is>
+          <t>Generate 10 pretty long and interesting facts about Jacqueline Kennedy Onassis</t>
+        </is>
+      </c>
+    </row>
+    <row r="75">
+      <c r="A75" t="n">
+        <v>88</v>
+      </c>
+      <c r="B75" t="inlineStr">
+        <is>
+          <t>Jim Henson</t>
+        </is>
+      </c>
+      <c r="C75" t="inlineStr">
+        <is>
+          <t>One of the most influential puppeteers of all time, he created some of the most beloved characters in television history.</t>
+        </is>
+      </c>
+      <c r="D75" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="E75" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="F75" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="G75" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="H75" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="I75" t="inlineStr">
+        <is>
+          <t>Generate 10 pretty long and interesting facts about Jim Henson</t>
+        </is>
+      </c>
+    </row>
+    <row r="76">
+      <c r="A76" t="n">
+        <v>89</v>
+      </c>
+      <c r="B76" t="inlineStr">
+        <is>
+          <t>Malcolm X</t>
+        </is>
+      </c>
+      <c r="C76" t="inlineStr">
+        <is>
+          <t>One of the most influential leaders of the Black Power movement, he was a vocal advocate for black liberation.</t>
+        </is>
+      </c>
+      <c r="D76" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="E76" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="F76" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="G76" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="H76" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="I76" t="inlineStr">
+        <is>
+          <t>Generate 10 pretty long and interesting facts about Malcolm X</t>
+        </is>
+      </c>
+    </row>
+    <row r="77">
+      <c r="A77" t="n">
+        <v>91</v>
+      </c>
+      <c r="B77" t="inlineStr">
+        <is>
+          <t>Maya Angelou</t>
+        </is>
+      </c>
+      <c r="C77" t="inlineStr">
+        <is>
+          <t>One of the most celebrated poets and authors of the 20th century, she wrote about her experiences as an African American woman.</t>
+        </is>
+      </c>
+      <c r="D77" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="E77" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="F77" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="G77" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="H77" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="I77" t="inlineStr">
+        <is>
+          <t>Generate 10 pretty long and interesting facts about Maya Angelou</t>
+        </is>
+      </c>
+    </row>
+    <row r="78">
+      <c r="A78" t="n">
+        <v>92</v>
+      </c>
+      <c r="B78" t="inlineStr">
+        <is>
+          <t>Barack Obama</t>
+        </is>
+      </c>
+      <c r="C78" t="inlineStr">
+        <is>
+          <t>44th President of the United States, he was the first African American to be elected to the presidency.</t>
+        </is>
+      </c>
+      <c r="D78" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="E78" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="F78" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="G78" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="H78" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="I78" t="inlineStr">
+        <is>
+          <t>Generate 10 pretty long and interesting facts about Barack Obama</t>
+        </is>
+      </c>
+    </row>
+    <row r="79">
+      <c r="A79" t="n">
+        <v>93</v>
+      </c>
+      <c r="B79" t="inlineStr">
+        <is>
+          <t>Benazir Bhutto</t>
+        </is>
+      </c>
+      <c r="C79" t="inlineStr">
+        <is>
+          <t>Prime Minister of Pakistan from 1988 to 1990 and again from 1993 to 1996, she was the first woman to be elected prime minister of a Muslim-majority country.</t>
+        </is>
+      </c>
+      <c r="D79" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="E79" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="F79" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="G79" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="H79" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="I79" t="inlineStr">
+        <is>
+          <t>Generate 10 pretty long and interesting facts about Benazir Bhutto</t>
+        </is>
+      </c>
+    </row>
+    <row r="80">
+      <c r="A80" t="n">
+        <v>94</v>
+      </c>
+      <c r="B80" t="inlineStr">
+        <is>
+          <t>Betty Friedan</t>
+        </is>
+      </c>
+      <c r="C80" t="inlineStr">
+        <is>
+          <t>Author of the book "The Feminine Mystique," which helped to spark the second wave of the feminist movement.</t>
+        </is>
+      </c>
+      <c r="D80" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="E80" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="F80" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="G80" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="H80" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="I80" t="inlineStr">
+        <is>
+          <t>Generate 10 pretty long and interesting facts about Betty Friedan</t>
+        </is>
+      </c>
+    </row>
+    <row r="81">
+      <c r="A81" t="n">
+        <v>95</v>
+      </c>
+      <c r="B81" t="inlineStr">
+        <is>
+          <t>Billie Jean King</t>
+        </is>
+      </c>
+      <c r="C81" t="inlineStr">
+        <is>
+          <t>One of the most successful tennis players of all time, she was a vocal advocate for gender equality.</t>
+        </is>
+      </c>
+      <c r="D81" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="E81" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="F81" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="G81" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="H81" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="I81" t="inlineStr">
+        <is>
+          <t>Generate 10 pretty long and interesting facts about Billie Jean King</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
Big thumbnail code revamp, file removal
</commit_message>
<xml_diff>
--- a/Historical Figures List.xlsx
+++ b/Historical Figures List.xlsx
@@ -561,7 +561,7 @@
       </c>
       <c r="H3" t="inlineStr">
         <is>
-          <t>No</t>
+          <t>Yes</t>
         </is>
       </c>
       <c r="I3" t="inlineStr">
@@ -596,7 +596,7 @@
       </c>
       <c r="F4" t="inlineStr">
         <is>
-          <t>Yes</t>
+          <t>No</t>
         </is>
       </c>
       <c r="G4" t="inlineStr">
@@ -641,7 +641,7 @@
       </c>
       <c r="F5" t="inlineStr">
         <is>
-          <t>Yes</t>
+          <t>No</t>
         </is>
       </c>
       <c r="G5" t="inlineStr">
@@ -686,7 +686,7 @@
       </c>
       <c r="F6" t="inlineStr">
         <is>
-          <t>Yes</t>
+          <t>No</t>
         </is>
       </c>
       <c r="G6" t="inlineStr">
@@ -731,7 +731,7 @@
       </c>
       <c r="F7" t="inlineStr">
         <is>
-          <t>Yes</t>
+          <t>No</t>
         </is>
       </c>
       <c r="G7" t="inlineStr">
@@ -776,7 +776,7 @@
       </c>
       <c r="F8" t="inlineStr">
         <is>
-          <t>Yes</t>
+          <t>No</t>
         </is>
       </c>
       <c r="G8" t="inlineStr">
@@ -831,7 +831,7 @@
       </c>
       <c r="H9" t="inlineStr">
         <is>
-          <t>No</t>
+          <t>Yes</t>
         </is>
       </c>
       <c r="I9" t="inlineStr">
@@ -866,7 +866,7 @@
       </c>
       <c r="F10" t="inlineStr">
         <is>
-          <t>Yes</t>
+          <t>No</t>
         </is>
       </c>
       <c r="G10" t="inlineStr">
@@ -991,12 +991,12 @@
       </c>
       <c r="D13" t="inlineStr">
         <is>
-          <t>No</t>
+          <t>Yes</t>
         </is>
       </c>
       <c r="E13" t="inlineStr">
         <is>
-          <t>No</t>
+          <t>Yes</t>
         </is>
       </c>
       <c r="F13" t="inlineStr">
@@ -1036,12 +1036,12 @@
       </c>
       <c r="D14" t="inlineStr">
         <is>
-          <t>No</t>
+          <t>Yes</t>
         </is>
       </c>
       <c r="E14" t="inlineStr">
         <is>
-          <t>No</t>
+          <t>Yes</t>
         </is>
       </c>
       <c r="F14" t="inlineStr">

</xml_diff>

<commit_message>
Update, will get around to removing images
</commit_message>
<xml_diff>
--- a/Historical Figures List.xlsx
+++ b/Historical Figures List.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20399"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26501"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\bencros\Documents\GitHub\Video-from-Script\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\benjc\Documents\GitHub\Video-from-Script\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C5C85706-70A7-4CFB-8F92-88CD963C9473}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{835C8C16-2F0B-4E7A-8581-D7A4BBF9EFF6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="11625" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-28920" yWindow="3315" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="657" uniqueCount="254">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="658" uniqueCount="255">
   <si>
     <t>Figure_ID</t>
   </si>
@@ -782,6 +782,9 @@
   </si>
   <si>
     <t>Generate 10 pretty long and interesting facts about J. R. R. Tolkien</t>
+  </si>
+  <si>
+    <t>Youtube_URL</t>
   </si>
 </sst>
 </file>
@@ -800,7 +803,6 @@
       <b/>
       <sz val="11"/>
       <name val="Calibri"/>
-      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -1145,15 +1147,25 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:I82"/>
+  <dimension ref="A1:J82"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A14" sqref="A14:XFD14"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="I2" sqref="I2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="26.42578125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="9.140625" hidden="1" customWidth="1"/>
+    <col min="4" max="4" width="14.140625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="19.7109375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="16.7109375" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="23.28515625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="22.42578125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="22.42578125" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1179,10 +1191,13 @@
         <v>7</v>
       </c>
       <c r="I1" s="1" t="s">
+        <v>254</v>
+      </c>
+      <c r="J1" s="1" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>1</v>
       </c>
@@ -1207,11 +1222,11 @@
       <c r="H2" t="s">
         <v>11</v>
       </c>
-      <c r="I2" t="s">
+      <c r="J2" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>2</v>
       </c>
@@ -1236,11 +1251,11 @@
       <c r="H3" t="s">
         <v>11</v>
       </c>
-      <c r="I3" t="s">
+      <c r="J3" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>3</v>
       </c>
@@ -1257,19 +1272,19 @@
         <v>11</v>
       </c>
       <c r="F4" t="s">
-        <v>18</v>
+        <v>11</v>
       </c>
       <c r="G4" t="s">
-        <v>18</v>
+        <v>11</v>
       </c>
       <c r="H4" t="s">
         <v>18</v>
       </c>
-      <c r="I4" t="s">
+      <c r="J4" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>4</v>
       </c>
@@ -1286,19 +1301,19 @@
         <v>11</v>
       </c>
       <c r="F5" t="s">
-        <v>18</v>
+        <v>11</v>
       </c>
       <c r="G5" t="s">
-        <v>18</v>
+        <v>11</v>
       </c>
       <c r="H5" t="s">
-        <v>18</v>
-      </c>
-      <c r="I5" t="s">
+        <v>11</v>
+      </c>
+      <c r="J5" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>5</v>
       </c>
@@ -1315,19 +1330,19 @@
         <v>11</v>
       </c>
       <c r="F6" t="s">
-        <v>18</v>
+        <v>11</v>
       </c>
       <c r="G6" t="s">
-        <v>18</v>
+        <v>11</v>
       </c>
       <c r="H6" t="s">
-        <v>18</v>
-      </c>
-      <c r="I6" t="s">
+        <v>11</v>
+      </c>
+      <c r="J6" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>6</v>
       </c>
@@ -1344,19 +1359,19 @@
         <v>11</v>
       </c>
       <c r="F7" t="s">
-        <v>18</v>
+        <v>11</v>
       </c>
       <c r="G7" t="s">
-        <v>18</v>
+        <v>11</v>
       </c>
       <c r="H7" t="s">
         <v>18</v>
       </c>
-      <c r="I7" t="s">
+      <c r="J7" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>7</v>
       </c>
@@ -1373,19 +1388,19 @@
         <v>11</v>
       </c>
       <c r="F8" t="s">
-        <v>18</v>
+        <v>11</v>
       </c>
       <c r="G8" t="s">
-        <v>18</v>
+        <v>11</v>
       </c>
       <c r="H8" t="s">
-        <v>18</v>
-      </c>
-      <c r="I8" t="s">
+        <v>11</v>
+      </c>
+      <c r="J8" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>8</v>
       </c>
@@ -1410,11 +1425,11 @@
       <c r="H9" t="s">
         <v>11</v>
       </c>
-      <c r="I9" t="s">
+      <c r="J9" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>9</v>
       </c>
@@ -1431,19 +1446,19 @@
         <v>11</v>
       </c>
       <c r="F10" t="s">
-        <v>18</v>
+        <v>11</v>
       </c>
       <c r="G10" t="s">
-        <v>18</v>
+        <v>11</v>
       </c>
       <c r="H10" t="s">
-        <v>18</v>
-      </c>
-      <c r="I10" t="s">
+        <v>11</v>
+      </c>
+      <c r="J10" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>10</v>
       </c>
@@ -1468,11 +1483,11 @@
       <c r="H11" t="s">
         <v>11</v>
       </c>
-      <c r="I11" t="s">
+      <c r="J11" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>11</v>
       </c>
@@ -1489,19 +1504,19 @@
         <v>11</v>
       </c>
       <c r="F12" t="s">
-        <v>18</v>
+        <v>11</v>
       </c>
       <c r="G12" t="s">
-        <v>18</v>
+        <v>11</v>
       </c>
       <c r="H12" t="s">
         <v>18</v>
       </c>
-      <c r="I12" t="s">
+      <c r="J12" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>12</v>
       </c>
@@ -1518,19 +1533,19 @@
         <v>11</v>
       </c>
       <c r="F13" t="s">
-        <v>18</v>
+        <v>11</v>
       </c>
       <c r="G13" t="s">
-        <v>18</v>
+        <v>11</v>
       </c>
       <c r="H13" t="s">
-        <v>18</v>
-      </c>
-      <c r="I13" t="s">
+        <v>11</v>
+      </c>
+      <c r="J13" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>14</v>
       </c>
@@ -1547,19 +1562,19 @@
         <v>11</v>
       </c>
       <c r="F14" t="s">
-        <v>18</v>
+        <v>11</v>
       </c>
       <c r="G14" t="s">
-        <v>18</v>
+        <v>11</v>
       </c>
       <c r="H14" t="s">
         <v>18</v>
       </c>
-      <c r="I14" t="s">
+      <c r="J14" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>15</v>
       </c>
@@ -1584,11 +1599,11 @@
       <c r="H15" t="s">
         <v>18</v>
       </c>
-      <c r="I15" t="s">
+      <c r="J15" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A16">
         <v>16</v>
       </c>
@@ -1613,11 +1628,11 @@
       <c r="H16" t="s">
         <v>18</v>
       </c>
-      <c r="I16" t="s">
+      <c r="J16" t="s">
         <v>55</v>
       </c>
     </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A17">
         <v>17</v>
       </c>
@@ -1642,11 +1657,11 @@
       <c r="H17" t="s">
         <v>18</v>
       </c>
-      <c r="I17" t="s">
+      <c r="J17" t="s">
         <v>58</v>
       </c>
     </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A18">
         <v>18</v>
       </c>
@@ -1671,11 +1686,11 @@
       <c r="H18" t="s">
         <v>18</v>
       </c>
-      <c r="I18" t="s">
+      <c r="J18" t="s">
         <v>61</v>
       </c>
     </row>
-    <row r="19" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A19">
         <v>19</v>
       </c>
@@ -1700,11 +1715,11 @@
       <c r="H19" t="s">
         <v>18</v>
       </c>
-      <c r="I19" t="s">
+      <c r="J19" t="s">
         <v>64</v>
       </c>
     </row>
-    <row r="20" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A20">
         <v>20</v>
       </c>
@@ -1729,11 +1744,11 @@
       <c r="H20" t="s">
         <v>18</v>
       </c>
-      <c r="I20" t="s">
+      <c r="J20" t="s">
         <v>67</v>
       </c>
     </row>
-    <row r="21" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A21">
         <v>21</v>
       </c>
@@ -1758,11 +1773,11 @@
       <c r="H21" t="s">
         <v>18</v>
       </c>
-      <c r="I21" t="s">
+      <c r="J21" t="s">
         <v>70</v>
       </c>
     </row>
-    <row r="22" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A22">
         <v>22</v>
       </c>
@@ -1787,11 +1802,11 @@
       <c r="H22" t="s">
         <v>18</v>
       </c>
-      <c r="I22" t="s">
+      <c r="J22" t="s">
         <v>73</v>
       </c>
     </row>
-    <row r="23" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A23">
         <v>23</v>
       </c>
@@ -1816,11 +1831,11 @@
       <c r="H23" t="s">
         <v>18</v>
       </c>
-      <c r="I23" t="s">
+      <c r="J23" t="s">
         <v>76</v>
       </c>
     </row>
-    <row r="24" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A24">
         <v>24</v>
       </c>
@@ -1845,11 +1860,11 @@
       <c r="H24" t="s">
         <v>18</v>
       </c>
-      <c r="I24" t="s">
+      <c r="J24" t="s">
         <v>79</v>
       </c>
     </row>
-    <row r="25" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A25">
         <v>25</v>
       </c>
@@ -1874,11 +1889,11 @@
       <c r="H25" t="s">
         <v>18</v>
       </c>
-      <c r="I25" t="s">
+      <c r="J25" t="s">
         <v>82</v>
       </c>
     </row>
-    <row r="26" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A26">
         <v>26</v>
       </c>
@@ -1903,11 +1918,11 @@
       <c r="H26" t="s">
         <v>18</v>
       </c>
-      <c r="I26" t="s">
+      <c r="J26" t="s">
         <v>85</v>
       </c>
     </row>
-    <row r="27" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A27">
         <v>27</v>
       </c>
@@ -1932,11 +1947,11 @@
       <c r="H27" t="s">
         <v>18</v>
       </c>
-      <c r="I27" t="s">
+      <c r="J27" t="s">
         <v>88</v>
       </c>
     </row>
-    <row r="28" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A28">
         <v>28</v>
       </c>
@@ -1961,11 +1976,11 @@
       <c r="H28" t="s">
         <v>18</v>
       </c>
-      <c r="I28" t="s">
+      <c r="J28" t="s">
         <v>91</v>
       </c>
     </row>
-    <row r="29" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A29">
         <v>29</v>
       </c>
@@ -1990,11 +2005,11 @@
       <c r="H29" t="s">
         <v>18</v>
       </c>
-      <c r="I29" t="s">
+      <c r="J29" t="s">
         <v>94</v>
       </c>
     </row>
-    <row r="30" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A30">
         <v>32</v>
       </c>
@@ -2019,11 +2034,11 @@
       <c r="H30" t="s">
         <v>18</v>
       </c>
-      <c r="I30" t="s">
+      <c r="J30" t="s">
         <v>97</v>
       </c>
     </row>
-    <row r="31" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A31">
         <v>34</v>
       </c>
@@ -2048,11 +2063,11 @@
       <c r="H31" t="s">
         <v>18</v>
       </c>
-      <c r="I31" t="s">
+      <c r="J31" t="s">
         <v>100</v>
       </c>
     </row>
-    <row r="32" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A32">
         <v>35</v>
       </c>
@@ -2077,11 +2092,11 @@
       <c r="H32" t="s">
         <v>18</v>
       </c>
-      <c r="I32" t="s">
+      <c r="J32" t="s">
         <v>103</v>
       </c>
     </row>
-    <row r="33" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A33">
         <v>36</v>
       </c>
@@ -2106,11 +2121,11 @@
       <c r="H33" t="s">
         <v>18</v>
       </c>
-      <c r="I33" t="s">
+      <c r="J33" t="s">
         <v>106</v>
       </c>
     </row>
-    <row r="34" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A34">
         <v>37</v>
       </c>
@@ -2135,11 +2150,11 @@
       <c r="H34" t="s">
         <v>18</v>
       </c>
-      <c r="I34" t="s">
+      <c r="J34" t="s">
         <v>109</v>
       </c>
     </row>
-    <row r="35" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A35">
         <v>38</v>
       </c>
@@ -2164,11 +2179,11 @@
       <c r="H35" t="s">
         <v>18</v>
       </c>
-      <c r="I35" t="s">
+      <c r="J35" t="s">
         <v>112</v>
       </c>
     </row>
-    <row r="36" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A36">
         <v>40</v>
       </c>
@@ -2193,11 +2208,11 @@
       <c r="H36" t="s">
         <v>18</v>
       </c>
-      <c r="I36" t="s">
+      <c r="J36" t="s">
         <v>115</v>
       </c>
     </row>
-    <row r="37" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A37">
         <v>42</v>
       </c>
@@ -2222,11 +2237,11 @@
       <c r="H37" t="s">
         <v>18</v>
       </c>
-      <c r="I37" t="s">
+      <c r="J37" t="s">
         <v>118</v>
       </c>
     </row>
-    <row r="38" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A38">
         <v>43</v>
       </c>
@@ -2251,11 +2266,11 @@
       <c r="H38" t="s">
         <v>18</v>
       </c>
-      <c r="I38" t="s">
+      <c r="J38" t="s">
         <v>121</v>
       </c>
     </row>
-    <row r="39" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A39">
         <v>45</v>
       </c>
@@ -2280,11 +2295,11 @@
       <c r="H39" t="s">
         <v>18</v>
       </c>
-      <c r="I39" t="s">
+      <c r="J39" t="s">
         <v>124</v>
       </c>
     </row>
-    <row r="40" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A40">
         <v>47</v>
       </c>
@@ -2309,11 +2324,11 @@
       <c r="H40" t="s">
         <v>18</v>
       </c>
-      <c r="I40" t="s">
+      <c r="J40" t="s">
         <v>127</v>
       </c>
     </row>
-    <row r="41" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A41">
         <v>48</v>
       </c>
@@ -2338,11 +2353,11 @@
       <c r="H41" t="s">
         <v>18</v>
       </c>
-      <c r="I41" t="s">
+      <c r="J41" t="s">
         <v>130</v>
       </c>
     </row>
-    <row r="42" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A42">
         <v>50</v>
       </c>
@@ -2367,11 +2382,11 @@
       <c r="H42" t="s">
         <v>18</v>
       </c>
-      <c r="I42" t="s">
+      <c r="J42" t="s">
         <v>133</v>
       </c>
     </row>
-    <row r="43" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A43">
         <v>51</v>
       </c>
@@ -2396,11 +2411,11 @@
       <c r="H43" t="s">
         <v>18</v>
       </c>
-      <c r="I43" t="s">
+      <c r="J43" t="s">
         <v>136</v>
       </c>
     </row>
-    <row r="44" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A44">
         <v>52</v>
       </c>
@@ -2425,11 +2440,11 @@
       <c r="H44" t="s">
         <v>18</v>
       </c>
-      <c r="I44" t="s">
+      <c r="J44" t="s">
         <v>139</v>
       </c>
     </row>
-    <row r="45" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A45">
         <v>53</v>
       </c>
@@ -2454,11 +2469,11 @@
       <c r="H45" t="s">
         <v>18</v>
       </c>
-      <c r="I45" t="s">
+      <c r="J45" t="s">
         <v>142</v>
       </c>
     </row>
-    <row r="46" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A46">
         <v>55</v>
       </c>
@@ -2483,11 +2498,11 @@
       <c r="H46" t="s">
         <v>18</v>
       </c>
-      <c r="I46" t="s">
+      <c r="J46" t="s">
         <v>145</v>
       </c>
     </row>
-    <row r="47" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A47">
         <v>56</v>
       </c>
@@ -2512,11 +2527,11 @@
       <c r="H47" t="s">
         <v>18</v>
       </c>
-      <c r="I47" t="s">
+      <c r="J47" t="s">
         <v>148</v>
       </c>
     </row>
-    <row r="48" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A48">
         <v>57</v>
       </c>
@@ -2541,11 +2556,11 @@
       <c r="H48" t="s">
         <v>18</v>
       </c>
-      <c r="I48" t="s">
+      <c r="J48" t="s">
         <v>151</v>
       </c>
     </row>
-    <row r="49" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A49">
         <v>58</v>
       </c>
@@ -2570,11 +2585,11 @@
       <c r="H49" t="s">
         <v>18</v>
       </c>
-      <c r="I49" t="s">
+      <c r="J49" t="s">
         <v>154</v>
       </c>
     </row>
-    <row r="50" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A50">
         <v>60</v>
       </c>
@@ -2599,11 +2614,11 @@
       <c r="H50" t="s">
         <v>18</v>
       </c>
-      <c r="I50" t="s">
+      <c r="J50" t="s">
         <v>157</v>
       </c>
     </row>
-    <row r="51" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A51">
         <v>61</v>
       </c>
@@ -2628,11 +2643,11 @@
       <c r="H51" t="s">
         <v>18</v>
       </c>
-      <c r="I51" t="s">
+      <c r="J51" t="s">
         <v>160</v>
       </c>
     </row>
-    <row r="52" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A52">
         <v>62</v>
       </c>
@@ -2657,11 +2672,11 @@
       <c r="H52" t="s">
         <v>18</v>
       </c>
-      <c r="I52" t="s">
+      <c r="J52" t="s">
         <v>163</v>
       </c>
     </row>
-    <row r="53" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A53">
         <v>63</v>
       </c>
@@ -2686,11 +2701,11 @@
       <c r="H53" t="s">
         <v>18</v>
       </c>
-      <c r="I53" t="s">
+      <c r="J53" t="s">
         <v>166</v>
       </c>
     </row>
-    <row r="54" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A54">
         <v>64</v>
       </c>
@@ -2715,11 +2730,11 @@
       <c r="H54" t="s">
         <v>18</v>
       </c>
-      <c r="I54" t="s">
+      <c r="J54" t="s">
         <v>169</v>
       </c>
     </row>
-    <row r="55" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A55">
         <v>65</v>
       </c>
@@ -2744,11 +2759,11 @@
       <c r="H55" t="s">
         <v>18</v>
       </c>
-      <c r="I55" t="s">
+      <c r="J55" t="s">
         <v>172</v>
       </c>
     </row>
-    <row r="56" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A56">
         <v>66</v>
       </c>
@@ -2773,11 +2788,11 @@
       <c r="H56" t="s">
         <v>18</v>
       </c>
-      <c r="I56" t="s">
+      <c r="J56" t="s">
         <v>175</v>
       </c>
     </row>
-    <row r="57" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A57">
         <v>67</v>
       </c>
@@ -2802,11 +2817,11 @@
       <c r="H57" t="s">
         <v>18</v>
       </c>
-      <c r="I57" t="s">
+      <c r="J57" t="s">
         <v>178</v>
       </c>
     </row>
-    <row r="58" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A58">
         <v>68</v>
       </c>
@@ -2831,11 +2846,11 @@
       <c r="H58" t="s">
         <v>18</v>
       </c>
-      <c r="I58" t="s">
+      <c r="J58" t="s">
         <v>181</v>
       </c>
     </row>
-    <row r="59" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A59">
         <v>69</v>
       </c>
@@ -2860,11 +2875,11 @@
       <c r="H59" t="s">
         <v>18</v>
       </c>
-      <c r="I59" t="s">
+      <c r="J59" t="s">
         <v>184</v>
       </c>
     </row>
-    <row r="60" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A60">
         <v>70</v>
       </c>
@@ -2889,11 +2904,11 @@
       <c r="H60" t="s">
         <v>18</v>
       </c>
-      <c r="I60" t="s">
+      <c r="J60" t="s">
         <v>187</v>
       </c>
     </row>
-    <row r="61" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A61">
         <v>71</v>
       </c>
@@ -2918,11 +2933,11 @@
       <c r="H61" t="s">
         <v>18</v>
       </c>
-      <c r="I61" t="s">
+      <c r="J61" t="s">
         <v>190</v>
       </c>
     </row>
-    <row r="62" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A62">
         <v>72</v>
       </c>
@@ -2947,11 +2962,11 @@
       <c r="H62" t="s">
         <v>18</v>
       </c>
-      <c r="I62" t="s">
+      <c r="J62" t="s">
         <v>193</v>
       </c>
     </row>
-    <row r="63" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A63">
         <v>73</v>
       </c>
@@ -2976,11 +2991,11 @@
       <c r="H63" t="s">
         <v>18</v>
       </c>
-      <c r="I63" t="s">
+      <c r="J63" t="s">
         <v>196</v>
       </c>
     </row>
-    <row r="64" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A64">
         <v>74</v>
       </c>
@@ -3005,11 +3020,11 @@
       <c r="H64" t="s">
         <v>18</v>
       </c>
-      <c r="I64" t="s">
+      <c r="J64" t="s">
         <v>199</v>
       </c>
     </row>
-    <row r="65" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A65">
         <v>75</v>
       </c>
@@ -3034,11 +3049,11 @@
       <c r="H65" t="s">
         <v>18</v>
       </c>
-      <c r="I65" t="s">
+      <c r="J65" t="s">
         <v>202</v>
       </c>
     </row>
-    <row r="66" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A66">
         <v>76</v>
       </c>
@@ -3063,11 +3078,11 @@
       <c r="H66" t="s">
         <v>18</v>
       </c>
-      <c r="I66" t="s">
+      <c r="J66" t="s">
         <v>205</v>
       </c>
     </row>
-    <row r="67" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A67">
         <v>77</v>
       </c>
@@ -3092,11 +3107,11 @@
       <c r="H67" t="s">
         <v>18</v>
       </c>
-      <c r="I67" t="s">
+      <c r="J67" t="s">
         <v>208</v>
       </c>
     </row>
-    <row r="68" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A68">
         <v>78</v>
       </c>
@@ -3121,11 +3136,11 @@
       <c r="H68" t="s">
         <v>18</v>
       </c>
-      <c r="I68" t="s">
+      <c r="J68" t="s">
         <v>211</v>
       </c>
     </row>
-    <row r="69" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A69">
         <v>79</v>
       </c>
@@ -3150,11 +3165,11 @@
       <c r="H69" t="s">
         <v>18</v>
       </c>
-      <c r="I69" t="s">
+      <c r="J69" t="s">
         <v>214</v>
       </c>
     </row>
-    <row r="70" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A70">
         <v>80</v>
       </c>
@@ -3179,11 +3194,11 @@
       <c r="H70" t="s">
         <v>18</v>
       </c>
-      <c r="I70" t="s">
+      <c r="J70" t="s">
         <v>217</v>
       </c>
     </row>
-    <row r="71" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A71">
         <v>83</v>
       </c>
@@ -3208,11 +3223,11 @@
       <c r="H71" t="s">
         <v>18</v>
       </c>
-      <c r="I71" t="s">
+      <c r="J71" t="s">
         <v>220</v>
       </c>
     </row>
-    <row r="72" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A72">
         <v>84</v>
       </c>
@@ -3237,11 +3252,11 @@
       <c r="H72" t="s">
         <v>18</v>
       </c>
-      <c r="I72" t="s">
+      <c r="J72" t="s">
         <v>223</v>
       </c>
     </row>
-    <row r="73" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A73">
         <v>85</v>
       </c>
@@ -3266,11 +3281,11 @@
       <c r="H73" t="s">
         <v>18</v>
       </c>
-      <c r="I73" t="s">
+      <c r="J73" t="s">
         <v>226</v>
       </c>
     </row>
-    <row r="74" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A74">
         <v>86</v>
       </c>
@@ -3295,11 +3310,11 @@
       <c r="H74" t="s">
         <v>18</v>
       </c>
-      <c r="I74" t="s">
+      <c r="J74" t="s">
         <v>229</v>
       </c>
     </row>
-    <row r="75" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A75">
         <v>88</v>
       </c>
@@ -3324,11 +3339,11 @@
       <c r="H75" t="s">
         <v>18</v>
       </c>
-      <c r="I75" t="s">
+      <c r="J75" t="s">
         <v>232</v>
       </c>
     </row>
-    <row r="76" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A76">
         <v>89</v>
       </c>
@@ -3353,11 +3368,11 @@
       <c r="H76" t="s">
         <v>18</v>
       </c>
-      <c r="I76" t="s">
+      <c r="J76" t="s">
         <v>235</v>
       </c>
     </row>
-    <row r="77" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A77">
         <v>91</v>
       </c>
@@ -3382,11 +3397,11 @@
       <c r="H77" t="s">
         <v>18</v>
       </c>
-      <c r="I77" t="s">
+      <c r="J77" t="s">
         <v>238</v>
       </c>
     </row>
-    <row r="78" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A78">
         <v>92</v>
       </c>
@@ -3411,11 +3426,11 @@
       <c r="H78" t="s">
         <v>18</v>
       </c>
-      <c r="I78" t="s">
+      <c r="J78" t="s">
         <v>241</v>
       </c>
     </row>
-    <row r="79" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A79">
         <v>93</v>
       </c>
@@ -3440,11 +3455,11 @@
       <c r="H79" t="s">
         <v>18</v>
       </c>
-      <c r="I79" t="s">
+      <c r="J79" t="s">
         <v>244</v>
       </c>
     </row>
-    <row r="80" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A80">
         <v>94</v>
       </c>
@@ -3469,11 +3484,11 @@
       <c r="H80" t="s">
         <v>18</v>
       </c>
-      <c r="I80" t="s">
+      <c r="J80" t="s">
         <v>247</v>
       </c>
     </row>
-    <row r="81" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A81">
         <v>95</v>
       </c>
@@ -3498,11 +3513,11 @@
       <c r="H81" t="s">
         <v>18</v>
       </c>
-      <c r="I81" t="s">
+      <c r="J81" t="s">
         <v>250</v>
       </c>
     </row>
-    <row r="82" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A82">
         <v>95</v>
       </c>
@@ -3519,20 +3534,19 @@
         <v>11</v>
       </c>
       <c r="F82" t="s">
-        <v>18</v>
+        <v>11</v>
       </c>
       <c r="G82" t="s">
-        <v>18</v>
+        <v>11</v>
       </c>
       <c r="H82" t="s">
-        <v>18</v>
-      </c>
-      <c r="I82" t="s">
+        <v>11</v>
+      </c>
+      <c r="J82" t="s">
         <v>253</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Loads more stuff laa
</commit_message>
<xml_diff>
--- a/Historical Figures List.xlsx
+++ b/Historical Figures List.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:J204"/>
+  <dimension ref="A1:J207"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -531,7 +531,7 @@
       </c>
       <c r="J2" t="inlineStr">
         <is>
-          <t>Generate 10 pretty long and interesting facts about Albert Einstein</t>
+          <t>Please provide me with 10 long and interesting facts about Albert Einstein. I have a youtube channel based on influential figures so this information must be accurate as my channel depends on it. Please make the output of the facts at least 700 words long. Thank you.</t>
         </is>
       </c>
     </row>
@@ -581,7 +581,7 @@
       </c>
       <c r="J3" t="inlineStr">
         <is>
-          <t>Generate 10 pretty long and interesting facts about Marie Curie</t>
+          <t>Please provide me with 10 long and interesting facts about Marie Curie. I have a youtube channel based on influential figures so this information must be accurate as my channel depends on it. Please make the output of the facts at least 700 words long. Thank you.</t>
         </is>
       </c>
     </row>
@@ -631,7 +631,7 @@
       </c>
       <c r="J4" t="inlineStr">
         <is>
-          <t>Generate 10 pretty long and interesting facts about Leonardo da Vinci</t>
+          <t>Please provide me with 10 long and interesting facts about Leonardo da Vinci. I have a youtube channel based on influential figures so this information must be accurate as my channel depends on it. Please make the output of the facts at least 700 words long. Thank you.</t>
         </is>
       </c>
     </row>
@@ -681,7 +681,7 @@
       </c>
       <c r="J5" t="inlineStr">
         <is>
-          <t>Generate 10 pretty long and interesting facts about Mahatma Gandhi</t>
+          <t>Please provide me with 10 long and interesting facts about Mahatma Gandhi. I have a youtube channel based on influential figures so this information must be accurate as my channel depends on it. Please make the output of the facts at least 700 words long. Thank you.</t>
         </is>
       </c>
     </row>
@@ -731,7 +731,7 @@
       </c>
       <c r="J6" t="inlineStr">
         <is>
-          <t>Generate 10 pretty long and interesting facts about Rosa Parks</t>
+          <t>Please provide me with 10 long and interesting facts about Rosa Parks. I have a youtube channel based on influential figures so this information must be accurate as my channel depends on it. Please make the output of the facts at least 700 words long. Thank you.</t>
         </is>
       </c>
     </row>
@@ -781,7 +781,7 @@
       </c>
       <c r="J7" t="inlineStr">
         <is>
-          <t>Generate 10 pretty long and interesting facts about Isaac Newton</t>
+          <t>Please provide me with 10 long and interesting facts about Isaac Newton. I have a youtube channel based on influential figures so this information must be accurate as my channel depends on it. Please make the output of the facts at least 700 words long. Thank you.</t>
         </is>
       </c>
     </row>
@@ -831,7 +831,7 @@
       </c>
       <c r="J8" t="inlineStr">
         <is>
-          <t>Generate 10 pretty long and interesting facts about Cleopatra</t>
+          <t>Please provide me with 10 long and interesting facts about Cleopatra. I have a youtube channel based on influential figures so this information must be accurate as my channel depends on it. Please make the output of the facts at least 700 words long. Thank you.</t>
         </is>
       </c>
     </row>
@@ -881,7 +881,7 @@
       </c>
       <c r="J9" t="inlineStr">
         <is>
-          <t>Generate 10 pretty long and interesting facts about Nelson Mandela</t>
+          <t>Please provide me with 10 long and interesting facts about Nelson Mandela. I have a youtube channel based on influential figures so this information must be accurate as my channel depends on it. Please make the output of the facts at least 700 words long. Thank you.</t>
         </is>
       </c>
     </row>
@@ -931,7 +931,7 @@
       </c>
       <c r="J10" t="inlineStr">
         <is>
-          <t>Generate 10 pretty long and interesting facts about William Shakespeare</t>
+          <t>Please provide me with 10 long and interesting facts about William Shakespeare. I have a youtube channel based on influential figures so this information must be accurate as my channel depends on it. Please make the output of the facts at least 700 words long. Thank you.</t>
         </is>
       </c>
     </row>
@@ -981,7 +981,7 @@
       </c>
       <c r="J11" t="inlineStr">
         <is>
-          <t>Generate 10 pretty long and interesting facts about Amelia Earhart</t>
+          <t>Please provide me with 10 long and interesting facts about Amelia Earhart. I have a youtube channel based on influential figures so this information must be accurate as my channel depends on it. Please make the output of the facts at least 700 words long. Thank you.</t>
         </is>
       </c>
     </row>
@@ -1031,7 +1031,7 @@
       </c>
       <c r="J12" t="inlineStr">
         <is>
-          <t>Generate 10 pretty long and interesting facts about Galileo Galilei</t>
+          <t>Please provide me with 10 long and interesting facts about Galileo Galilei. I have a youtube channel based on influential figures so this information must be accurate as my channel depends on it. Please make the output of the facts at least 700 words long. Thank you.</t>
         </is>
       </c>
     </row>
@@ -1081,7 +1081,7 @@
       </c>
       <c r="J13" t="inlineStr">
         <is>
-          <t>Generate 10 pretty long and interesting facts about Joan of Arc</t>
+          <t>Please provide me with 10 long and interesting facts about Joan of Arc. I have a youtube channel based on influential figures so this information must be accurate as my channel depends on it. Please make the output of the facts at least 700 words long. Thank you.</t>
         </is>
       </c>
     </row>
@@ -1131,7 +1131,7 @@
       </c>
       <c r="J14" t="inlineStr">
         <is>
-          <t>Generate 10 pretty long and interesting facts about Alexander the Great</t>
+          <t>Please provide me with 10 long and interesting facts about Alexander the Great. I have a youtube channel based on influential figures so this information must be accurate as my channel depends on it. Please make the output of the facts at least 700 words long. Thank you.</t>
         </is>
       </c>
     </row>
@@ -1181,7 +1181,7 @@
       </c>
       <c r="J15" t="inlineStr">
         <is>
-          <t>Generate 10 pretty long and interesting facts about Thomas Edison</t>
+          <t>Please provide me with 10 long and interesting facts about Thomas Edison. I have a youtube channel based on influential figures so this information must be accurate as my channel depends on it. Please make the output of the facts at least 700 words long. Thank you.</t>
         </is>
       </c>
     </row>
@@ -1231,7 +1231,7 @@
       </c>
       <c r="J16" t="inlineStr">
         <is>
-          <t>Generate 10 pretty long and interesting facts about Martin Luther King Jr.</t>
+          <t>Please provide me with 10 long and interesting facts about Martin Luther King Jr.. I have a youtube channel based on influential figures so this information must be accurate as my channel depends on it. Please make the output of the facts at least 700 words long. Thank you.</t>
         </is>
       </c>
     </row>
@@ -1281,7 +1281,7 @@
       </c>
       <c r="J17" t="inlineStr">
         <is>
-          <t>Generate 10 pretty long and interesting facts about Marie Antoinette</t>
+          <t>Please provide me with 10 long and interesting facts about Marie Antoinette. I have a youtube channel based on influential figures so this information must be accurate as my channel depends on it. Please make the output of the facts at least 700 words long. Thank you.</t>
         </is>
       </c>
     </row>
@@ -1331,7 +1331,7 @@
       </c>
       <c r="J18" t="inlineStr">
         <is>
-          <t>Generate 10 pretty long and interesting facts about Winston Churchill</t>
+          <t>Please provide me with 10 long and interesting facts about Winston Churchill. I have a youtube channel based on influential figures so this information must be accurate as my channel depends on it. Please make the output of the facts at least 700 words long. Thank you.</t>
         </is>
       </c>
     </row>
@@ -1381,7 +1381,7 @@
       </c>
       <c r="J19" t="inlineStr">
         <is>
-          <t>Generate 10 pretty long and interesting facts about Socrates</t>
+          <t>Please provide me with 10 long and interesting facts about Socrates. I have a youtube channel based on influential figures so this information must be accurate as my channel depends on it. Please make the output of the facts at least 700 words long. Thank you.</t>
         </is>
       </c>
     </row>
@@ -1431,7 +1431,7 @@
       </c>
       <c r="J20" t="inlineStr">
         <is>
-          <t>Generate 10 pretty long and interesting facts about Frida Kahlo</t>
+          <t>Please provide me with 10 long and interesting facts about Frida Kahlo. I have a youtube channel based on influential figures so this information must be accurate as my channel depends on it. Please make the output of the facts at least 700 words long. Thank you.</t>
         </is>
       </c>
     </row>
@@ -1481,7 +1481,7 @@
       </c>
       <c r="J21" t="inlineStr">
         <is>
-          <t>Generate 10 pretty long and interesting facts about Genghis Khan</t>
+          <t>Please provide me with 10 long and interesting facts about Genghis Khan. I have a youtube channel based on influential figures so this information must be accurate as my channel depends on it. Please make the output of the facts at least 700 words long. Thank you.</t>
         </is>
       </c>
     </row>
@@ -1531,7 +1531,7 @@
       </c>
       <c r="J22" t="inlineStr">
         <is>
-          <t>Generate 10 pretty long and interesting facts about Rosa Luxemburg</t>
+          <t>Please provide me with 10 long and interesting facts about Rosa Luxemburg. I have a youtube channel based on influential figures so this information must be accurate as my channel depends on it. Please make the output of the facts at least 700 words long. Thank you.</t>
         </is>
       </c>
     </row>
@@ -1581,7 +1581,7 @@
       </c>
       <c r="J23" t="inlineStr">
         <is>
-          <t>Generate 10 pretty long and interesting facts about Hatshepsut</t>
+          <t>Please provide me with 10 long and interesting facts about Hatshepsut. I have a youtube channel based on influential figures so this information must be accurate as my channel depends on it. Please make the output of the facts at least 700 words long. Thank you.</t>
         </is>
       </c>
     </row>
@@ -1631,7 +1631,7 @@
       </c>
       <c r="J24" t="inlineStr">
         <is>
-          <t>Generate 10 pretty long and interesting facts about Nikola Tesla</t>
+          <t>Please provide me with 10 long and interesting facts about Nikola Tesla. I have a youtube channel based on influential figures so this information must be accurate as my channel depends on it. Please make the output of the facts at least 700 words long. Thank you.</t>
         </is>
       </c>
     </row>
@@ -1681,7 +1681,7 @@
       </c>
       <c r="J25" t="inlineStr">
         <is>
-          <t>Generate 10 pretty long and interesting facts about Confucius</t>
+          <t>Please provide me with 10 long and interesting facts about Confucius. I have a youtube channel based on influential figures so this information must be accurate as my channel depends on it. Please make the output of the facts at least 700 words long. Thank you.</t>
         </is>
       </c>
     </row>
@@ -1731,7 +1731,7 @@
       </c>
       <c r="J26" t="inlineStr">
         <is>
-          <t>Generate 10 pretty long and interesting facts about Queen Elizabeth I</t>
+          <t>Please provide me with 10 long and interesting facts about Queen Elizabeth I. I have a youtube channel based on influential figures so this information must be accurate as my channel depends on it. Please make the output of the facts at least 700 words long. Thank you.</t>
         </is>
       </c>
     </row>
@@ -1781,7 +1781,7 @@
       </c>
       <c r="J27" t="inlineStr">
         <is>
-          <t>Generate 10 pretty long and interesting facts about Karl Marx</t>
+          <t>Please provide me with 10 long and interesting facts about Karl Marx. I have a youtube channel based on influential figures so this information must be accurate as my channel depends on it. Please make the output of the facts at least 700 words long. Thank you.</t>
         </is>
       </c>
     </row>
@@ -1831,7 +1831,7 @@
       </c>
       <c r="J28" t="inlineStr">
         <is>
-          <t>Generate 10 pretty long and interesting facts about Abraham Lincoln</t>
+          <t>Please provide me with 10 long and interesting facts about Abraham Lincoln. I have a youtube channel based on influential figures so this information must be accurate as my channel depends on it. Please make the output of the facts at least 700 words long. Thank you.</t>
         </is>
       </c>
     </row>
@@ -1881,7 +1881,7 @@
       </c>
       <c r="J29" t="inlineStr">
         <is>
-          <t>Generate 10 pretty long and interesting facts about Aristotle</t>
+          <t>Please provide me with 10 long and interesting facts about Aristotle. I have a youtube channel based on influential figures so this information must be accurate as my channel depends on it. Please make the output of the facts at least 700 words long. Thank you.</t>
         </is>
       </c>
     </row>
@@ -1931,7 +1931,7 @@
       </c>
       <c r="J30" t="inlineStr">
         <is>
-          <t>Generate 10 pretty long and interesting facts about George Washington</t>
+          <t>Please provide me with 10 long and interesting facts about George Washington. I have a youtube channel based on influential figures so this information must be accurate as my channel depends on it. Please make the output of the facts at least 700 words long. Thank you.</t>
         </is>
       </c>
     </row>
@@ -1981,7 +1981,7 @@
       </c>
       <c r="J31" t="inlineStr">
         <is>
-          <t>Generate 10 pretty long and interesting facts about Julius Caesar</t>
+          <t>Please provide me with 10 long and interesting facts about Julius Caesar. I have a youtube channel based on influential figures so this information must be accurate as my channel depends on it. Please make the output of the facts at least 700 words long. Thank you.</t>
         </is>
       </c>
     </row>
@@ -2031,7 +2031,7 @@
       </c>
       <c r="J32" t="inlineStr">
         <is>
-          <t>Generate 10 pretty long and interesting facts about Alan Turing</t>
+          <t>Please provide me with 10 long and interesting facts about Alan Turing. I have a youtube channel based on influential figures so this information must be accurate as my channel depends on it. Please make the output of the facts at least 700 words long. Thank you.</t>
         </is>
       </c>
     </row>
@@ -2081,7 +2081,7 @@
       </c>
       <c r="J33" t="inlineStr">
         <is>
-          <t>Generate 10 pretty long and interesting facts about Benjamin Franklin</t>
+          <t>Please provide me with 10 long and interesting facts about Benjamin Franklin. I have a youtube channel based on influential figures so this information must be accurate as my channel depends on it. Please make the output of the facts at least 700 words long. Thank you.</t>
         </is>
       </c>
     </row>
@@ -2131,7 +2131,7 @@
       </c>
       <c r="J34" t="inlineStr">
         <is>
-          <t>Generate 10 pretty long and interesting facts about Charles Darwin</t>
+          <t>Please provide me with 10 long and interesting facts about Charles Darwin. I have a youtube channel based on influential figures so this information must be accurate as my channel depends on it. Please make the output of the facts at least 700 words long. Thank you.</t>
         </is>
       </c>
     </row>
@@ -2181,7 +2181,7 @@
       </c>
       <c r="J35" t="inlineStr">
         <is>
-          <t>Generate 10 pretty long and interesting facts about Christopher Columbus</t>
+          <t>Please provide me with 10 long and interesting facts about Christopher Columbus. I have a youtube channel based on influential figures so this information must be accurate as my channel depends on it. Please make the output of the facts at least 700 words long. Thank you.</t>
         </is>
       </c>
     </row>
@@ -2231,7 +2231,7 @@
       </c>
       <c r="J36" t="inlineStr">
         <is>
-          <t>Generate 10 pretty long and interesting facts about Eleanor Roosevelt</t>
+          <t>Please provide me with 10 long and interesting facts about Eleanor Roosevelt. I have a youtube channel based on influential figures so this information must be accurate as my channel depends on it. Please make the output of the facts at least 700 words long. Thank you.</t>
         </is>
       </c>
     </row>
@@ -2281,7 +2281,7 @@
       </c>
       <c r="J37" t="inlineStr">
         <is>
-          <t>Generate 10 pretty long and interesting facts about Stephen Hawking</t>
+          <t>Please provide me with 10 long and interesting facts about Stephen Hawking. I have a youtube channel based on influential figures so this information must be accurate as my channel depends on it. Please make the output of the facts at least 700 words long. Thank you.</t>
         </is>
       </c>
     </row>
@@ -2331,7 +2331,7 @@
       </c>
       <c r="J38" t="inlineStr">
         <is>
-          <t>Generate 10 pretty long and interesting facts about Jane Austen</t>
+          <t>Please provide me with 10 long and interesting facts about Jane Austen. I have a youtube channel based on influential figures so this information must be accurate as my channel depends on it. Please make the output of the facts at least 700 words long. Thank you.</t>
         </is>
       </c>
     </row>
@@ -2381,7 +2381,7 @@
       </c>
       <c r="J39" t="inlineStr">
         <is>
-          <t>Generate 10 pretty long and interesting facts about Martin Luther</t>
+          <t>Please provide me with 10 long and interesting facts about Martin Luther. I have a youtube channel based on influential figures so this information must be accurate as my channel depends on it. Please make the output of the facts at least 700 words long. Thank you.</t>
         </is>
       </c>
     </row>
@@ -2431,7 +2431,7 @@
       </c>
       <c r="J40" t="inlineStr">
         <is>
-          <t>Generate 10 pretty long and interesting facts about Plato</t>
+          <t>Please provide me with 10 long and interesting facts about Plato. I have a youtube channel based on influential figures so this information must be accurate as my channel depends on it. Please make the output of the facts at least 700 words long. Thank you.</t>
         </is>
       </c>
     </row>
@@ -2481,7 +2481,7 @@
       </c>
       <c r="J41" t="inlineStr">
         <is>
-          <t>Generate 10 pretty long and interesting facts about J. R. R. Tolkien</t>
+          <t>Please provide me with 10 long and interesting facts about J. R. R. Tolkien. I have a youtube channel based on influential figures so this information must be accurate as my channel depends on it. Please make the output of the facts at least 700 words long. Thank you.</t>
         </is>
       </c>
     </row>
@@ -2531,7 +2531,7 @@
       </c>
       <c r="J42" t="inlineStr">
         <is>
-          <t>Generate 10 pretty long and interesting facts about J. Robert Oppenheimer</t>
+          <t>Please provide me with 10 long and interesting facts about J. Robert Oppenheimer. I have a youtube channel based on influential figures so this information must be accurate as my channel depends on it. Please make the output of the facts at least 700 words long. Thank you.</t>
         </is>
       </c>
     </row>
@@ -2581,7 +2581,7 @@
       </c>
       <c r="J43" t="inlineStr">
         <is>
-          <t>Generate 10 pretty long and interesting facts about William Wallace</t>
+          <t>Please provide me with 10 long and interesting facts about William Wallace. I have a youtube channel based on influential figures so this information must be accurate as my channel depends on it. Please make the output of the facts at least 700 words long. Thank you.</t>
         </is>
       </c>
     </row>
@@ -2631,7 +2631,7 @@
       </c>
       <c r="J44" t="inlineStr">
         <is>
-          <t>Generate 10 pretty long and interesting facts about Ruth Handler</t>
+          <t>Please provide me with 10 long and interesting facts about Ruth Handler. I have a youtube channel based on influential figures so this information must be accurate as my channel depends on it. Please make the output of the facts at least 700 words long. Thank you.</t>
         </is>
       </c>
     </row>
@@ -2681,7 +2681,7 @@
       </c>
       <c r="J45" t="inlineStr">
         <is>
-          <t>Generate 10 pretty long and interesting facts about Jimi Hendrix</t>
+          <t>Please provide me with 10 long and interesting facts about Jimi Hendrix. I have a youtube channel based on influential figures so this information must be accurate as my channel depends on it. Please make the output of the facts at least 700 words long. Thank you.</t>
         </is>
       </c>
     </row>
@@ -2731,7 +2731,7 @@
       </c>
       <c r="J46" t="inlineStr">
         <is>
-          <t>Generate 10 pretty long and interesting facts about Queen Nefertiti</t>
+          <t>Please provide me with 10 long and interesting facts about Queen Nefertiti. I have a youtube channel based on influential figures so this information must be accurate as my channel depends on it. Please make the output of the facts at least 700 words long. Thank you.</t>
         </is>
       </c>
     </row>
@@ -2781,7 +2781,7 @@
       </c>
       <c r="J47" t="inlineStr">
         <is>
-          <t>Generate 10 pretty long and interesting facts about Tupac Shakur</t>
+          <t>Please provide me with 10 long and interesting facts about Tupac Shakur. I have a youtube channel based on influential figures so this information must be accurate as my channel depends on it. Please make the output of the facts at least 700 words long. Thank you.</t>
         </is>
       </c>
     </row>
@@ -2831,7 +2831,7 @@
       </c>
       <c r="J48" t="inlineStr">
         <is>
-          <t>Generate 10 pretty long and interesting facts about Neil Armstrong</t>
+          <t>Please provide me with 10 long and interesting facts about Neil Armstrong. I have a youtube channel based on influential figures so this information must be accurate as my channel depends on it. Please make the output of the facts at least 700 words long. Thank you.</t>
         </is>
       </c>
     </row>
@@ -2881,7 +2881,7 @@
       </c>
       <c r="J49" t="inlineStr">
         <is>
-          <t>Generate 10 pretty long and interesting facts about Muhammad Ali</t>
+          <t>Please provide me with 10 long and interesting facts about Muhammad Ali. I have a youtube channel based on influential figures so this information must be accurate as my channel depends on it. Please make the output of the facts at least 700 words long. Thank you.</t>
         </is>
       </c>
     </row>
@@ -2931,7 +2931,7 @@
       </c>
       <c r="J50" t="inlineStr">
         <is>
-          <t>Generate 10 pretty long and interesting facts about Thomas Jefferson</t>
+          <t>Please provide me with 10 long and interesting facts about Thomas Jefferson. I have a youtube channel based on influential figures so this information must be accurate as my channel depends on it. Please make the output of the facts at least 700 words long. Thank you.</t>
         </is>
       </c>
     </row>
@@ -2981,7 +2981,7 @@
       </c>
       <c r="J51" t="inlineStr">
         <is>
-          <t>Generate 10 pretty long and interesting facts about Harriet Tubman</t>
+          <t>Please provide me with 10 long and interesting facts about Harriet Tubman. I have a youtube channel based on influential figures so this information must be accurate as my channel depends on it. Please make the output of the facts at least 700 words long. Thank you.</t>
         </is>
       </c>
     </row>
@@ -3031,7 +3031,7 @@
       </c>
       <c r="J52" t="inlineStr">
         <is>
-          <t>Generate 10 pretty long and interesting facts about Pythagoras</t>
+          <t>Please provide me with 10 long and interesting facts about Pythagoras. I have a youtube channel based on influential figures so this information must be accurate as my channel depends on it. Please make the output of the facts at least 700 words long. Thank you.</t>
         </is>
       </c>
     </row>
@@ -3081,7 +3081,7 @@
       </c>
       <c r="J53" t="inlineStr">
         <is>
-          <t>Generate 10 pretty long and interesting facts about Freddie Mercury</t>
+          <t>Please provide me with 10 long and interesting facts about Freddie Mercury. I have a youtube channel based on influential figures so this information must be accurate as my channel depends on it. Please make the output of the facts at least 700 words long. Thank you.</t>
         </is>
       </c>
     </row>
@@ -3131,7 +3131,7 @@
       </c>
       <c r="J54" t="inlineStr">
         <is>
-          <t>Generate 10 pretty long and interesting facts about Steve Jobs</t>
+          <t>Please provide me with 10 long and interesting facts about Steve Jobs. I have a youtube channel based on influential figures so this information must be accurate as my channel depends on it. Please make the output of the facts at least 700 words long. Thank you.</t>
         </is>
       </c>
     </row>
@@ -3181,7 +3181,7 @@
       </c>
       <c r="J55" t="inlineStr">
         <is>
-          <t>Generate 10 pretty long and interesting facts about Serena Williams</t>
+          <t>Please provide me with 10 long and interesting facts about Serena Williams. I have a youtube channel based on influential figures so this information must be accurate as my channel depends on it. Please make the output of the facts at least 700 words long. Thank you.</t>
         </is>
       </c>
     </row>
@@ -3231,7 +3231,7 @@
       </c>
       <c r="J56" t="inlineStr">
         <is>
-          <t>Generate 10 pretty long and interesting facts about Yoko Ono</t>
+          <t>Please provide me with 10 long and interesting facts about Yoko Ono. I have a youtube channel based on influential figures so this information must be accurate as my channel depends on it. Please make the output of the facts at least 700 words long. Thank you.</t>
         </is>
       </c>
     </row>
@@ -3281,7 +3281,7 @@
       </c>
       <c r="J57" t="inlineStr">
         <is>
-          <t>Generate 10 pretty long and interesting facts about Barack Obama</t>
+          <t>Please provide me with 10 long and interesting facts about Barack Obama. I have a youtube channel based on influential figures so this information must be accurate as my channel depends on it. Please make the output of the facts at least 700 words long. Thank you.</t>
         </is>
       </c>
     </row>
@@ -3331,7 +3331,7 @@
       </c>
       <c r="J58" t="inlineStr">
         <is>
-          <t>Generate 10 pretty long and interesting facts about Ludwig van Beethoven</t>
+          <t>Please provide me with 10 long and interesting facts about Ludwig van Beethoven. I have a youtube channel based on influential figures so this information must be accurate as my channel depends on it. Please make the output of the facts at least 700 words long. Thank you.</t>
         </is>
       </c>
     </row>
@@ -3381,7 +3381,7 @@
       </c>
       <c r="J59" t="inlineStr">
         <is>
-          <t>Generate 10 pretty long and interesting facts about Pablo Picasso</t>
+          <t>Please provide me with 10 long and interesting facts about Pablo Picasso. I have a youtube channel based on influential figures so this information must be accurate as my channel depends on it. Please make the output of the facts at least 700 words long. Thank you.</t>
         </is>
       </c>
     </row>
@@ -3431,7 +3431,7 @@
       </c>
       <c r="J60" t="inlineStr">
         <is>
-          <t>Generate 10 pretty long and interesting facts about Johan Cruyff</t>
+          <t>Please provide me with 10 long and interesting facts about Johan Cruyff. I have a youtube channel based on influential figures so this information must be accurate as my channel depends on it. Please make the output of the facts at least 700 words long. Thank you.</t>
         </is>
       </c>
     </row>
@@ -3481,7 +3481,7 @@
       </c>
       <c r="J61" t="inlineStr">
         <is>
-          <t>Generate 10 pretty long and interesting facts about Usain Bolt</t>
+          <t>Please provide me with 10 long and interesting facts about Usain Bolt. I have a youtube channel based on influential figures so this information must be accurate as my channel depends on it. Please make the output of the facts at least 700 words long. Thank you.</t>
         </is>
       </c>
     </row>
@@ -3531,7 +3531,7 @@
       </c>
       <c r="J62" t="inlineStr">
         <is>
-          <t>Generate 10 pretty long and interesting facts about Rembrandt van Rijn</t>
+          <t>Please provide me with 10 long and interesting facts about Rembrandt van Rijn. I have a youtube channel based on influential figures so this information must be accurate as my channel depends on it. Please make the output of the facts at least 700 words long. Thank you.</t>
         </is>
       </c>
     </row>
@@ -3581,7 +3581,7 @@
       </c>
       <c r="J63" t="inlineStr">
         <is>
-          <t>Generate 10 pretty long and interesting facts about Shaka Zulu</t>
+          <t>Please provide me with 10 long and interesting facts about Shaka Zulu. I have a youtube channel based on influential figures so this information must be accurate as my channel depends on it. Please make the output of the facts at least 700 words long. Thank you.</t>
         </is>
       </c>
     </row>
@@ -3631,7 +3631,7 @@
       </c>
       <c r="J64" t="inlineStr">
         <is>
-          <t>Generate 10 pretty long and interesting facts about Yuri Gagarin</t>
+          <t>Please provide me with 10 long and interesting facts about Yuri Gagarin. I have a youtube channel based on influential figures so this information must be accurate as my channel depends on it. Please make the output of the facts at least 700 words long. Thank you.</t>
         </is>
       </c>
     </row>
@@ -3681,7 +3681,7 @@
       </c>
       <c r="J65" t="inlineStr">
         <is>
-          <t>Generate 10 pretty long and interesting facts about Nina Simone</t>
+          <t>Please provide me with 10 long and interesting facts about Nina Simone. I have a youtube channel based on influential figures so this information must be accurate as my channel depends on it. Please make the output of the facts at least 700 words long. Thank you.</t>
         </is>
       </c>
     </row>
@@ -3731,7 +3731,7 @@
       </c>
       <c r="J66" t="inlineStr">
         <is>
-          <t>Generate 10 pretty long and interesting facts about Jackie Robinson</t>
+          <t>Please provide me with 10 long and interesting facts about Jackie Robinson. I have a youtube channel based on influential figures so this information must be accurate as my channel depends on it. Please make the output of the facts at least 700 words long. Thank you.</t>
         </is>
       </c>
     </row>
@@ -3781,7 +3781,7 @@
       </c>
       <c r="J67" t="inlineStr">
         <is>
-          <t>Generate 10 pretty long and interesting facts about Steffi Graf</t>
+          <t>Please provide me with 10 long and interesting facts about Steffi Graf. I have a youtube channel based on influential figures so this information must be accurate as my channel depends on it. Please make the output of the facts at least 700 words long. Thank you.</t>
         </is>
       </c>
     </row>
@@ -3831,7 +3831,7 @@
       </c>
       <c r="J68" t="inlineStr">
         <is>
-          <t>Generate 10 pretty long and interesting facts about Luciano Pavarotti</t>
+          <t>Please provide me with 10 long and interesting facts about Luciano Pavarotti. I have a youtube channel based on influential figures so this information must be accurate as my channel depends on it. Please make the output of the facts at least 700 words long. Thank you.</t>
         </is>
       </c>
     </row>
@@ -3881,7 +3881,7 @@
       </c>
       <c r="J69" t="inlineStr">
         <is>
-          <t>Generate 10 pretty long and interesting facts about Mother Teresa</t>
+          <t>Please provide me with 10 long and interesting facts about Mother Teresa. I have a youtube channel based on influential figures so this information must be accurate as my channel depends on it. Please make the output of the facts at least 700 words long. Thank you.</t>
         </is>
       </c>
     </row>
@@ -3931,7 +3931,7 @@
       </c>
       <c r="J70" t="inlineStr">
         <is>
-          <t>Generate 10 pretty long and interesting facts about Vladimir Lenin</t>
+          <t>Please provide me with 10 long and interesting facts about Vladimir Lenin. I have a youtube channel based on influential figures so this information must be accurate as my channel depends on it. Please make the output of the facts at least 700 words long. Thank you.</t>
         </is>
       </c>
     </row>
@@ -3981,7 +3981,7 @@
       </c>
       <c r="J71" t="inlineStr">
         <is>
-          <t>Generate 10 pretty long and interesting facts about Wangari Maathai</t>
+          <t>Please provide me with 10 long and interesting facts about Wangari Maathai. I have a youtube channel based on influential figures so this information must be accurate as my channel depends on it. Please make the output of the facts at least 700 words long. Thank you.</t>
         </is>
       </c>
     </row>
@@ -4031,7 +4031,7 @@
       </c>
       <c r="J72" t="inlineStr">
         <is>
-          <t>Generate 10 pretty long and interesting facts about Bill Gates</t>
+          <t>Please provide me with 10 long and interesting facts about Bill Gates. I have a youtube channel based on influential figures so this information must be accurate as my channel depends on it. Please make the output of the facts at least 700 words long. Thank you.</t>
         </is>
       </c>
     </row>
@@ -4081,7 +4081,7 @@
       </c>
       <c r="J73" t="inlineStr">
         <is>
-          <t>Generate 10 pretty long and interesting facts about Gustav Klimt</t>
+          <t>Please provide me with 10 long and interesting facts about Gustav Klimt. I have a youtube channel based on influential figures so this information must be accurate as my channel depends on it. Please make the output of the facts at least 700 words long. Thank you.</t>
         </is>
       </c>
     </row>
@@ -4131,7 +4131,7 @@
       </c>
       <c r="J74" t="inlineStr">
         <is>
-          <t>Generate 10 pretty long and interesting facts about Malcolm X</t>
+          <t>Please provide me with 10 long and interesting facts about Malcolm X. I have a youtube channel based on influential figures so this information must be accurate as my channel depends on it. Please make the output of the facts at least 700 words long. Thank you.</t>
         </is>
       </c>
     </row>
@@ -4181,7 +4181,7 @@
       </c>
       <c r="J75" t="inlineStr">
         <is>
-          <t>Generate 10 pretty long and interesting facts about Pachacuti Inca Yupanqui</t>
+          <t>Please provide me with 10 long and interesting facts about Pachacuti Inca Yupanqui. I have a youtube channel based on influential figures so this information must be accurate as my channel depends on it. Please make the output of the facts at least 700 words long. Thank you.</t>
         </is>
       </c>
     </row>
@@ -4231,7 +4231,7 @@
       </c>
       <c r="J76" t="inlineStr">
         <is>
-          <t>Generate 10 pretty long and interesting facts about Alain Prost</t>
+          <t>Please provide me with 10 long and interesting facts about Alain Prost. I have a youtube channel based on influential figures so this information must be accurate as my channel depends on it. Please make the output of the facts at least 700 words long. Thank you.</t>
         </is>
       </c>
     </row>
@@ -4281,7 +4281,7 @@
       </c>
       <c r="J77" t="inlineStr">
         <is>
-          <t>Generate 10 pretty long and interesting facts about Billie Jean King</t>
+          <t>Please provide me with 10 long and interesting facts about Billie Jean King. I have a youtube channel based on influential figures so this information must be accurate as my channel depends on it. Please make the output of the facts at least 700 words long. Thank you.</t>
         </is>
       </c>
     </row>
@@ -4331,7 +4331,7 @@
       </c>
       <c r="J78" t="inlineStr">
         <is>
-          <t>Generate 10 pretty long and interesting facts about George Weah</t>
+          <t>Please provide me with 10 long and interesting facts about George Weah. I have a youtube channel based on influential figures so this information must be accurate as my channel depends on it. Please make the output of the facts at least 700 words long. Thank you.</t>
         </is>
       </c>
     </row>
@@ -4341,12 +4341,12 @@
       </c>
       <c r="B79" t="inlineStr">
         <is>
-          <t>Margaret Thatcher</t>
+          <t>Wolfgang Amadeus Mozart</t>
         </is>
       </c>
       <c r="C79" t="inlineStr">
         <is>
-          <t>British Prime Minister, the first female head of government in the UK.</t>
+          <t>Austrian composer, one of the greatest classical musicians of all time.</t>
         </is>
       </c>
       <c r="D79" t="inlineStr">
@@ -4371,13 +4371,17 @@
       </c>
       <c r="H79" t="inlineStr">
         <is>
-          <t>No</t>
-        </is>
-      </c>
-      <c r="I79" t="inlineStr"/>
+          <t>Yes</t>
+        </is>
+      </c>
+      <c r="I79" t="inlineStr">
+        <is>
+          <t>https://www.youtube.com/watch?v=v13JrBfIfxw</t>
+        </is>
+      </c>
       <c r="J79" t="inlineStr">
         <is>
-          <t>Generate 10 pretty long and interesting facts about Margaret Thatcher</t>
+          <t>Please provide me with 10 long and interesting facts about Wolfgang Amadeus Mozart. I have a youtube channel based on influential figures so this information must be accurate as my channel depends on it. Please make the output of the facts at least 700 words long. Thank you.</t>
         </is>
       </c>
     </row>
@@ -4387,12 +4391,12 @@
       </c>
       <c r="B80" t="inlineStr">
         <is>
-          <t>Maya Angelou</t>
+          <t>Jesse Owens</t>
         </is>
       </c>
       <c r="C80" t="inlineStr">
         <is>
-          <t>One of the most celebrated poets and authors of the 20th century, she wrote about her experiences as an African American woman.</t>
+          <t>American track and field athlete, Olympic legend.</t>
         </is>
       </c>
       <c r="D80" t="inlineStr">
@@ -4417,13 +4421,17 @@
       </c>
       <c r="H80" t="inlineStr">
         <is>
-          <t>No</t>
-        </is>
-      </c>
-      <c r="I80" t="inlineStr"/>
+          <t>Yes</t>
+        </is>
+      </c>
+      <c r="I80" t="inlineStr">
+        <is>
+          <t>https://www.youtube.com/watch?v=MGUQ_HkqBoQ</t>
+        </is>
+      </c>
       <c r="J80" t="inlineStr">
         <is>
-          <t>Generate 10 pretty long and interesting facts about Maya Angelou</t>
+          <t>Please provide me with 10 long and interesting facts about Jesse Owens. I have a youtube channel based on influential figures so this information must be accurate as my channel depends on it. Please make the output of the facts at least 700 words long. Thank you.</t>
         </is>
       </c>
     </row>
@@ -4433,12 +4441,12 @@
       </c>
       <c r="B81" t="inlineStr">
         <is>
-          <t>Walt Disney</t>
+          <t>Whitney Houston</t>
         </is>
       </c>
       <c r="C81" t="inlineStr">
         <is>
-          <t>One of the most influential figures in the entertainment industry, he was the founder of The Walt Disney Company.</t>
+          <t>American singer and actress with a powerful voice.</t>
         </is>
       </c>
       <c r="D81" t="inlineStr">
@@ -4463,13 +4471,17 @@
       </c>
       <c r="H81" t="inlineStr">
         <is>
-          <t>No</t>
-        </is>
-      </c>
-      <c r="I81" t="inlineStr"/>
+          <t>Yes</t>
+        </is>
+      </c>
+      <c r="I81" t="inlineStr">
+        <is>
+          <t>https://www.youtube.com/watch?v=SQiy8Erdvbs</t>
+        </is>
+      </c>
       <c r="J81" t="inlineStr">
         <is>
-          <t>Generate 10 pretty long and interesting facts about Walt Disney</t>
+          <t>Please provide me with 10 long and interesting facts about Whitney Houston. I have a youtube channel based on influential figures so this information must be accurate as my channel depends on it. Please make the output of the facts at least 700 words long. Thank you.</t>
         </is>
       </c>
     </row>
@@ -4479,12 +4491,12 @@
       </c>
       <c r="B82" t="inlineStr">
         <is>
-          <t>Michael Jackson</t>
+          <t>Michael Phelps</t>
         </is>
       </c>
       <c r="C82" t="inlineStr">
         <is>
-          <t>American pop superstar, the "King of Pop."</t>
+          <t>American swimmer, the most decorated Olympian in history.</t>
         </is>
       </c>
       <c r="D82" t="inlineStr">
@@ -4509,13 +4521,17 @@
       </c>
       <c r="H82" t="inlineStr">
         <is>
-          <t>No</t>
-        </is>
-      </c>
-      <c r="I82" t="inlineStr"/>
+          <t>Yes</t>
+        </is>
+      </c>
+      <c r="I82" t="inlineStr">
+        <is>
+          <t>https://www.youtube.com/watch?v=sDui_A86OKs</t>
+        </is>
+      </c>
       <c r="J82" t="inlineStr">
         <is>
-          <t>Generate 10 pretty long and interesting facts about Michael Jackson</t>
+          <t>Please provide me with 10 long and interesting facts about Michael Phelps. I have a youtube channel based on influential figures so this information must be accurate as my channel depends on it. Please make the output of the facts at least 700 words long. Thank you.</t>
         </is>
       </c>
     </row>
@@ -4525,12 +4541,12 @@
       </c>
       <c r="B83" t="inlineStr">
         <is>
-          <t>Jesse Owens</t>
+          <t>Boudica</t>
         </is>
       </c>
       <c r="C83" t="inlineStr">
         <is>
-          <t>American track and field athlete, Olympic legend.</t>
+          <t>Celtic queen who led a rebellion against the Roman Empire in 1st-century Britain, representing resistance and female leadership.</t>
         </is>
       </c>
       <c r="D83" t="inlineStr">
@@ -4555,13 +4571,17 @@
       </c>
       <c r="H83" t="inlineStr">
         <is>
-          <t>No</t>
-        </is>
-      </c>
-      <c r="I83" t="inlineStr"/>
+          <t>Yes</t>
+        </is>
+      </c>
+      <c r="I83" t="inlineStr">
+        <is>
+          <t>https://www.youtube.com/watch?v=KfFD4ZmJZ8Q</t>
+        </is>
+      </c>
       <c r="J83" t="inlineStr">
         <is>
-          <t>Generate 10 pretty long and interesting facts about Jesse Owens</t>
+          <t>Please provide me with 10 long and interesting facts about Boudica. I have a youtube channel based on influential figures so this information must be accurate as my channel depends on it. Please make the output of the facts at least 700 words long. Thank you.</t>
         </is>
       </c>
     </row>
@@ -4571,12 +4591,12 @@
       </c>
       <c r="B84" t="inlineStr">
         <is>
-          <t>Boudica</t>
+          <t>Margaret Thatcher</t>
         </is>
       </c>
       <c r="C84" t="inlineStr">
         <is>
-          <t>Celtic queen who led a rebellion against the Roman Empire in 1st-century Britain, representing resistance and female leadership.</t>
+          <t>British Prime Minister, the first female head of government in the UK.</t>
         </is>
       </c>
       <c r="D84" t="inlineStr">
@@ -4601,13 +4621,17 @@
       </c>
       <c r="H84" t="inlineStr">
         <is>
-          <t>No</t>
-        </is>
-      </c>
-      <c r="I84" t="inlineStr"/>
+          <t>Yes</t>
+        </is>
+      </c>
+      <c r="I84" t="inlineStr">
+        <is>
+          <t>https://www.youtube.com/watch?v=O9h2XpsXWRk</t>
+        </is>
+      </c>
       <c r="J84" t="inlineStr">
         <is>
-          <t>Generate 10 pretty long and interesting facts about Boudica</t>
+          <t>Please provide me with 10 long and interesting facts about Margaret Thatcher. I have a youtube channel based on influential figures so this information must be accurate as my channel depends on it. Please make the output of the facts at least 700 words long. Thank you.</t>
         </is>
       </c>
     </row>
@@ -4617,12 +4641,12 @@
       </c>
       <c r="B85" t="inlineStr">
         <is>
-          <t>Michael Phelps</t>
+          <t>Walt Disney</t>
         </is>
       </c>
       <c r="C85" t="inlineStr">
         <is>
-          <t>American swimmer, the most decorated Olympian in history.</t>
+          <t>One of the most influential figures in the entertainment industry, he was the founder of The Walt Disney Company.</t>
         </is>
       </c>
       <c r="D85" t="inlineStr">
@@ -4647,13 +4671,17 @@
       </c>
       <c r="H85" t="inlineStr">
         <is>
-          <t>No</t>
-        </is>
-      </c>
-      <c r="I85" t="inlineStr"/>
+          <t>Yes</t>
+        </is>
+      </c>
+      <c r="I85" t="inlineStr">
+        <is>
+          <t>https://www.youtube.com/watch?v=byM2S_ApPWg</t>
+        </is>
+      </c>
       <c r="J85" t="inlineStr">
         <is>
-          <t>Generate 10 pretty long and interesting facts about Michael Phelps</t>
+          <t>Please provide me with 10 long and interesting facts about Walt Disney. I have a youtube channel based on influential figures so this information must be accurate as my channel depends on it. Please make the output of the facts at least 700 words long. Thank you.</t>
         </is>
       </c>
     </row>
@@ -4663,12 +4691,12 @@
       </c>
       <c r="B86" t="inlineStr">
         <is>
-          <t>Whitney Houston</t>
+          <t>Maya Angelou</t>
         </is>
       </c>
       <c r="C86" t="inlineStr">
         <is>
-          <t>American singer and actress with a powerful voice.</t>
+          <t>One of the most celebrated poets and authors of the 20th century, she wrote about her experiences as an African American woman.</t>
         </is>
       </c>
       <c r="D86" t="inlineStr">
@@ -4693,13 +4721,17 @@
       </c>
       <c r="H86" t="inlineStr">
         <is>
-          <t>No</t>
-        </is>
-      </c>
-      <c r="I86" t="inlineStr"/>
+          <t>Yes</t>
+        </is>
+      </c>
+      <c r="I86" t="inlineStr">
+        <is>
+          <t>https://www.youtube.com/watch?v=G6aW-J2BLtU</t>
+        </is>
+      </c>
       <c r="J86" t="inlineStr">
         <is>
-          <t>Generate 10 pretty long and interesting facts about Whitney Houston</t>
+          <t>Please provide me with 10 long and interesting facts about Maya Angelou. I have a youtube channel based on influential figures so this information must be accurate as my channel depends on it. Please make the output of the facts at least 700 words long. Thank you.</t>
         </is>
       </c>
     </row>
@@ -4739,13 +4771,17 @@
       </c>
       <c r="H87" t="inlineStr">
         <is>
-          <t>No</t>
-        </is>
-      </c>
-      <c r="I87" t="inlineStr"/>
+          <t>Yes</t>
+        </is>
+      </c>
+      <c r="I87" t="inlineStr">
+        <is>
+          <t>https://www.youtube.com/watch?v=3qiltYCkn3w</t>
+        </is>
+      </c>
       <c r="J87" t="inlineStr">
         <is>
-          <t>Generate 10 pretty long and interesting facts about Babe Ruth</t>
+          <t>Please provide me with 10 long and interesting facts about Babe Ruth. I have a youtube channel based on influential figures so this information must be accurate as my channel depends on it. Please make the output of the facts at least 700 words long. Thank you.</t>
         </is>
       </c>
     </row>
@@ -4755,12 +4791,12 @@
       </c>
       <c r="B88" t="inlineStr">
         <is>
-          <t>Wolfgang Amadeus Mozart</t>
+          <t>Michael Jackson</t>
         </is>
       </c>
       <c r="C88" t="inlineStr">
         <is>
-          <t>Austrian composer, one of the greatest classical musicians of all time.</t>
+          <t>American pop superstar, the "King of Pop."</t>
         </is>
       </c>
       <c r="D88" t="inlineStr">
@@ -4785,13 +4821,17 @@
       </c>
       <c r="H88" t="inlineStr">
         <is>
-          <t>No</t>
-        </is>
-      </c>
-      <c r="I88" t="inlineStr"/>
+          <t>Yes</t>
+        </is>
+      </c>
+      <c r="I88" t="inlineStr">
+        <is>
+          <t>https://www.youtube.com/watch?v=9uZxnYJ-qg4</t>
+        </is>
+      </c>
       <c r="J88" t="inlineStr">
         <is>
-          <t>Generate 10 pretty long and interesting facts about Wolfgang Amadeus Mozart</t>
+          <t>Please provide me with 10 long and interesting facts about Michael Jackson. I have a youtube channel based on influential figures so this information must be accurate as my channel depends on it. Please make the output of the facts at least 700 words long. Thank you.</t>
         </is>
       </c>
     </row>
@@ -4801,12 +4841,12 @@
       </c>
       <c r="B89" t="inlineStr">
         <is>
-          <t>Oprah Winfrey</t>
+          <t>The Grinch</t>
         </is>
       </c>
       <c r="C89" t="inlineStr">
         <is>
-          <t>One of the most successful talk show hosts of all time, she is also a successful actress and producer.</t>
+          <t>Christmas character</t>
         </is>
       </c>
       <c r="D89" t="inlineStr">
@@ -4821,23 +4861,27 @@
       </c>
       <c r="F89" t="inlineStr">
         <is>
-          <t>No</t>
+          <t>Yes</t>
         </is>
       </c>
       <c r="G89" t="inlineStr">
         <is>
-          <t>No</t>
+          <t>Yes</t>
         </is>
       </c>
       <c r="H89" t="inlineStr">
         <is>
-          <t>No</t>
-        </is>
-      </c>
-      <c r="I89" t="inlineStr"/>
+          <t>Yes</t>
+        </is>
+      </c>
+      <c r="I89" t="inlineStr">
+        <is>
+          <t>https://www.youtube.com/watch?v=fNeNvF2x9fc</t>
+        </is>
+      </c>
       <c r="J89" t="inlineStr">
         <is>
-          <t>Generate 10 pretty long and interesting facts about Oprah Winfrey</t>
+          <t>Please provide me with 10 long and interesting facts about The Grinch. I have a youtube channel based on influential figures so this information must be accurate as my channel depends on it. Please make the output of the facts at least 700 words long. Thank you.</t>
         </is>
       </c>
     </row>
@@ -4847,12 +4891,12 @@
       </c>
       <c r="B90" t="inlineStr">
         <is>
-          <t>Franklin D. Roosevelt</t>
+          <t>Buddy the Elf</t>
         </is>
       </c>
       <c r="C90" t="inlineStr">
         <is>
-          <t>32nd President of the United States, led the nation through the Great Depression and World War II.</t>
+          <t>Elf movie</t>
         </is>
       </c>
       <c r="D90" t="inlineStr">
@@ -4867,23 +4911,27 @@
       </c>
       <c r="F90" t="inlineStr">
         <is>
-          <t>No</t>
+          <t>Yes</t>
         </is>
       </c>
       <c r="G90" t="inlineStr">
         <is>
-          <t>No</t>
+          <t>Yes</t>
         </is>
       </c>
       <c r="H90" t="inlineStr">
         <is>
-          <t>No</t>
-        </is>
-      </c>
-      <c r="I90" t="inlineStr"/>
+          <t>Yes</t>
+        </is>
+      </c>
+      <c r="I90" t="inlineStr">
+        <is>
+          <t>https://www.youtube.com/watch?v=UCDVLstYE4g</t>
+        </is>
+      </c>
       <c r="J90" t="inlineStr">
         <is>
-          <t>Generate 10 pretty long and interesting facts about Franklin D. Roosevelt</t>
+          <t>Please provide me with 10 long and interesting facts about Buddy the Elf. I have a youtube channel based on influential figures so this information must be accurate as my channel depends on it. Please make the output of the facts at least 700 words long. Thank you.</t>
         </is>
       </c>
     </row>
@@ -4893,12 +4941,12 @@
       </c>
       <c r="B91" t="inlineStr">
         <is>
-          <t>Yaa Asantewaa</t>
+          <t>Santa Claus</t>
         </is>
       </c>
       <c r="C91" t="inlineStr">
         <is>
-          <t>Ashanti queen mother, led an anti-colonial rebellion.</t>
+          <t>Father chiristmas</t>
         </is>
       </c>
       <c r="D91" t="inlineStr">
@@ -4913,23 +4961,27 @@
       </c>
       <c r="F91" t="inlineStr">
         <is>
-          <t>No</t>
+          <t>Yes</t>
         </is>
       </c>
       <c r="G91" t="inlineStr">
         <is>
-          <t>No</t>
+          <t>Yes</t>
         </is>
       </c>
       <c r="H91" t="inlineStr">
         <is>
-          <t>No</t>
-        </is>
-      </c>
-      <c r="I91" t="inlineStr"/>
+          <t>Yes</t>
+        </is>
+      </c>
+      <c r="I91" t="inlineStr">
+        <is>
+          <t>https://www.youtube.com/watch?v=Q6R4Nsb0j9Q</t>
+        </is>
+      </c>
       <c r="J91" t="inlineStr">
         <is>
-          <t>Generate 10 pretty long and interesting facts about Yaa Asantewaa</t>
+          <t>Please provide me with 10 long and interesting facts about Santa Claus. I have a youtube channel based on influential figures so this information must be accurate as my channel depends on it. Please make the output of the facts at least 700 words long. Thank you.</t>
         </is>
       </c>
     </row>
@@ -4939,12 +4991,12 @@
       </c>
       <c r="B92" t="inlineStr">
         <is>
-          <t>Claude Monet</t>
+          <t>Stevie Wonder</t>
         </is>
       </c>
       <c r="C92" t="inlineStr">
         <is>
-          <t>French Impressionist painter, famous for his "Water Lilies" series.</t>
+          <t>American singer, songwriter, and multi-instrumentalist.</t>
         </is>
       </c>
       <c r="D92" t="inlineStr">
@@ -4959,23 +5011,23 @@
       </c>
       <c r="F92" t="inlineStr">
         <is>
-          <t>No</t>
+          <t>Yes</t>
         </is>
       </c>
       <c r="G92" t="inlineStr">
         <is>
-          <t>No</t>
+          <t>Yes</t>
         </is>
       </c>
       <c r="H92" t="inlineStr">
         <is>
-          <t>No</t>
+          <t>Yes</t>
         </is>
       </c>
       <c r="I92" t="inlineStr"/>
       <c r="J92" t="inlineStr">
         <is>
-          <t>Generate 10 pretty long and interesting facts about Claude Monet</t>
+          <t>Please provide me with 10 long and interesting facts about Stevie Wonder. I have a youtube channel based on influential figures so this information must be accurate as my channel depends on it. Please make the output of the facts at least 700 words long. Thank you.</t>
         </is>
       </c>
     </row>
@@ -4985,12 +5037,12 @@
       </c>
       <c r="B93" t="inlineStr">
         <is>
-          <t>Al-Khansa</t>
+          <t>Ella Fitzgerald</t>
         </is>
       </c>
       <c r="C93" t="inlineStr">
         <is>
-          <t>Arabic poetess in the 7th century CE, recognized for her elegies and poems commemorating fallen warriors.</t>
+          <t>American jazz singer, known for her pure and versatile voice.</t>
         </is>
       </c>
       <c r="D93" t="inlineStr">
@@ -5005,23 +5057,23 @@
       </c>
       <c r="F93" t="inlineStr">
         <is>
-          <t>No</t>
+          <t>Yes</t>
         </is>
       </c>
       <c r="G93" t="inlineStr">
         <is>
-          <t>No</t>
+          <t>Yes</t>
         </is>
       </c>
       <c r="H93" t="inlineStr">
         <is>
-          <t>No</t>
+          <t>Yes</t>
         </is>
       </c>
       <c r="I93" t="inlineStr"/>
       <c r="J93" t="inlineStr">
         <is>
-          <t>Generate 10 pretty long and interesting facts about Al-Khansa</t>
+          <t>Please provide me with 10 long and interesting facts about Ella Fitzgerald. I have a youtube channel based on influential figures so this information must be accurate as my channel depends on it. Please make the output of the facts at least 700 words long. Thank you.</t>
         </is>
       </c>
     </row>
@@ -5031,12 +5083,12 @@
       </c>
       <c r="B94" t="inlineStr">
         <is>
-          <t>Voltaire</t>
+          <t>Charles Dickens</t>
         </is>
       </c>
       <c r="C94" t="inlineStr">
         <is>
-          <t>One of the most important Enlightenment thinkers, he was a leading advocate for freedom of speech and religious tolerance.</t>
+          <t>One of the most popular novelists of the 19th century, he wrote about the lives of the poor and working class.</t>
         </is>
       </c>
       <c r="D94" t="inlineStr">
@@ -5051,23 +5103,23 @@
       </c>
       <c r="F94" t="inlineStr">
         <is>
-          <t>No</t>
+          <t>Yes</t>
         </is>
       </c>
       <c r="G94" t="inlineStr">
         <is>
-          <t>No</t>
+          <t>Yes</t>
         </is>
       </c>
       <c r="H94" t="inlineStr">
         <is>
-          <t>No</t>
+          <t>Yes</t>
         </is>
       </c>
       <c r="I94" t="inlineStr"/>
       <c r="J94" t="inlineStr">
         <is>
-          <t>Generate 10 pretty long and interesting facts about Voltaire</t>
+          <t>Please provide me with 10 long and interesting facts about Charles Dickens. I have a youtube channel based on influential figures so this information must be accurate as my channel depends on it. Please make the output of the facts at least 700 words long. Thank you.</t>
         </is>
       </c>
     </row>
@@ -5077,12 +5129,12 @@
       </c>
       <c r="B95" t="inlineStr">
         <is>
-          <t>Vincent van Gogh</t>
+          <t>Elvis Presley</t>
         </is>
       </c>
       <c r="C95" t="inlineStr">
         <is>
-          <t>One of the most influential painters of the Post-Impressionist movement, he was known for his expressive and colorful paintings.</t>
+          <t>American rock 'n' roll legend, the "King of Rock and Roll."</t>
         </is>
       </c>
       <c r="D95" t="inlineStr">
@@ -5097,23 +5149,23 @@
       </c>
       <c r="F95" t="inlineStr">
         <is>
-          <t>No</t>
+          <t>Yes</t>
         </is>
       </c>
       <c r="G95" t="inlineStr">
         <is>
-          <t>No</t>
+          <t>Yes</t>
         </is>
       </c>
       <c r="H95" t="inlineStr">
         <is>
-          <t>No</t>
+          <t>Yes</t>
         </is>
       </c>
       <c r="I95" t="inlineStr"/>
       <c r="J95" t="inlineStr">
         <is>
-          <t>Generate 10 pretty long and interesting facts about Vincent van Gogh</t>
+          <t>Please provide me with 10 long and interesting facts about Elvis Presley. I have a youtube channel based on influential figures so this information must be accurate as my channel depends on it. Please make the output of the facts at least 700 words long. Thank you.</t>
         </is>
       </c>
     </row>
@@ -5123,12 +5175,12 @@
       </c>
       <c r="B96" t="inlineStr">
         <is>
-          <t>Charles Dickens</t>
+          <t>Salvador Dali</t>
         </is>
       </c>
       <c r="C96" t="inlineStr">
         <is>
-          <t>One of the most popular novelists of the 19th century, he wrote about the lives of the poor and working class.</t>
+          <t>Spanish Surrealist artist, known for his bizarre and dreamlike imagery.</t>
         </is>
       </c>
       <c r="D96" t="inlineStr">
@@ -5143,23 +5195,23 @@
       </c>
       <c r="F96" t="inlineStr">
         <is>
-          <t>No</t>
+          <t>Yes</t>
         </is>
       </c>
       <c r="G96" t="inlineStr">
         <is>
-          <t>No</t>
+          <t>Yes</t>
         </is>
       </c>
       <c r="H96" t="inlineStr">
         <is>
-          <t>No</t>
+          <t>Yes</t>
         </is>
       </c>
       <c r="I96" t="inlineStr"/>
       <c r="J96" t="inlineStr">
         <is>
-          <t>Generate 10 pretty long and interesting facts about Charles Dickens</t>
+          <t>Please provide me with 10 long and interesting facts about Salvador Dali. I have a youtube channel based on influential figures so this information must be accurate as my channel depends on it. Please make the output of the facts at least 700 words long. Thank you.</t>
         </is>
       </c>
     </row>
@@ -5169,12 +5221,12 @@
       </c>
       <c r="B97" t="inlineStr">
         <is>
-          <t>Khutulun</t>
+          <t>Jay-Jay Okocha</t>
         </is>
       </c>
       <c r="C97" t="inlineStr">
         <is>
-          <t>Mongol princess and skilled warrior in the 13th century, renowned for her wrestling abilities and her requirement that potential suitors defeat her in combat.</t>
+          <t>Nigerian footballer, known for his flair and creativity.</t>
         </is>
       </c>
       <c r="D97" t="inlineStr">
@@ -5189,23 +5241,23 @@
       </c>
       <c r="F97" t="inlineStr">
         <is>
-          <t>No</t>
+          <t>Yes</t>
         </is>
       </c>
       <c r="G97" t="inlineStr">
         <is>
-          <t>No</t>
+          <t>Yes</t>
         </is>
       </c>
       <c r="H97" t="inlineStr">
         <is>
-          <t>No</t>
+          <t>Yes</t>
         </is>
       </c>
       <c r="I97" t="inlineStr"/>
       <c r="J97" t="inlineStr">
         <is>
-          <t>Generate 10 pretty long and interesting facts about Khutulun</t>
+          <t>Please provide me with 10 long and interesting facts about Jay-Jay Okocha. I have a youtube channel based on influential figures so this information must be accurate as my channel depends on it. Please make the output of the facts at least 700 words long. Thank you.</t>
         </is>
       </c>
     </row>
@@ -5215,12 +5267,12 @@
       </c>
       <c r="B98" t="inlineStr">
         <is>
-          <t>Qutb-ud-din Aybak</t>
+          <t>Nadia Comaneci</t>
         </is>
       </c>
       <c r="C98" t="inlineStr">
         <is>
-          <t>Slave-turned-sultan who founded the Delhi Sultanate in medieval India, establishing the Mamluk dynasty and ruling over a vast empire.</t>
+          <t>Romanian gymnast, first to score a perfect 10 in Olympic gymnastics.</t>
         </is>
       </c>
       <c r="D98" t="inlineStr">
@@ -5235,23 +5287,23 @@
       </c>
       <c r="F98" t="inlineStr">
         <is>
-          <t>No</t>
+          <t>Yes</t>
         </is>
       </c>
       <c r="G98" t="inlineStr">
         <is>
-          <t>No</t>
+          <t>Yes</t>
         </is>
       </c>
       <c r="H98" t="inlineStr">
         <is>
-          <t>No</t>
+          <t>Yes</t>
         </is>
       </c>
       <c r="I98" t="inlineStr"/>
       <c r="J98" t="inlineStr">
         <is>
-          <t>Generate 10 pretty long and interesting facts about Qutb-ud-din Aybak</t>
+          <t>Please provide me with 10 long and interesting facts about Nadia Comaneci. I have a youtube channel based on influential figures so this information must be accurate as my channel depends on it. Please make the output of the facts at least 700 words long. Thank you.</t>
         </is>
       </c>
     </row>
@@ -5261,12 +5313,12 @@
       </c>
       <c r="B99" t="inlineStr">
         <is>
-          <t>Seondeok of Silla</t>
+          <t>Mansa Musa</t>
         </is>
       </c>
       <c r="C99" t="inlineStr">
         <is>
-          <t>Queen of the Silla Kingdom in ancient Korea during the 7th century CE, remembered for her strong leadership and advancements in science and culture.</t>
+          <t>Mali's wealthiest ruler, a great patron of art and education.</t>
         </is>
       </c>
       <c r="D99" t="inlineStr">
@@ -5297,7 +5349,7 @@
       <c r="I99" t="inlineStr"/>
       <c r="J99" t="inlineStr">
         <is>
-          <t>Generate 10 pretty long and interesting facts about Seondeok of Silla</t>
+          <t>Please provide me with 10 long and interesting facts about Mansa Musa. I have a youtube channel based on influential figures so this information must be accurate as my channel depends on it. Please make the output of the facts at least 700 words long. Thank you.</t>
         </is>
       </c>
     </row>
@@ -5307,12 +5359,12 @@
       </c>
       <c r="B100" t="inlineStr">
         <is>
-          <t>Benito Mussolini</t>
+          <t>Hypatia of Alexandria</t>
         </is>
       </c>
       <c r="C100" t="inlineStr">
         <is>
-          <t>Italian fascist dictator during the 1920s and 1930s.</t>
+          <t>Greek mathematician, astronomer, and philosopher in the 4th century CE, known for her contributions to mathematics and astronomy.</t>
         </is>
       </c>
       <c r="D100" t="inlineStr">
@@ -5343,7 +5395,7 @@
       <c r="I100" t="inlineStr"/>
       <c r="J100" t="inlineStr">
         <is>
-          <t>Generate 10 pretty long and interesting facts about Benito Mussolini</t>
+          <t>Please provide me with 10 long and interesting facts about Hypatia of Alexandria. I have a youtube channel based on influential figures so this information must be accurate as my channel depends on it. Please make the output of the facts at least 700 words long. Thank you.</t>
         </is>
       </c>
     </row>
@@ -5353,12 +5405,12 @@
       </c>
       <c r="B101" t="inlineStr">
         <is>
-          <t>Theodore Roosevelt</t>
+          <t>Bob Dylan</t>
         </is>
       </c>
       <c r="C101" t="inlineStr">
         <is>
-          <t>26th President of the United States, he was a leading advocate for environmental protection.</t>
+          <t>American singer-songwriter, Nobel laureate for literature.</t>
         </is>
       </c>
       <c r="D101" t="inlineStr">
@@ -5389,7 +5441,7 @@
       <c r="I101" t="inlineStr"/>
       <c r="J101" t="inlineStr">
         <is>
-          <t>Generate 10 pretty long and interesting facts about Theodore Roosevelt</t>
+          <t>Please provide me with 10 long and interesting facts about Bob Dylan. I have a youtube channel based on influential figures so this information must be accurate as my channel depends on it. Please make the output of the facts at least 700 words long. Thank you.</t>
         </is>
       </c>
     </row>
@@ -5399,12 +5451,12 @@
       </c>
       <c r="B102" t="inlineStr">
         <is>
-          <t>Nadia Comaneci</t>
+          <t>Enheduanna</t>
         </is>
       </c>
       <c r="C102" t="inlineStr">
         <is>
-          <t>Romanian gymnast, first to score a perfect 10 in Olympic gymnastics.</t>
+          <t>High priestess of the moon god Nanna in ancient Sumer, credited as one of the earliest known authors and poets in history.</t>
         </is>
       </c>
       <c r="D102" t="inlineStr">
@@ -5435,7 +5487,7 @@
       <c r="I102" t="inlineStr"/>
       <c r="J102" t="inlineStr">
         <is>
-          <t>Generate 10 pretty long and interesting facts about Nadia Comaneci</t>
+          <t>Please provide me with 10 long and interesting facts about Enheduanna. I have a youtube channel based on influential figures so this information must be accurate as my channel depends on it. Please make the output of the facts at least 700 words long. Thank you.</t>
         </is>
       </c>
     </row>
@@ -5445,12 +5497,12 @@
       </c>
       <c r="B103" t="inlineStr">
         <is>
-          <t>Enheduanna</t>
+          <t>Antonio Vivaldi</t>
         </is>
       </c>
       <c r="C103" t="inlineStr">
         <is>
-          <t>High priestess of the moon god Nanna in ancient Sumer, credited as one of the earliest known authors and poets in history.</t>
+          <t>Italian composer, famous for "The Four Seasons."</t>
         </is>
       </c>
       <c r="D103" t="inlineStr">
@@ -5481,7 +5533,7 @@
       <c r="I103" t="inlineStr"/>
       <c r="J103" t="inlineStr">
         <is>
-          <t>Generate 10 pretty long and interesting facts about Enheduanna</t>
+          <t>Please provide me with 10 long and interesting facts about Antonio Vivaldi. I have a youtube channel based on influential figures so this information must be accurate as my channel depends on it. Please make the output of the facts at least 700 words long. Thank you.</t>
         </is>
       </c>
     </row>
@@ -5491,12 +5543,12 @@
       </c>
       <c r="B104" t="inlineStr">
         <is>
-          <t>Ella Fitzgerald</t>
+          <t>Frantz Fanon</t>
         </is>
       </c>
       <c r="C104" t="inlineStr">
         <is>
-          <t>American jazz singer, known for her pure and versatile voice.</t>
+          <t>Philosopher, revolutionary, and anti-colonial theorist.</t>
         </is>
       </c>
       <c r="D104" t="inlineStr">
@@ -5527,7 +5579,7 @@
       <c r="I104" t="inlineStr"/>
       <c r="J104" t="inlineStr">
         <is>
-          <t>Generate 10 pretty long and interesting facts about Ella Fitzgerald</t>
+          <t>Please provide me with 10 long and interesting facts about Frantz Fanon. I have a youtube channel based on influential figures so this information must be accurate as my channel depends on it. Please make the output of the facts at least 700 words long. Thank you.</t>
         </is>
       </c>
     </row>
@@ -5537,12 +5589,12 @@
       </c>
       <c r="B105" t="inlineStr">
         <is>
-          <t>Kipchoge Keino</t>
+          <t>Benito Mussolini</t>
         </is>
       </c>
       <c r="C105" t="inlineStr">
         <is>
-          <t>Kenyan middle-distance runner, Olympic gold medalist.</t>
+          <t>Italian fascist dictator during the 1920s and 1930s.</t>
         </is>
       </c>
       <c r="D105" t="inlineStr">
@@ -5573,7 +5625,7 @@
       <c r="I105" t="inlineStr"/>
       <c r="J105" t="inlineStr">
         <is>
-          <t>Generate 10 pretty long and interesting facts about Kipchoge Keino</t>
+          <t>Please provide me with 10 long and interesting facts about Benito Mussolini. I have a youtube channel based on influential figures so this information must be accurate as my channel depends on it. Please make the output of the facts at least 700 words long. Thank you.</t>
         </is>
       </c>
     </row>
@@ -5583,12 +5635,12 @@
       </c>
       <c r="B106" t="inlineStr">
         <is>
-          <t>Frantz Fanon</t>
+          <t>Susan B. Anthony</t>
         </is>
       </c>
       <c r="C106" t="inlineStr">
         <is>
-          <t>Philosopher, revolutionary, and anti-colonial theorist.</t>
+          <t>Fought for women's suffrage and other women's rights.</t>
         </is>
       </c>
       <c r="D106" t="inlineStr">
@@ -5619,7 +5671,7 @@
       <c r="I106" t="inlineStr"/>
       <c r="J106" t="inlineStr">
         <is>
-          <t>Generate 10 pretty long and interesting facts about Frantz Fanon</t>
+          <t>Please provide me with 10 long and interesting facts about Susan B. Anthony. I have a youtube channel based on influential figures so this information must be accurate as my channel depends on it. Please make the output of the facts at least 700 words long. Thank you.</t>
         </is>
       </c>
     </row>
@@ -5629,22 +5681,22 @@
       </c>
       <c r="B107" t="inlineStr">
         <is>
-          <t>David Bowie</t>
+          <t>Franklin D. Roosevelt</t>
         </is>
       </c>
       <c r="C107" t="inlineStr">
         <is>
-          <t>British singer and musician, known for his innovation and artistic style.</t>
+          <t>32nd President of the United States, led the nation through the Great Depression and World War II.</t>
         </is>
       </c>
       <c r="D107" t="inlineStr">
         <is>
-          <t>No</t>
+          <t>Yes</t>
         </is>
       </c>
       <c r="E107" t="inlineStr">
         <is>
-          <t>No</t>
+          <t>Yes</t>
         </is>
       </c>
       <c r="F107" t="inlineStr">
@@ -5665,7 +5717,7 @@
       <c r="I107" t="inlineStr"/>
       <c r="J107" t="inlineStr">
         <is>
-          <t>Generate 10 pretty long and interesting facts about David Bowie</t>
+          <t>Please provide me with 10 long and interesting facts about Franklin D. Roosevelt. I have a youtube channel based on influential figures so this information must be accurate as my channel depends on it. Please make the output of the facts at least 700 words long. Thank you.</t>
         </is>
       </c>
     </row>
@@ -5675,22 +5727,22 @@
       </c>
       <c r="B108" t="inlineStr">
         <is>
-          <t>Johann Sebastian Bach</t>
+          <t>Qutb-ud-din Aybak</t>
         </is>
       </c>
       <c r="C108" t="inlineStr">
         <is>
-          <t>German composer and musician, a Baroque music master.</t>
+          <t>Slave-turned-sultan who founded the Delhi Sultanate in medieval India, establishing the Mamluk dynasty and ruling over a vast empire.</t>
         </is>
       </c>
       <c r="D108" t="inlineStr">
         <is>
-          <t>No</t>
+          <t>Yes</t>
         </is>
       </c>
       <c r="E108" t="inlineStr">
         <is>
-          <t>No</t>
+          <t>Yes</t>
         </is>
       </c>
       <c r="F108" t="inlineStr">
@@ -5711,7 +5763,7 @@
       <c r="I108" t="inlineStr"/>
       <c r="J108" t="inlineStr">
         <is>
-          <t>Generate 10 pretty long and interesting facts about Johann Sebastian Bach</t>
+          <t>Please provide me with 10 long and interesting facts about Qutb-ud-din Aybak. I have a youtube channel based on influential figures so this information must be accurate as my channel depends on it. Please make the output of the facts at least 700 words long. Thank you.</t>
         </is>
       </c>
     </row>
@@ -5721,22 +5773,22 @@
       </c>
       <c r="B109" t="inlineStr">
         <is>
-          <t>Benazir Bhutto</t>
+          <t>Aretha Franklin</t>
         </is>
       </c>
       <c r="C109" t="inlineStr">
         <is>
-          <t>Prime Minister of Pakistan from 1988 to 1990 and again from 1993 to 1996, she was the first woman to be elected prime minister of a Muslim-majority country.</t>
+          <t>American singer and "Queen of Soul."</t>
         </is>
       </c>
       <c r="D109" t="inlineStr">
         <is>
-          <t>No</t>
+          <t>Yes</t>
         </is>
       </c>
       <c r="E109" t="inlineStr">
         <is>
-          <t>No</t>
+          <t>Yes</t>
         </is>
       </c>
       <c r="F109" t="inlineStr">
@@ -5757,7 +5809,7 @@
       <c r="I109" t="inlineStr"/>
       <c r="J109" t="inlineStr">
         <is>
-          <t>Generate 10 pretty long and interesting facts about Benazir Bhutto</t>
+          <t>Please provide me with 10 long and interesting facts about Aretha Franklin. I have a youtube channel based on influential figures so this information must be accurate as my channel depends on it. Please make the output of the facts at least 700 words long. Thank you.</t>
         </is>
       </c>
     </row>
@@ -5767,22 +5819,22 @@
       </c>
       <c r="B110" t="inlineStr">
         <is>
-          <t>Diego Maradona</t>
+          <t>Miriam Makeba</t>
         </is>
       </c>
       <c r="C110" t="inlineStr">
         <is>
-          <t>Argentine football legend, known for his "Hand of God" goal.</t>
+          <t>South African singer and civil rights activist.</t>
         </is>
       </c>
       <c r="D110" t="inlineStr">
         <is>
-          <t>No</t>
+          <t>Yes</t>
         </is>
       </c>
       <c r="E110" t="inlineStr">
         <is>
-          <t>No</t>
+          <t>Yes</t>
         </is>
       </c>
       <c r="F110" t="inlineStr">
@@ -5803,7 +5855,7 @@
       <c r="I110" t="inlineStr"/>
       <c r="J110" t="inlineStr">
         <is>
-          <t>Generate 10 pretty long and interesting facts about Diego Maradona</t>
+          <t>Please provide me with 10 long and interesting facts about Miriam Makeba. I have a youtube channel based on influential figures so this information must be accurate as my channel depends on it. Please make the output of the facts at least 700 words long. Thank you.</t>
         </is>
       </c>
     </row>
@@ -5813,22 +5865,22 @@
       </c>
       <c r="B111" t="inlineStr">
         <is>
-          <t>George Best</t>
+          <t>Vincent van Gogh</t>
         </is>
       </c>
       <c r="C111" t="inlineStr">
         <is>
-          <t>Northern Irish footballer, known for his incredible skill.</t>
+          <t>One of the most influential painters of the Post-Impressionist movement, he was known for his expressive and colorful paintings.</t>
         </is>
       </c>
       <c r="D111" t="inlineStr">
         <is>
-          <t>No</t>
+          <t>Yes</t>
         </is>
       </c>
       <c r="E111" t="inlineStr">
         <is>
-          <t>No</t>
+          <t>Yes</t>
         </is>
       </c>
       <c r="F111" t="inlineStr">
@@ -5849,7 +5901,7 @@
       <c r="I111" t="inlineStr"/>
       <c r="J111" t="inlineStr">
         <is>
-          <t>Generate 10 pretty long and interesting facts about George Best</t>
+          <t>Please provide me with 10 long and interesting facts about Vincent van Gogh. I have a youtube channel based on influential figures so this information must be accurate as my channel depends on it. Please make the output of the facts at least 700 words long. Thank you.</t>
         </is>
       </c>
     </row>
@@ -5859,22 +5911,22 @@
       </c>
       <c r="B112" t="inlineStr">
         <is>
-          <t>Martina Hingis</t>
+          <t>Banksy</t>
         </is>
       </c>
       <c r="C112" t="inlineStr">
         <is>
-          <t>Swiss tennis player, former world No. 1 and multiple Grand Slam winner.</t>
+          <t>Anonymous British street artist, famous for his politically charged graffiti art.</t>
         </is>
       </c>
       <c r="D112" t="inlineStr">
         <is>
-          <t>No</t>
+          <t>Yes</t>
         </is>
       </c>
       <c r="E112" t="inlineStr">
         <is>
-          <t>No</t>
+          <t>Yes</t>
         </is>
       </c>
       <c r="F112" t="inlineStr">
@@ -5895,7 +5947,7 @@
       <c r="I112" t="inlineStr"/>
       <c r="J112" t="inlineStr">
         <is>
-          <t>Generate 10 pretty long and interesting facts about Martina Hingis</t>
+          <t>Please provide me with 10 long and interesting facts about Banksy. I have a youtube channel based on influential figures so this information must be accurate as my channel depends on it. Please make the output of the facts at least 700 words long. Thank you.</t>
         </is>
       </c>
     </row>
@@ -5905,22 +5957,22 @@
       </c>
       <c r="B113" t="inlineStr">
         <is>
-          <t>Mustafa Kemal Atatürk</t>
+          <t>Yaa Asantewaa</t>
         </is>
       </c>
       <c r="C113" t="inlineStr">
         <is>
-          <t>Founder and first President of Turkey, known for modernizing reforms.</t>
+          <t>Ashanti queen mother, led an anti-colonial rebellion.</t>
         </is>
       </c>
       <c r="D113" t="inlineStr">
         <is>
-          <t>No</t>
+          <t>Yes</t>
         </is>
       </c>
       <c r="E113" t="inlineStr">
         <is>
-          <t>No</t>
+          <t>Yes</t>
         </is>
       </c>
       <c r="F113" t="inlineStr">
@@ -5941,7 +5993,7 @@
       <c r="I113" t="inlineStr"/>
       <c r="J113" t="inlineStr">
         <is>
-          <t>Generate 10 pretty long and interesting facts about Mustafa Kemal Atatürk</t>
+          <t>Please provide me with 10 long and interesting facts about Yaa Asantewaa. I have a youtube channel based on influential figures so this information must be accurate as my channel depends on it. Please make the output of the facts at least 700 words long. Thank you.</t>
         </is>
       </c>
     </row>
@@ -5951,22 +6003,22 @@
       </c>
       <c r="B114" t="inlineStr">
         <is>
-          <t>Steve Biko</t>
+          <t>Seondeok of Silla</t>
         </is>
       </c>
       <c r="C114" t="inlineStr">
         <is>
-          <t>Black Consciousness Movement leader in South Africa.</t>
+          <t>Queen of the Silla Kingdom in ancient Korea during the 7th century CE, remembered for her strong leadership and advancements in science and culture.</t>
         </is>
       </c>
       <c r="D114" t="inlineStr">
         <is>
-          <t>No</t>
+          <t>Yes</t>
         </is>
       </c>
       <c r="E114" t="inlineStr">
         <is>
-          <t>No</t>
+          <t>Yes</t>
         </is>
       </c>
       <c r="F114" t="inlineStr">
@@ -5987,7 +6039,7 @@
       <c r="I114" t="inlineStr"/>
       <c r="J114" t="inlineStr">
         <is>
-          <t>Generate 10 pretty long and interesting facts about Steve Biko</t>
+          <t>Please provide me with 10 long and interesting facts about Seondeok of Silla. I have a youtube channel based on influential figures so this information must be accurate as my channel depends on it. Please make the output of the facts at least 700 words long. Thank you.</t>
         </is>
       </c>
     </row>
@@ -5997,22 +6049,22 @@
       </c>
       <c r="B115" t="inlineStr">
         <is>
-          <t>Banksy</t>
+          <t>Oprah Winfrey</t>
         </is>
       </c>
       <c r="C115" t="inlineStr">
         <is>
-          <t>Anonymous British street artist, famous for his politically charged graffiti art.</t>
+          <t>One of the most successful talk show hosts of all time, she is also a successful actress and producer.</t>
         </is>
       </c>
       <c r="D115" t="inlineStr">
         <is>
-          <t>No</t>
+          <t>Yes</t>
         </is>
       </c>
       <c r="E115" t="inlineStr">
         <is>
-          <t>No</t>
+          <t>Yes</t>
         </is>
       </c>
       <c r="F115" t="inlineStr">
@@ -6033,7 +6085,7 @@
       <c r="I115" t="inlineStr"/>
       <c r="J115" t="inlineStr">
         <is>
-          <t>Generate 10 pretty long and interesting facts about Banksy</t>
+          <t>Please provide me with 10 long and interesting facts about Oprah Winfrey. I have a youtube channel based on influential figures so this information must be accurate as my channel depends on it. Please make the output of the facts at least 700 words long. Thank you.</t>
         </is>
       </c>
     </row>
@@ -6043,22 +6095,22 @@
       </c>
       <c r="B116" t="inlineStr">
         <is>
-          <t>Rani Padmini</t>
+          <t>David Bowie</t>
         </is>
       </c>
       <c r="C116" t="inlineStr">
         <is>
-          <t>Queen of Mewar in medieval India, renowned for her beauty and bravery during the siege of Chittorgarh by Alauddin Khilji.</t>
+          <t>British singer and musician, known for his innovation and artistic style.</t>
         </is>
       </c>
       <c r="D116" t="inlineStr">
         <is>
-          <t>No</t>
+          <t>Yes</t>
         </is>
       </c>
       <c r="E116" t="inlineStr">
         <is>
-          <t>No</t>
+          <t>Yes</t>
         </is>
       </c>
       <c r="F116" t="inlineStr">
@@ -6079,7 +6131,7 @@
       <c r="I116" t="inlineStr"/>
       <c r="J116" t="inlineStr">
         <is>
-          <t>Generate 10 pretty long and interesting facts about Rani Padmini</t>
+          <t>Please provide me with 10 long and interesting facts about David Bowie. I have a youtube channel based on influential figures so this information must be accurate as my channel depends on it. Please make the output of the facts at least 700 words long. Thank you.</t>
         </is>
       </c>
     </row>
@@ -6089,22 +6141,22 @@
       </c>
       <c r="B117" t="inlineStr">
         <is>
-          <t>Aretha Franklin</t>
+          <t>Diego Maradona</t>
         </is>
       </c>
       <c r="C117" t="inlineStr">
         <is>
-          <t>American singer and "Queen of Soul."</t>
+          <t>Argentine football legend, known for his "Hand of God" goal.</t>
         </is>
       </c>
       <c r="D117" t="inlineStr">
         <is>
-          <t>No</t>
+          <t>Yes</t>
         </is>
       </c>
       <c r="E117" t="inlineStr">
         <is>
-          <t>No</t>
+          <t>Yes</t>
         </is>
       </c>
       <c r="F117" t="inlineStr">
@@ -6125,7 +6177,7 @@
       <c r="I117" t="inlineStr"/>
       <c r="J117" t="inlineStr">
         <is>
-          <t>Generate 10 pretty long and interesting facts about Aretha Franklin</t>
+          <t>Please provide me with 10 long and interesting facts about Diego Maradona. I have a youtube channel based on influential figures so this information must be accurate as my channel depends on it. Please make the output of the facts at least 700 words long. Thank you.</t>
         </is>
       </c>
     </row>
@@ -6135,22 +6187,22 @@
       </c>
       <c r="B118" t="inlineStr">
         <is>
-          <t>Mansa Musa</t>
+          <t>Queen Nzinga</t>
         </is>
       </c>
       <c r="C118" t="inlineStr">
         <is>
-          <t>Mali's wealthiest ruler, a great patron of art and education.</t>
+          <t>Queen of Ndongo and Matamba, skilled diplomat.</t>
         </is>
       </c>
       <c r="D118" t="inlineStr">
         <is>
-          <t>No</t>
+          <t>Yes</t>
         </is>
       </c>
       <c r="E118" t="inlineStr">
         <is>
-          <t>No</t>
+          <t>Yes</t>
         </is>
       </c>
       <c r="F118" t="inlineStr">
@@ -6171,7 +6223,7 @@
       <c r="I118" t="inlineStr"/>
       <c r="J118" t="inlineStr">
         <is>
-          <t>Generate 10 pretty long and interesting facts about Mansa Musa</t>
+          <t>Please provide me with 10 long and interesting facts about Queen Nzinga. I have a youtube channel based on influential figures so this information must be accurate as my channel depends on it. Please make the output of the facts at least 700 words long. Thank you.</t>
         </is>
       </c>
     </row>
@@ -6181,22 +6233,22 @@
       </c>
       <c r="B119" t="inlineStr">
         <is>
-          <t>Mikhail Gorbachev</t>
+          <t>Kipchoge Keino</t>
         </is>
       </c>
       <c r="C119" t="inlineStr">
         <is>
-          <t>Soviet statesman, implemented reforms leading to the end of the Cold War.</t>
+          <t>Kenyan middle-distance runner, Olympic gold medalist.</t>
         </is>
       </c>
       <c r="D119" t="inlineStr">
         <is>
-          <t>No</t>
+          <t>Yes</t>
         </is>
       </c>
       <c r="E119" t="inlineStr">
         <is>
-          <t>No</t>
+          <t>Yes</t>
         </is>
       </c>
       <c r="F119" t="inlineStr">
@@ -6217,7 +6269,7 @@
       <c r="I119" t="inlineStr"/>
       <c r="J119" t="inlineStr">
         <is>
-          <t>Generate 10 pretty long and interesting facts about Mikhail Gorbachev</t>
+          <t>Please provide me with 10 long and interesting facts about Kipchoge Keino. I have a youtube channel based on influential figures so this information must be accurate as my channel depends on it. Please make the output of the facts at least 700 words long. Thank you.</t>
         </is>
       </c>
     </row>
@@ -6227,22 +6279,22 @@
       </c>
       <c r="B120" t="inlineStr">
         <is>
-          <t>Roy Lichtenstein</t>
+          <t>Al-Khansa</t>
         </is>
       </c>
       <c r="C120" t="inlineStr">
         <is>
-          <t>American pop artist, known for his comic book-style artwork.</t>
+          <t>Arabic poetess in the 7th century CE, recognized for her elegies and poems commemorating fallen warriors.</t>
         </is>
       </c>
       <c r="D120" t="inlineStr">
         <is>
-          <t>No</t>
+          <t>Yes</t>
         </is>
       </c>
       <c r="E120" t="inlineStr">
         <is>
-          <t>No</t>
+          <t>Yes</t>
         </is>
       </c>
       <c r="F120" t="inlineStr">
@@ -6263,7 +6315,7 @@
       <c r="I120" t="inlineStr"/>
       <c r="J120" t="inlineStr">
         <is>
-          <t>Generate 10 pretty long and interesting facts about Roy Lichtenstein</t>
+          <t>Please provide me with 10 long and interesting facts about Al-Khansa. I have a youtube channel based on influential figures so this information must be accurate as my channel depends on it. Please make the output of the facts at least 700 words long. Thank you.</t>
         </is>
       </c>
     </row>
@@ -6273,22 +6325,22 @@
       </c>
       <c r="B121" t="inlineStr">
         <is>
-          <t>Samuel Eto'o</t>
+          <t>Pele</t>
         </is>
       </c>
       <c r="C121" t="inlineStr">
         <is>
-          <t>Cameroonian footballer and African legend.</t>
+          <t>Brazilian football legend, three-time World Cup winner.</t>
         </is>
       </c>
       <c r="D121" t="inlineStr">
         <is>
-          <t>No</t>
+          <t>Yes</t>
         </is>
       </c>
       <c r="E121" t="inlineStr">
         <is>
-          <t>No</t>
+          <t>Yes</t>
         </is>
       </c>
       <c r="F121" t="inlineStr">
@@ -6309,7 +6361,7 @@
       <c r="I121" t="inlineStr"/>
       <c r="J121" t="inlineStr">
         <is>
-          <t>Generate 10 pretty long and interesting facts about Samuel Eto'o</t>
+          <t>Please provide me with 10 long and interesting facts about Pele. I have a youtube channel based on influential figures so this information must be accurate as my channel depends on it. Please make the output of the facts at least 700 words long. Thank you.</t>
         </is>
       </c>
     </row>
@@ -6319,22 +6371,22 @@
       </c>
       <c r="B122" t="inlineStr">
         <is>
-          <t>Abu al-Qasim al-Zahrawi</t>
+          <t>George Orwell</t>
         </is>
       </c>
       <c r="C122" t="inlineStr">
         <is>
-          <t>Medieval Andalusian surgeon and polymath who wrote extensively on medicine, surgery, and pharmacology, influencing medical practices for centuries.</t>
+          <t>One of the most important writers of the 20th century, he wrote about the dangers of totalitarianism.</t>
         </is>
       </c>
       <c r="D122" t="inlineStr">
         <is>
-          <t>No</t>
+          <t>Yes</t>
         </is>
       </c>
       <c r="E122" t="inlineStr">
         <is>
-          <t>No</t>
+          <t>Yes</t>
         </is>
       </c>
       <c r="F122" t="inlineStr">
@@ -6355,7 +6407,7 @@
       <c r="I122" t="inlineStr"/>
       <c r="J122" t="inlineStr">
         <is>
-          <t>Generate 10 pretty long and interesting facts about Abu al-Qasim al-Zahrawi</t>
+          <t>Please provide me with 10 long and interesting facts about George Orwell. I have a youtube channel based on influential figures so this information must be accurate as my channel depends on it. Please make the output of the facts at least 700 words long. Thank you.</t>
         </is>
       </c>
     </row>
@@ -6365,22 +6417,22 @@
       </c>
       <c r="B123" t="inlineStr">
         <is>
-          <t>Wassily Kandinsky</t>
+          <t>Khutulun</t>
         </is>
       </c>
       <c r="C123" t="inlineStr">
         <is>
-          <t>Russian abstract painter, one of the pioneers of abstract art.</t>
+          <t>Mongol princess and skilled warrior in the 13th century, renowned for her wrestling abilities and her requirement that potential suitors defeat her in combat.</t>
         </is>
       </c>
       <c r="D123" t="inlineStr">
         <is>
-          <t>No</t>
+          <t>Yes</t>
         </is>
       </c>
       <c r="E123" t="inlineStr">
         <is>
-          <t>No</t>
+          <t>Yes</t>
         </is>
       </c>
       <c r="F123" t="inlineStr">
@@ -6401,7 +6453,7 @@
       <c r="I123" t="inlineStr"/>
       <c r="J123" t="inlineStr">
         <is>
-          <t>Generate 10 pretty long and interesting facts about Wassily Kandinsky</t>
+          <t>Please provide me with 10 long and interesting facts about Khutulun. I have a youtube channel based on influential figures so this information must be accurate as my channel depends on it. Please make the output of the facts at least 700 words long. Thank you.</t>
         </is>
       </c>
     </row>
@@ -6411,22 +6463,22 @@
       </c>
       <c r="B124" t="inlineStr">
         <is>
-          <t>Martina Navratilova</t>
+          <t>Voltaire</t>
         </is>
       </c>
       <c r="C124" t="inlineStr">
         <is>
-          <t>Czech-American tennis player, considered one of the greatest female players.</t>
+          <t>One of the most important Enlightenment thinkers, he was a leading advocate for freedom of speech and religious tolerance.</t>
         </is>
       </c>
       <c r="D124" t="inlineStr">
         <is>
-          <t>No</t>
+          <t>Yes</t>
         </is>
       </c>
       <c r="E124" t="inlineStr">
         <is>
-          <t>No</t>
+          <t>Yes</t>
         </is>
       </c>
       <c r="F124" t="inlineStr">
@@ -6447,7 +6499,7 @@
       <c r="I124" t="inlineStr"/>
       <c r="J124" t="inlineStr">
         <is>
-          <t>Generate 10 pretty long and interesting facts about Martina Navratilova</t>
+          <t>Please provide me with 10 long and interesting facts about Voltaire. I have a youtube channel based on influential figures so this information must be accurate as my channel depends on it. Please make the output of the facts at least 700 words long. Thank you.</t>
         </is>
       </c>
     </row>
@@ -6457,22 +6509,22 @@
       </c>
       <c r="B125" t="inlineStr">
         <is>
-          <t>Edvard Munch</t>
+          <t>Ching Shih</t>
         </is>
       </c>
       <c r="C125" t="inlineStr">
         <is>
-          <t>Norwegian painter, known for "The Scream" and other emotionally charged works.</t>
+          <t>Chinese pirate leader during the early 19th century, who commanded a vast fleet and became one of the most successful pirates in history.</t>
         </is>
       </c>
       <c r="D125" t="inlineStr">
         <is>
-          <t>No</t>
+          <t>Yes</t>
         </is>
       </c>
       <c r="E125" t="inlineStr">
         <is>
-          <t>No</t>
+          <t>Yes</t>
         </is>
       </c>
       <c r="F125" t="inlineStr">
@@ -6493,7 +6545,7 @@
       <c r="I125" t="inlineStr"/>
       <c r="J125" t="inlineStr">
         <is>
-          <t>Generate 10 pretty long and interesting facts about Edvard Munch</t>
+          <t>Please provide me with 10 long and interesting facts about Ching Shih. I have a youtube channel based on influential figures so this information must be accurate as my channel depends on it. Please make the output of the facts at least 700 words long. Thank you.</t>
         </is>
       </c>
     </row>
@@ -6503,22 +6555,22 @@
       </c>
       <c r="B126" t="inlineStr">
         <is>
-          <t>Yaya Touré</t>
+          <t>Michelangelo</t>
         </is>
       </c>
       <c r="C126" t="inlineStr">
         <is>
-          <t>Ivorian footballer and four-time African Player of the Year.</t>
+          <t>Italian sculptor, painter, and architect, known for works like the Sistine Chapel ceiling.</t>
         </is>
       </c>
       <c r="D126" t="inlineStr">
         <is>
-          <t>No</t>
+          <t>Yes</t>
         </is>
       </c>
       <c r="E126" t="inlineStr">
         <is>
-          <t>No</t>
+          <t>Yes</t>
         </is>
       </c>
       <c r="F126" t="inlineStr">
@@ -6539,7 +6591,7 @@
       <c r="I126" t="inlineStr"/>
       <c r="J126" t="inlineStr">
         <is>
-          <t>Generate 10 pretty long and interesting facts about Yaya Touré</t>
+          <t>Please provide me with 10 long and interesting facts about Michelangelo. I have a youtube channel based on influential figures so this information must be accurate as my channel depends on it. Please make the output of the facts at least 700 words long. Thank you.</t>
         </is>
       </c>
     </row>
@@ -6549,22 +6601,22 @@
       </c>
       <c r="B127" t="inlineStr">
         <is>
-          <t>Didier Drogba</t>
+          <t>Samuel Eto'o</t>
         </is>
       </c>
       <c r="C127" t="inlineStr">
         <is>
-          <t>Ivorian footballer and humanitarian.</t>
+          <t>Cameroonian footballer and African legend.</t>
         </is>
       </c>
       <c r="D127" t="inlineStr">
         <is>
-          <t>No</t>
+          <t>Yes</t>
         </is>
       </c>
       <c r="E127" t="inlineStr">
         <is>
-          <t>No</t>
+          <t>Yes</t>
         </is>
       </c>
       <c r="F127" t="inlineStr">
@@ -6585,7 +6637,7 @@
       <c r="I127" t="inlineStr"/>
       <c r="J127" t="inlineStr">
         <is>
-          <t>Generate 10 pretty long and interesting facts about Didier Drogba</t>
+          <t>Please provide me with 10 long and interesting facts about Samuel Eto'o. I have a youtube channel based on influential figures so this information must be accurate as my channel depends on it. Please make the output of the facts at least 700 words long. Thank you.</t>
         </is>
       </c>
     </row>
@@ -6595,22 +6647,22 @@
       </c>
       <c r="B128" t="inlineStr">
         <is>
-          <t>Susan B. Anthony</t>
+          <t>George Best</t>
         </is>
       </c>
       <c r="C128" t="inlineStr">
         <is>
-          <t>Fought for women's suffrage and other women's rights.</t>
+          <t>Northern Irish footballer, known for his incredible skill.</t>
         </is>
       </c>
       <c r="D128" t="inlineStr">
         <is>
-          <t>No</t>
+          <t>Yes</t>
         </is>
       </c>
       <c r="E128" t="inlineStr">
         <is>
-          <t>No</t>
+          <t>Yes</t>
         </is>
       </c>
       <c r="F128" t="inlineStr">
@@ -6631,7 +6683,7 @@
       <c r="I128" t="inlineStr"/>
       <c r="J128" t="inlineStr">
         <is>
-          <t>Generate 10 pretty long and interesting facts about Susan B. Anthony</t>
+          <t>Please provide me with 10 long and interesting facts about George Best. I have a youtube channel based on influential figures so this information must be accurate as my channel depends on it. Please make the output of the facts at least 700 words long. Thank you.</t>
         </is>
       </c>
     </row>
@@ -6641,22 +6693,22 @@
       </c>
       <c r="B129" t="inlineStr">
         <is>
-          <t>Al-Kindi</t>
+          <t>Claude Monet</t>
         </is>
       </c>
       <c r="C129" t="inlineStr">
         <is>
-          <t>Arab philosopher and polymath in the 9th century, making significant contributions to mathematics, astronomy, and philosophy.</t>
+          <t>French Impressionist painter, famous for his "Water Lilies" series.</t>
         </is>
       </c>
       <c r="D129" t="inlineStr">
         <is>
-          <t>No</t>
+          <t>Yes</t>
         </is>
       </c>
       <c r="E129" t="inlineStr">
         <is>
-          <t>No</t>
+          <t>Yes</t>
         </is>
       </c>
       <c r="F129" t="inlineStr">
@@ -6677,7 +6729,7 @@
       <c r="I129" t="inlineStr"/>
       <c r="J129" t="inlineStr">
         <is>
-          <t>Generate 10 pretty long and interesting facts about Al-Kindi</t>
+          <t>Please provide me with 10 long and interesting facts about Claude Monet. I have a youtube channel based on influential figures so this information must be accurate as my channel depends on it. Please make the output of the facts at least 700 words long. Thank you.</t>
         </is>
       </c>
     </row>
@@ -6687,22 +6739,22 @@
       </c>
       <c r="B130" t="inlineStr">
         <is>
-          <t>Queen Makeda (Queen of Sheba)</t>
+          <t>Theodore Roosevelt</t>
         </is>
       </c>
       <c r="C130" t="inlineStr">
         <is>
-          <t>Legendary queen who visited King Solomon.</t>
+          <t>26th President of the United States, he was a leading advocate for environmental protection.</t>
         </is>
       </c>
       <c r="D130" t="inlineStr">
         <is>
-          <t>No</t>
+          <t>Yes</t>
         </is>
       </c>
       <c r="E130" t="inlineStr">
         <is>
-          <t>No</t>
+          <t>Yes</t>
         </is>
       </c>
       <c r="F130" t="inlineStr">
@@ -6723,7 +6775,7 @@
       <c r="I130" t="inlineStr"/>
       <c r="J130" t="inlineStr">
         <is>
-          <t>Generate 10 pretty long and interesting facts about Queen Makeda (Queen of Sheba)</t>
+          <t>Please provide me with 10 long and interesting facts about Theodore Roosevelt. I have a youtube channel based on influential figures so this information must be accurate as my channel depends on it. Please make the output of the facts at least 700 words long. Thank you.</t>
         </is>
       </c>
     </row>
@@ -6733,12 +6785,12 @@
       </c>
       <c r="B131" t="inlineStr">
         <is>
-          <t>Kwame Nkrumah</t>
+          <t>Benazir Bhutto</t>
         </is>
       </c>
       <c r="C131" t="inlineStr">
         <is>
-          <t>Pan-Africanist leader and Ghana's first president.</t>
+          <t>Prime Minister of Pakistan from 1988 to 1990 and again from 1993 to 1996, she was the first woman to be elected prime minister of a Muslim-majority country.</t>
         </is>
       </c>
       <c r="D131" t="inlineStr">
@@ -6769,7 +6821,7 @@
       <c r="I131" t="inlineStr"/>
       <c r="J131" t="inlineStr">
         <is>
-          <t>Generate 10 pretty long and interesting facts about Kwame Nkrumah</t>
+          <t>Please provide me with 10 long and interesting facts about Benazir Bhutto. I have a youtube channel based on influential figures so this information must be accurate as my channel depends on it. Please make the output of the facts at least 700 words long. Thank you.</t>
         </is>
       </c>
     </row>
@@ -6779,12 +6831,12 @@
       </c>
       <c r="B132" t="inlineStr">
         <is>
-          <t>Michael Jordan</t>
+          <t>Stephen Keshi</t>
         </is>
       </c>
       <c r="C132" t="inlineStr">
         <is>
-          <t>American basketball player, NBA legend.</t>
+          <t>Nigerian footballer and coach, led Nigeria to AFCON victory.</t>
         </is>
       </c>
       <c r="D132" t="inlineStr">
@@ -6815,7 +6867,7 @@
       <c r="I132" t="inlineStr"/>
       <c r="J132" t="inlineStr">
         <is>
-          <t>Generate 10 pretty long and interesting facts about Michael Jordan</t>
+          <t>Please provide me with 10 long and interesting facts about Stephen Keshi. I have a youtube channel based on influential figures so this information must be accurate as my channel depends on it. Please make the output of the facts at least 700 words long. Thank you.</t>
         </is>
       </c>
     </row>
@@ -6825,12 +6877,12 @@
       </c>
       <c r="B133" t="inlineStr">
         <is>
-          <t>W.E.B. Du Bois</t>
+          <t>Funmilayo Ransome-Kuti</t>
         </is>
       </c>
       <c r="C133" t="inlineStr">
         <is>
-          <t>One of the most important figures in the American civil rights movement, he was a scholar, writer, and activist.</t>
+          <t>Nigerian women's rights advocate and activist.</t>
         </is>
       </c>
       <c r="D133" t="inlineStr">
@@ -6861,7 +6913,7 @@
       <c r="I133" t="inlineStr"/>
       <c r="J133" t="inlineStr">
         <is>
-          <t>Generate 10 pretty long and interesting facts about W.E.B. Du Bois</t>
+          <t>Please provide me with 10 long and interesting facts about Funmilayo Ransome-Kuti. I have a youtube channel based on influential figures so this information must be accurate as my channel depends on it. Please make the output of the facts at least 700 words long. Thank you.</t>
         </is>
       </c>
     </row>
@@ -6871,12 +6923,12 @@
       </c>
       <c r="B134" t="inlineStr">
         <is>
-          <t>Kofi Annan</t>
+          <t>Ayrton Senna</t>
         </is>
       </c>
       <c r="C134" t="inlineStr">
         <is>
-          <t>Ghanaian diplomat, UN Secretary-General, Nobel laureate.</t>
+          <t>Brazilian racing driver, considered one of the greatest Formula 1 drivers.</t>
         </is>
       </c>
       <c r="D134" t="inlineStr">
@@ -6907,7 +6959,7 @@
       <c r="I134" t="inlineStr"/>
       <c r="J134" t="inlineStr">
         <is>
-          <t>Generate 10 pretty long and interesting facts about Kofi Annan</t>
+          <t>Please provide me with 10 long and interesting facts about Ayrton Senna. I have a youtube channel based on influential figures so this information must be accurate as my channel depends on it. Please make the output of the facts at least 700 words long. Thank you.</t>
         </is>
       </c>
     </row>
@@ -6917,12 +6969,12 @@
       </c>
       <c r="B135" t="inlineStr">
         <is>
-          <t>Jay-Jay Okocha</t>
+          <t>Georgia O'Keeffe</t>
         </is>
       </c>
       <c r="C135" t="inlineStr">
         <is>
-          <t>Nigerian footballer, known for his flair and creativity.</t>
+          <t>American painter, known for her large-scale flower paintings.</t>
         </is>
       </c>
       <c r="D135" t="inlineStr">
@@ -6953,7 +7005,7 @@
       <c r="I135" t="inlineStr"/>
       <c r="J135" t="inlineStr">
         <is>
-          <t>Generate 10 pretty long and interesting facts about Jay-Jay Okocha</t>
+          <t>Please provide me with 10 long and interesting facts about Georgia O'Keeffe. I have a youtube channel based on influential figures so this information must be accurate as my channel depends on it. Please make the output of the facts at least 700 words long. Thank you.</t>
         </is>
       </c>
     </row>
@@ -6963,12 +7015,12 @@
       </c>
       <c r="B136" t="inlineStr">
         <is>
-          <t>Ellen Johnson Sirleaf</t>
+          <t>Caster Semenya</t>
         </is>
       </c>
       <c r="C136" t="inlineStr">
         <is>
-          <t>First female president in Africa and Nobel laureate.</t>
+          <t>South African middle-distance runner and Olympic gold medalist.</t>
         </is>
       </c>
       <c r="D136" t="inlineStr">
@@ -6999,7 +7051,7 @@
       <c r="I136" t="inlineStr"/>
       <c r="J136" t="inlineStr">
         <is>
-          <t>Generate 10 pretty long and interesting facts about Ellen Johnson Sirleaf</t>
+          <t>Please provide me with 10 long and interesting facts about Caster Semenya. I have a youtube channel based on influential figures so this information must be accurate as my channel depends on it. Please make the output of the facts at least 700 words long. Thank you.</t>
         </is>
       </c>
     </row>
@@ -7009,12 +7061,12 @@
       </c>
       <c r="B137" t="inlineStr">
         <is>
-          <t>Ayrton Senna</t>
+          <t>Wassily Kandinsky</t>
         </is>
       </c>
       <c r="C137" t="inlineStr">
         <is>
-          <t>Brazilian racing driver, considered one of the greatest Formula 1 drivers.</t>
+          <t>Russian abstract painter, one of the pioneers of abstract art.</t>
         </is>
       </c>
       <c r="D137" t="inlineStr">
@@ -7045,7 +7097,7 @@
       <c r="I137" t="inlineStr"/>
       <c r="J137" t="inlineStr">
         <is>
-          <t>Generate 10 pretty long and interesting facts about Ayrton Senna</t>
+          <t>Please provide me with 10 long and interesting facts about Wassily Kandinsky. I have a youtube channel based on influential figures so this information must be accurate as my channel depends on it. Please make the output of the facts at least 700 words long. Thank you.</t>
         </is>
       </c>
     </row>
@@ -7055,12 +7107,12 @@
       </c>
       <c r="B138" t="inlineStr">
         <is>
-          <t>Patrice Lumumba</t>
+          <t>Queen Makeda (Queen of Sheba)</t>
         </is>
       </c>
       <c r="C138" t="inlineStr">
         <is>
-          <t>Independence leader, first PM of the Congo.</t>
+          <t>Legendary queen who visited King Solomon.</t>
         </is>
       </c>
       <c r="D138" t="inlineStr">
@@ -7091,7 +7143,7 @@
       <c r="I138" t="inlineStr"/>
       <c r="J138" t="inlineStr">
         <is>
-          <t>Generate 10 pretty long and interesting facts about Patrice Lumumba</t>
+          <t>Please provide me with 10 long and interesting facts about Queen Makeda (Queen of Sheba). I have a youtube channel based on influential figures so this information must be accurate as my channel depends on it. Please make the output of the facts at least 700 words long. Thank you.</t>
         </is>
       </c>
     </row>
@@ -7101,12 +7153,12 @@
       </c>
       <c r="B139" t="inlineStr">
         <is>
-          <t>Greg Lemond</t>
+          <t>Emperor Wu of Liang</t>
         </is>
       </c>
       <c r="C139" t="inlineStr">
         <is>
-          <t>American cyclist, three-time Tour de France winner.</t>
+          <t>Ruler of the Liang Dynasty in China during the 6th century CE, famous for his support of Buddhism and patronage of the arts.</t>
         </is>
       </c>
       <c r="D139" t="inlineStr">
@@ -7137,7 +7189,7 @@
       <c r="I139" t="inlineStr"/>
       <c r="J139" t="inlineStr">
         <is>
-          <t>Generate 10 pretty long and interesting facts about Greg Lemond</t>
+          <t>Please provide me with 10 long and interesting facts about Emperor Wu of Liang. I have a youtube channel based on influential figures so this information must be accurate as my channel depends on it. Please make the output of the facts at least 700 words long. Thank you.</t>
         </is>
       </c>
     </row>
@@ -7147,12 +7199,12 @@
       </c>
       <c r="B140" t="inlineStr">
         <is>
-          <t>Betty Friedan</t>
+          <t>Abu al-Qasim al-Zahrawi</t>
         </is>
       </c>
       <c r="C140" t="inlineStr">
         <is>
-          <t>Author of the book "The Feminine Mystique," which helped to spark the second wave of the feminist movement.</t>
+          <t>Medieval Andalusian surgeon and polymath who wrote extensively on medicine, surgery, and pharmacology, influencing medical practices for centuries.</t>
         </is>
       </c>
       <c r="D140" t="inlineStr">
@@ -7183,7 +7235,7 @@
       <c r="I140" t="inlineStr"/>
       <c r="J140" t="inlineStr">
         <is>
-          <t>Generate 10 pretty long and interesting facts about Betty Friedan</t>
+          <t>Please provide me with 10 long and interesting facts about Abu al-Qasim al-Zahrawi. I have a youtube channel based on influential figures so this information must be accurate as my channel depends on it. Please make the output of the facts at least 700 words long. Thank you.</t>
         </is>
       </c>
     </row>
@@ -7193,12 +7245,12 @@
       </c>
       <c r="B141" t="inlineStr">
         <is>
-          <t>Bjorn Borg</t>
+          <t>Haile Selassie</t>
         </is>
       </c>
       <c r="C141" t="inlineStr">
         <is>
-          <t>Swedish tennis legend, dominated the tennis world in the late 1970s.</t>
+          <t>Emperor of Ethiopia and African unity advocate.</t>
         </is>
       </c>
       <c r="D141" t="inlineStr">
@@ -7229,7 +7281,7 @@
       <c r="I141" t="inlineStr"/>
       <c r="J141" t="inlineStr">
         <is>
-          <t>Generate 10 pretty long and interesting facts about Bjorn Borg</t>
+          <t>Please provide me with 10 long and interesting facts about Haile Selassie. I have a youtube channel based on influential figures so this information must be accurate as my channel depends on it. Please make the output of the facts at least 700 words long. Thank you.</t>
         </is>
       </c>
     </row>
@@ -7239,12 +7291,12 @@
       </c>
       <c r="B142" t="inlineStr">
         <is>
-          <t>Ono no Komachi</t>
+          <t>W.E.B. Du Bois</t>
         </is>
       </c>
       <c r="C142" t="inlineStr">
         <is>
-          <t>Japanese poet in the 9th century, one of the "Six Immortals of Poetry" known for her lyrical and emotional verses.</t>
+          <t>One of the most important figures in the American civil rights movement, he was a scholar, writer, and activist.</t>
         </is>
       </c>
       <c r="D142" t="inlineStr">
@@ -7275,7 +7327,7 @@
       <c r="I142" t="inlineStr"/>
       <c r="J142" t="inlineStr">
         <is>
-          <t>Generate 10 pretty long and interesting facts about Ono no Komachi</t>
+          <t>Please provide me with 10 long and interesting facts about W.E.B. Du Bois. I have a youtube channel based on influential figures so this information must be accurate as my channel depends on it. Please make the output of the facts at least 700 words long. Thank you.</t>
         </is>
       </c>
     </row>
@@ -7285,12 +7337,12 @@
       </c>
       <c r="B143" t="inlineStr">
         <is>
-          <t>Hakeem Olajuwon</t>
+          <t>Kofi Annan</t>
         </is>
       </c>
       <c r="C143" t="inlineStr">
         <is>
-          <t>Nigerian-American basketball player, NBA legend.</t>
+          <t>Ghanaian diplomat, UN Secretary-General, Nobel laureate.</t>
         </is>
       </c>
       <c r="D143" t="inlineStr">
@@ -7321,7 +7373,7 @@
       <c r="I143" t="inlineStr"/>
       <c r="J143" t="inlineStr">
         <is>
-          <t>Generate 10 pretty long and interesting facts about Hakeem Olajuwon</t>
+          <t>Please provide me with 10 long and interesting facts about Kofi Annan. I have a youtube channel based on influential figures so this information must be accurate as my channel depends on it. Please make the output of the facts at least 700 words long. Thank you.</t>
         </is>
       </c>
     </row>
@@ -7331,12 +7383,12 @@
       </c>
       <c r="B144" t="inlineStr">
         <is>
-          <t>Ching Shih</t>
+          <t>Maria Mutola</t>
         </is>
       </c>
       <c r="C144" t="inlineStr">
         <is>
-          <t>Chinese pirate leader during the early 19th century, who commanded a vast fleet and became one of the most successful pirates in history.</t>
+          <t>Mozambican middle-distance runner, Olympic gold medalist.</t>
         </is>
       </c>
       <c r="D144" t="inlineStr">
@@ -7367,7 +7419,7 @@
       <c r="I144" t="inlineStr"/>
       <c r="J144" t="inlineStr">
         <is>
-          <t>Generate 10 pretty long and interesting facts about Ching Shih</t>
+          <t>Please provide me with 10 long and interesting facts about Maria Mutola. I have a youtube channel based on influential figures so this information must be accurate as my channel depends on it. Please make the output of the facts at least 700 words long. Thank you.</t>
         </is>
       </c>
     </row>
@@ -7377,12 +7429,12 @@
       </c>
       <c r="B145" t="inlineStr">
         <is>
-          <t>Jomo Kenyatta</t>
+          <t>Wilhelmina Drucker</t>
         </is>
       </c>
       <c r="C145" t="inlineStr">
         <is>
-          <t>Founding father and first president of Kenya.</t>
+          <t>One of the first women to be elected to the German parliament, she was a leading figure in the women's suffrage movement.</t>
         </is>
       </c>
       <c r="D145" t="inlineStr">
@@ -7413,7 +7465,7 @@
       <c r="I145" t="inlineStr"/>
       <c r="J145" t="inlineStr">
         <is>
-          <t>Generate 10 pretty long and interesting facts about Jomo Kenyatta</t>
+          <t>Please provide me with 10 long and interesting facts about Wilhelmina Drucker. I have a youtube channel based on influential figures so this information must be accurate as my channel depends on it. Please make the output of the facts at least 700 words long. Thank you.</t>
         </is>
       </c>
     </row>
@@ -7423,12 +7475,12 @@
       </c>
       <c r="B146" t="inlineStr">
         <is>
-          <t>Elon Musk</t>
+          <t>Golda Meir</t>
         </is>
       </c>
       <c r="C146" t="inlineStr">
         <is>
-          <t>Co-founder of Tesla and SpaceX, he is one of the most innovative entrepreneurs of our time.</t>
+          <t>Israeli Prime Minister and one of the world's first female heads of government.</t>
         </is>
       </c>
       <c r="D146" t="inlineStr">
@@ -7459,7 +7511,7 @@
       <c r="I146" t="inlineStr"/>
       <c r="J146" t="inlineStr">
         <is>
-          <t>Generate 10 pretty long and interesting facts about Elon Musk</t>
+          <t>Please provide me with 10 long and interesting facts about Golda Meir. I have a youtube channel based on influential figures so this information must be accurate as my channel depends on it. Please make the output of the facts at least 700 words long. Thank you.</t>
         </is>
       </c>
     </row>
@@ -7469,12 +7521,12 @@
       </c>
       <c r="B147" t="inlineStr">
         <is>
-          <t>Pele</t>
+          <t>Hicham El Guerrouj</t>
         </is>
       </c>
       <c r="C147" t="inlineStr">
         <is>
-          <t>Brazilian football legend, three-time World Cup winner.</t>
+          <t>Moroccan middle-distance runner, Olympic gold medalist.</t>
         </is>
       </c>
       <c r="D147" t="inlineStr">
@@ -7505,7 +7557,7 @@
       <c r="I147" t="inlineStr"/>
       <c r="J147" t="inlineStr">
         <is>
-          <t>Generate 10 pretty long and interesting facts about Pele</t>
+          <t>Please provide me with 10 long and interesting facts about Hicham El Guerrouj. I have a youtube channel based on influential figures so this information must be accurate as my channel depends on it. Please make the output of the facts at least 700 words long. Thank you.</t>
         </is>
       </c>
     </row>
@@ -7515,12 +7567,12 @@
       </c>
       <c r="B148" t="inlineStr">
         <is>
-          <t>Tomoe Gozen</t>
+          <t>Elon Musk</t>
         </is>
       </c>
       <c r="C148" t="inlineStr">
         <is>
-          <t>Female samurai warrior during the 12th century in Japan, renowned for her combat skills and bravery on the battlefield.</t>
+          <t>Co-founder of Tesla and SpaceX, he is one of the most innovative entrepreneurs of our time.</t>
         </is>
       </c>
       <c r="D148" t="inlineStr">
@@ -7551,7 +7603,7 @@
       <c r="I148" t="inlineStr"/>
       <c r="J148" t="inlineStr">
         <is>
-          <t>Generate 10 pretty long and interesting facts about Tomoe Gozen</t>
+          <t>Please provide me with 10 long and interesting facts about Elon Musk. I have a youtube channel based on influential figures so this information must be accurate as my channel depends on it. Please make the output of the facts at least 700 words long. Thank you.</t>
         </is>
       </c>
     </row>
@@ -7561,12 +7613,12 @@
       </c>
       <c r="B149" t="inlineStr">
         <is>
-          <t>Miriam Makeba</t>
+          <t>Michael Essien</t>
         </is>
       </c>
       <c r="C149" t="inlineStr">
         <is>
-          <t>South African singer and civil rights activist.</t>
+          <t>Ghanaian footballer, known for his versatility.</t>
         </is>
       </c>
       <c r="D149" t="inlineStr">
@@ -7597,7 +7649,7 @@
       <c r="I149" t="inlineStr"/>
       <c r="J149" t="inlineStr">
         <is>
-          <t>Generate 10 pretty long and interesting facts about Miriam Makeba</t>
+          <t>Please provide me with 10 long and interesting facts about Michael Essien. I have a youtube channel based on influential figures so this information must be accurate as my channel depends on it. Please make the output of the facts at least 700 words long. Thank you.</t>
         </is>
       </c>
     </row>
@@ -7607,12 +7659,12 @@
       </c>
       <c r="B150" t="inlineStr">
         <is>
-          <t>Jim Henson</t>
+          <t>Mikhail Gorbachev</t>
         </is>
       </c>
       <c r="C150" t="inlineStr">
         <is>
-          <t>One of the most influential puppeteers of all time, he created some of the most beloved characters in television history.</t>
+          <t>Soviet statesman, implemented reforms leading to the end of the Cold War.</t>
         </is>
       </c>
       <c r="D150" t="inlineStr">
@@ -7643,7 +7695,7 @@
       <c r="I150" t="inlineStr"/>
       <c r="J150" t="inlineStr">
         <is>
-          <t>Generate 10 pretty long and interesting facts about Jim Henson</t>
+          <t>Please provide me with 10 long and interesting facts about Mikhail Gorbachev. I have a youtube channel based on influential figures so this information must be accurate as my channel depends on it. Please make the output of the facts at least 700 words long. Thank you.</t>
         </is>
       </c>
     </row>
@@ -7653,12 +7705,12 @@
       </c>
       <c r="B151" t="inlineStr">
         <is>
-          <t>Harvey Milk</t>
+          <t>Blessing Okagbare</t>
         </is>
       </c>
       <c r="C151" t="inlineStr">
         <is>
-          <t>One of the first openly gay elected officials in the United States, he was a leading figure in the gay rights movement.</t>
+          <t>Nigerian track and field athlete, Olympic medalist.</t>
         </is>
       </c>
       <c r="D151" t="inlineStr">
@@ -7689,7 +7741,7 @@
       <c r="I151" t="inlineStr"/>
       <c r="J151" t="inlineStr">
         <is>
-          <t>Generate 10 pretty long and interesting facts about Harvey Milk</t>
+          <t>Please provide me with 10 long and interesting facts about Blessing Okagbare. I have a youtube channel based on influential figures so this information must be accurate as my channel depends on it. Please make the output of the facts at least 700 words long. Thank you.</t>
         </is>
       </c>
     </row>
@@ -7699,12 +7751,12 @@
       </c>
       <c r="B152" t="inlineStr">
         <is>
-          <t>Daenerys Targaryen</t>
+          <t>Tina Fey</t>
         </is>
       </c>
       <c r="C152" t="inlineStr">
         <is>
-          <t>A fictional character in the "Game of Thrones" series, she is a powerful and inspiring leader.</t>
+          <t>One of the most successful comedians of all time, she is also a successful actress and writer.</t>
         </is>
       </c>
       <c r="D152" t="inlineStr">
@@ -7735,7 +7787,7 @@
       <c r="I152" t="inlineStr"/>
       <c r="J152" t="inlineStr">
         <is>
-          <t>Generate 10 pretty long and interesting facts about Daenerys Targaryen</t>
+          <t>Please provide me with 10 long and interesting facts about Tina Fey. I have a youtube channel based on influential figures so this information must be accurate as my channel depends on it. Please make the output of the facts at least 700 words long. Thank you.</t>
         </is>
       </c>
     </row>
@@ -7745,12 +7797,12 @@
       </c>
       <c r="B153" t="inlineStr">
         <is>
-          <t>Frank Sinatra</t>
+          <t>John Lennon</t>
         </is>
       </c>
       <c r="C153" t="inlineStr">
         <is>
-          <t>American singer and actor, known for his timeless classics.</t>
+          <t>British singer, songwriter, and member of The Beatles.</t>
         </is>
       </c>
       <c r="D153" t="inlineStr">
@@ -7781,7 +7833,7 @@
       <c r="I153" t="inlineStr"/>
       <c r="J153" t="inlineStr">
         <is>
-          <t>Generate 10 pretty long and interesting facts about Frank Sinatra</t>
+          <t>Please provide me with 10 long and interesting facts about John Lennon. I have a youtube channel based on influential figures so this information must be accurate as my channel depends on it. Please make the output of the facts at least 700 words long. Thank you.</t>
         </is>
       </c>
     </row>
@@ -7827,7 +7879,7 @@
       <c r="I154" t="inlineStr"/>
       <c r="J154" t="inlineStr">
         <is>
-          <t>Generate 10 pretty long and interesting facts about Aung San Suu Kyi</t>
+          <t>Please provide me with 10 long and interesting facts about Aung San Suu Kyi. I have a youtube channel based on influential figures so this information must be accurate as my channel depends on it. Please make the output of the facts at least 700 words long. Thank you.</t>
         </is>
       </c>
     </row>
@@ -7837,12 +7889,12 @@
       </c>
       <c r="B155" t="inlineStr">
         <is>
-          <t>Michael Essien</t>
+          <t>Empress Jingu</t>
         </is>
       </c>
       <c r="C155" t="inlineStr">
         <is>
-          <t>Ghanaian footballer, known for his versatility.</t>
+          <t>Legendary Japanese empress who led successful military campaigns, including the conquest of Korea, during the 3rd century.</t>
         </is>
       </c>
       <c r="D155" t="inlineStr">
@@ -7873,7 +7925,7 @@
       <c r="I155" t="inlineStr"/>
       <c r="J155" t="inlineStr">
         <is>
-          <t>Generate 10 pretty long and interesting facts about Michael Essien</t>
+          <t>Please provide me with 10 long and interesting facts about Empress Jingu. I have a youtube channel based on influential figures so this information must be accurate as my channel depends on it. Please make the output of the facts at least 700 words long. Thank you.</t>
         </is>
       </c>
     </row>
@@ -7883,12 +7935,12 @@
       </c>
       <c r="B156" t="inlineStr">
         <is>
-          <t>Chen Guangcheng</t>
+          <t>Thomas Sankara</t>
         </is>
       </c>
       <c r="C156" t="inlineStr">
         <is>
-          <t>Fought for the rights of people with disabilities in China and was imprisoned for his activism.</t>
+          <t>Burkina Faso's revolutionary leader and president.</t>
         </is>
       </c>
       <c r="D156" t="inlineStr">
@@ -7919,7 +7971,7 @@
       <c r="I156" t="inlineStr"/>
       <c r="J156" t="inlineStr">
         <is>
-          <t>Generate 10 pretty long and interesting facts about Chen Guangcheng</t>
+          <t>Please provide me with 10 long and interesting facts about Thomas Sankara. I have a youtube channel based on influential figures so this information must be accurate as my channel depends on it. Please make the output of the facts at least 700 words long. Thank you.</t>
         </is>
       </c>
     </row>
@@ -7929,12 +7981,12 @@
       </c>
       <c r="B157" t="inlineStr">
         <is>
-          <t>George Orwell</t>
+          <t>Mustafa Kemal Atatürk</t>
         </is>
       </c>
       <c r="C157" t="inlineStr">
         <is>
-          <t>One of the most important writers of the 20th century, he wrote about the dangers of totalitarianism.</t>
+          <t>Founder and first President of Turkey, known for modernizing reforms.</t>
         </is>
       </c>
       <c r="D157" t="inlineStr">
@@ -7965,7 +8017,7 @@
       <c r="I157" t="inlineStr"/>
       <c r="J157" t="inlineStr">
         <is>
-          <t>Generate 10 pretty long and interesting facts about George Orwell</t>
+          <t>Please provide me with 10 long and interesting facts about Mustafa Kemal Atatürk. I have a youtube channel based on influential figures so this information must be accurate as my channel depends on it. Please make the output of the facts at least 700 words long. Thank you.</t>
         </is>
       </c>
     </row>
@@ -7975,12 +8027,12 @@
       </c>
       <c r="B158" t="inlineStr">
         <is>
-          <t>Mao Zedong</t>
+          <t>Blessing Awodibu</t>
         </is>
       </c>
       <c r="C158" t="inlineStr">
         <is>
-          <t>Chinese communist revolutionary and founding father of the People's Republic of China.</t>
+          <t>South African bodybuilder and social media influencer.</t>
         </is>
       </c>
       <c r="D158" t="inlineStr">
@@ -8011,7 +8063,7 @@
       <c r="I158" t="inlineStr"/>
       <c r="J158" t="inlineStr">
         <is>
-          <t>Generate 10 pretty long and interesting facts about Mao Zedong</t>
+          <t>Please provide me with 10 long and interesting facts about Blessing Awodibu. I have a youtube channel based on influential figures so this information must be accurate as my channel depends on it. Please make the output of the facts at least 700 words long. Thank you.</t>
         </is>
       </c>
     </row>
@@ -8021,12 +8073,12 @@
       </c>
       <c r="B159" t="inlineStr">
         <is>
-          <t>Bob Dylan</t>
+          <t>Rani Padmini</t>
         </is>
       </c>
       <c r="C159" t="inlineStr">
         <is>
-          <t>American singer-songwriter, Nobel laureate for literature.</t>
+          <t>Queen of Mewar in medieval India, renowned for her beauty and bravery during the siege of Chittorgarh by Alauddin Khilji.</t>
         </is>
       </c>
       <c r="D159" t="inlineStr">
@@ -8057,7 +8109,7 @@
       <c r="I159" t="inlineStr"/>
       <c r="J159" t="inlineStr">
         <is>
-          <t>Generate 10 pretty long and interesting facts about Bob Dylan</t>
+          <t>Please provide me with 10 long and interesting facts about Rani Padmini. I have a youtube channel based on influential figures so this information must be accurate as my channel depends on it. Please make the output of the facts at least 700 words long. Thank you.</t>
         </is>
       </c>
     </row>
@@ -8067,12 +8119,12 @@
       </c>
       <c r="B160" t="inlineStr">
         <is>
-          <t>Blessing Awodibu</t>
+          <t>Xenophon</t>
         </is>
       </c>
       <c r="C160" t="inlineStr">
         <is>
-          <t>South African bodybuilder and social media influencer.</t>
+          <t>A Greek historian and soldier, he wrote about the Peloponnesian War and the Anabasis.</t>
         </is>
       </c>
       <c r="D160" t="inlineStr">
@@ -8103,7 +8155,7 @@
       <c r="I160" t="inlineStr"/>
       <c r="J160" t="inlineStr">
         <is>
-          <t>Generate 10 pretty long and interesting facts about Blessing Awodibu</t>
+          <t>Please provide me with 10 long and interesting facts about Xenophon. I have a youtube channel based on influential figures so this information must be accurate as my channel depends on it. Please make the output of the facts at least 700 words long. Thank you.</t>
         </is>
       </c>
     </row>
@@ -8113,12 +8165,12 @@
       </c>
       <c r="B161" t="inlineStr">
         <is>
-          <t>Jelimo Pamela</t>
+          <t>Jean-Claude Killy</t>
         </is>
       </c>
       <c r="C161" t="inlineStr">
         <is>
-          <t>Kenyan middle-distance runner, Olympic gold medalist.</t>
+          <t>French alpine ski racer, triple Olympic gold medalist.</t>
         </is>
       </c>
       <c r="D161" t="inlineStr">
@@ -8149,7 +8201,7 @@
       <c r="I161" t="inlineStr"/>
       <c r="J161" t="inlineStr">
         <is>
-          <t>Generate 10 pretty long and interesting facts about Jelimo Pamela</t>
+          <t>Please provide me with 10 long and interesting facts about Jean-Claude Killy. I have a youtube channel based on influential figures so this information must be accurate as my channel depends on it. Please make the output of the facts at least 700 words long. Thank you.</t>
         </is>
       </c>
     </row>
@@ -8159,12 +8211,12 @@
       </c>
       <c r="B162" t="inlineStr">
         <is>
-          <t>Vivian Cheruiyot</t>
+          <t>Roy Lichtenstein</t>
         </is>
       </c>
       <c r="C162" t="inlineStr">
         <is>
-          <t>Kenyan long-distance runner, Olympic gold medalist.</t>
+          <t>American pop artist, known for his comic book-style artwork.</t>
         </is>
       </c>
       <c r="D162" t="inlineStr">
@@ -8195,7 +8247,7 @@
       <c r="I162" t="inlineStr"/>
       <c r="J162" t="inlineStr">
         <is>
-          <t>Generate 10 pretty long and interesting facts about Vivian Cheruiyot</t>
+          <t>Please provide me with 10 long and interesting facts about Roy Lichtenstein. I have a youtube channel based on influential figures so this information must be accurate as my channel depends on it. Please make the output of the facts at least 700 words long. Thank you.</t>
         </is>
       </c>
     </row>
@@ -8205,12 +8257,12 @@
       </c>
       <c r="B163" t="inlineStr">
         <is>
-          <t>Jean-Claude Killy</t>
+          <t>Jawaharlal Nehru</t>
         </is>
       </c>
       <c r="C163" t="inlineStr">
         <is>
-          <t>French alpine ski racer, triple Olympic gold medalist.</t>
+          <t>Indian independence leader and the first Prime Minister of India.</t>
         </is>
       </c>
       <c r="D163" t="inlineStr">
@@ -8241,7 +8293,7 @@
       <c r="I163" t="inlineStr"/>
       <c r="J163" t="inlineStr">
         <is>
-          <t>Generate 10 pretty long and interesting facts about Jean-Claude Killy</t>
+          <t>Please provide me with 10 long and interesting facts about Jawaharlal Nehru. I have a youtube channel based on influential figures so this information must be accurate as my channel depends on it. Please make the output of the facts at least 700 words long. Thank you.</t>
         </is>
       </c>
     </row>
@@ -8251,12 +8303,12 @@
       </c>
       <c r="B164" t="inlineStr">
         <is>
-          <t>Stephen Keshi</t>
+          <t>Ho Chi Minh</t>
         </is>
       </c>
       <c r="C164" t="inlineStr">
         <is>
-          <t>Nigerian footballer and coach, led Nigeria to AFCON victory.</t>
+          <t>Vietnamese communist revolutionary and President of North Vietnam.</t>
         </is>
       </c>
       <c r="D164" t="inlineStr">
@@ -8287,7 +8339,7 @@
       <c r="I164" t="inlineStr"/>
       <c r="J164" t="inlineStr">
         <is>
-          <t>Generate 10 pretty long and interesting facts about Stephen Keshi</t>
+          <t>Please provide me with 10 long and interesting facts about Ho Chi Minh. I have a youtube channel based on influential figures so this information must be accurate as my channel depends on it. Please make the output of the facts at least 700 words long. Thank you.</t>
         </is>
       </c>
     </row>
@@ -8297,12 +8349,12 @@
       </c>
       <c r="B165" t="inlineStr">
         <is>
-          <t>Xenophon</t>
+          <t>Jelimo Pamela</t>
         </is>
       </c>
       <c r="C165" t="inlineStr">
         <is>
-          <t>A Greek historian and soldier, he wrote about the Peloponnesian War and the Anabasis.</t>
+          <t>Kenyan middle-distance runner, Olympic gold medalist.</t>
         </is>
       </c>
       <c r="D165" t="inlineStr">
@@ -8333,7 +8385,7 @@
       <c r="I165" t="inlineStr"/>
       <c r="J165" t="inlineStr">
         <is>
-          <t>Generate 10 pretty long and interesting facts about Xenophon</t>
+          <t>Please provide me with 10 long and interesting facts about Jelimo Pamela. I have a youtube channel based on influential figures so this information must be accurate as my channel depends on it. Please make the output of the facts at least 700 words long. Thank you.</t>
         </is>
       </c>
     </row>
@@ -8343,12 +8395,12 @@
       </c>
       <c r="B166" t="inlineStr">
         <is>
-          <t>Michelangelo</t>
+          <t>Andy Warhol</t>
         </is>
       </c>
       <c r="C166" t="inlineStr">
         <is>
-          <t>Italian sculptor, painter, and architect, known for works like the Sistine Chapel ceiling.</t>
+          <t>American pop art pioneer, known for his iconic portraits and prints.</t>
         </is>
       </c>
       <c r="D166" t="inlineStr">
@@ -8379,7 +8431,7 @@
       <c r="I166" t="inlineStr"/>
       <c r="J166" t="inlineStr">
         <is>
-          <t>Generate 10 pretty long and interesting facts about Michelangelo</t>
+          <t>Please provide me with 10 long and interesting facts about Andy Warhol. I have a youtube channel based on influential figures so this information must be accurate as my channel depends on it. Please make the output of the facts at least 700 words long. Thank you.</t>
         </is>
       </c>
     </row>
@@ -8389,12 +8441,12 @@
       </c>
       <c r="B167" t="inlineStr">
         <is>
-          <t>Stevie Wonder</t>
+          <t>Jackson Pollock</t>
         </is>
       </c>
       <c r="C167" t="inlineStr">
         <is>
-          <t>American singer, songwriter, and multi-instrumentalist.</t>
+          <t>American abstract expressionist painter, known for his unique drip painting technique.</t>
         </is>
       </c>
       <c r="D167" t="inlineStr">
@@ -8425,7 +8477,7 @@
       <c r="I167" t="inlineStr"/>
       <c r="J167" t="inlineStr">
         <is>
-          <t>Generate 10 pretty long and interesting facts about Stevie Wonder</t>
+          <t>Please provide me with 10 long and interesting facts about Jackson Pollock. I have a youtube channel based on influential figures so this information must be accurate as my channel depends on it. Please make the output of the facts at least 700 words long. Thank you.</t>
         </is>
       </c>
     </row>
@@ -8435,12 +8487,12 @@
       </c>
       <c r="B168" t="inlineStr">
         <is>
-          <t>Empress Jingu</t>
+          <t>Betty Friedan</t>
         </is>
       </c>
       <c r="C168" t="inlineStr">
         <is>
-          <t>Legendary Japanese empress who led successful military campaigns, including the conquest of Korea, during the 3rd century.</t>
+          <t>Author of the book "The Feminine Mystique," which helped to spark the second wave of the feminist movement.</t>
         </is>
       </c>
       <c r="D168" t="inlineStr">
@@ -8471,7 +8523,7 @@
       <c r="I168" t="inlineStr"/>
       <c r="J168" t="inlineStr">
         <is>
-          <t>Generate 10 pretty long and interesting facts about Empress Jingu</t>
+          <t>Please provide me with 10 long and interesting facts about Betty Friedan. I have a youtube channel based on influential figures so this information must be accurate as my channel depends on it. Please make the output of the facts at least 700 words long. Thank you.</t>
         </is>
       </c>
     </row>
@@ -8481,12 +8533,12 @@
       </c>
       <c r="B169" t="inlineStr">
         <is>
-          <t>Hicham El Guerrouj</t>
+          <t>Blessing Oborududu</t>
         </is>
       </c>
       <c r="C169" t="inlineStr">
         <is>
-          <t>Moroccan middle-distance runner, Olympic gold medalist.</t>
+          <t>Nigerian wrestler, first African female wrestling Olympic medalist.</t>
         </is>
       </c>
       <c r="D169" t="inlineStr">
@@ -8517,7 +8569,7 @@
       <c r="I169" t="inlineStr"/>
       <c r="J169" t="inlineStr">
         <is>
-          <t>Generate 10 pretty long and interesting facts about Hicham El Guerrouj</t>
+          <t>Please provide me with 10 long and interesting facts about Blessing Oborududu. I have a youtube channel based on influential figures so this information must be accurate as my channel depends on it. Please make the output of the facts at least 700 words long. Thank you.</t>
         </is>
       </c>
     </row>
@@ -8527,12 +8579,12 @@
       </c>
       <c r="B170" t="inlineStr">
         <is>
-          <t>Ibn Battuta</t>
+          <t>Tomoe Gozen</t>
         </is>
       </c>
       <c r="C170" t="inlineStr">
         <is>
-          <t>Moroccan explorer and scholar who embarked on extensive travels throughout the Islamic world, chronicling his journeys in his renowned travelogue.</t>
+          <t>Female samurai warrior during the 12th century in Japan, renowned for her combat skills and bravery on the battlefield.</t>
         </is>
       </c>
       <c r="D170" t="inlineStr">
@@ -8563,7 +8615,7 @@
       <c r="I170" t="inlineStr"/>
       <c r="J170" t="inlineStr">
         <is>
-          <t>Generate 10 pretty long and interesting facts about Ibn Battuta</t>
+          <t>Please provide me with 10 long and interesting facts about Tomoe Gozen. I have a youtube channel based on influential figures so this information must be accurate as my channel depends on it. Please make the output of the facts at least 700 words long. Thank you.</t>
         </is>
       </c>
     </row>
@@ -8573,12 +8625,12 @@
       </c>
       <c r="B171" t="inlineStr">
         <is>
-          <t>Blessing Oborududu</t>
+          <t>Daenerys Targaryen</t>
         </is>
       </c>
       <c r="C171" t="inlineStr">
         <is>
-          <t>Nigerian wrestler, first African female wrestling Olympic medalist.</t>
+          <t>A fictional character in the "Game of Thrones" series, she is a powerful and inspiring leader.</t>
         </is>
       </c>
       <c r="D171" t="inlineStr">
@@ -8609,7 +8661,7 @@
       <c r="I171" t="inlineStr"/>
       <c r="J171" t="inlineStr">
         <is>
-          <t>Generate 10 pretty long and interesting facts about Blessing Oborududu</t>
+          <t>Please provide me with 10 long and interesting facts about Daenerys Targaryen. I have a youtube channel based on influential figures so this information must be accurate as my channel depends on it. Please make the output of the facts at least 700 words long. Thank you.</t>
         </is>
       </c>
     </row>
@@ -8619,12 +8671,12 @@
       </c>
       <c r="B172" t="inlineStr">
         <is>
-          <t>Haile Selassie</t>
+          <t>Frank Sinatra</t>
         </is>
       </c>
       <c r="C172" t="inlineStr">
         <is>
-          <t>Emperor of Ethiopia and African unity advocate.</t>
+          <t>American singer and actor, known for his timeless classics.</t>
         </is>
       </c>
       <c r="D172" t="inlineStr">
@@ -8655,7 +8707,7 @@
       <c r="I172" t="inlineStr"/>
       <c r="J172" t="inlineStr">
         <is>
-          <t>Generate 10 pretty long and interesting facts about Haile Selassie</t>
+          <t>Please provide me with 10 long and interesting facts about Frank Sinatra. I have a youtube channel based on influential figures so this information must be accurate as my channel depends on it. Please make the output of the facts at least 700 words long. Thank you.</t>
         </is>
       </c>
     </row>
@@ -8665,12 +8717,12 @@
       </c>
       <c r="B173" t="inlineStr">
         <is>
-          <t>Al-Maʿarri</t>
+          <t>Yaya Touré</t>
         </is>
       </c>
       <c r="C173" t="inlineStr">
         <is>
-          <t>Arabian philosopher and poet in the 11th century, known for his skepticism and critical views on religious and societal norms.</t>
+          <t>Ivorian footballer and four-time African Player of the Year.</t>
         </is>
       </c>
       <c r="D173" t="inlineStr">
@@ -8701,7 +8753,7 @@
       <c r="I173" t="inlineStr"/>
       <c r="J173" t="inlineStr">
         <is>
-          <t>Generate 10 pretty long and interesting facts about Al-Maʿarri</t>
+          <t>Please provide me with 10 long and interesting facts about Yaya Touré. I have a youtube channel based on influential figures so this information must be accurate as my channel depends on it. Please make the output of the facts at least 700 words long. Thank you.</t>
         </is>
       </c>
     </row>
@@ -8711,12 +8763,12 @@
       </c>
       <c r="B174" t="inlineStr">
         <is>
-          <t>Abebe Bikila</t>
+          <t>Steve Biko</t>
         </is>
       </c>
       <c r="C174" t="inlineStr">
         <is>
-          <t>Ethiopian marathon runner and Olympic champion.</t>
+          <t>Black Consciousness Movement leader in South Africa.</t>
         </is>
       </c>
       <c r="D174" t="inlineStr">
@@ -8747,7 +8799,7 @@
       <c r="I174" t="inlineStr"/>
       <c r="J174" t="inlineStr">
         <is>
-          <t>Generate 10 pretty long and interesting facts about Abebe Bikila</t>
+          <t>Please provide me with 10 long and interesting facts about Steve Biko. I have a youtube channel based on influential figures so this information must be accurate as my channel depends on it. Please make the output of the facts at least 700 words long. Thank you.</t>
         </is>
       </c>
     </row>
@@ -8757,12 +8809,12 @@
       </c>
       <c r="B175" t="inlineStr">
         <is>
-          <t>Emperor Wu of Liang</t>
+          <t>Queen Ranavalona III</t>
         </is>
       </c>
       <c r="C175" t="inlineStr">
         <is>
-          <t>Ruler of the Liang Dynasty in China during the 6th century CE, famous for his support of Buddhism and patronage of the arts.</t>
+          <t>Last sovereign of the Kingdom of Madagascar.</t>
         </is>
       </c>
       <c r="D175" t="inlineStr">
@@ -8793,7 +8845,7 @@
       <c r="I175" t="inlineStr"/>
       <c r="J175" t="inlineStr">
         <is>
-          <t>Generate 10 pretty long and interesting facts about Emperor Wu of Liang</t>
+          <t>Please provide me with 10 long and interesting facts about Queen Ranavalona III. I have a youtube channel based on influential figures so this information must be accurate as my channel depends on it. Please make the output of the facts at least 700 words long. Thank you.</t>
         </is>
       </c>
     </row>
@@ -8803,12 +8855,12 @@
       </c>
       <c r="B176" t="inlineStr">
         <is>
-          <t>Jacqueline Kennedy Onassis</t>
+          <t>Abebe Bikila</t>
         </is>
       </c>
       <c r="C176" t="inlineStr">
         <is>
-          <t>One of the most popular First Ladies of the 20th century, she was also a successful author.</t>
+          <t>Ethiopian marathon runner and Olympic champion.</t>
         </is>
       </c>
       <c r="D176" t="inlineStr">
@@ -8839,7 +8891,7 @@
       <c r="I176" t="inlineStr"/>
       <c r="J176" t="inlineStr">
         <is>
-          <t>Generate 10 pretty long and interesting facts about Jacqueline Kennedy Onassis</t>
+          <t>Please provide me with 10 long and interesting facts about Abebe Bikila. I have a youtube channel based on influential figures so this information must be accurate as my channel depends on it. Please make the output of the facts at least 700 words long. Thank you.</t>
         </is>
       </c>
     </row>
@@ -8849,12 +8901,12 @@
       </c>
       <c r="B177" t="inlineStr">
         <is>
-          <t>Tina Fey</t>
+          <t>Patrice Lumumba</t>
         </is>
       </c>
       <c r="C177" t="inlineStr">
         <is>
-          <t>One of the most successful comedians of all time, she is also a successful actress and writer.</t>
+          <t>Independence leader, first PM of the Congo.</t>
         </is>
       </c>
       <c r="D177" t="inlineStr">
@@ -8885,7 +8937,7 @@
       <c r="I177" t="inlineStr"/>
       <c r="J177" t="inlineStr">
         <is>
-          <t>Generate 10 pretty long and interesting facts about Tina Fey</t>
+          <t>Please provide me with 10 long and interesting facts about Patrice Lumumba. I have a youtube channel based on influential figures so this information must be accurate as my channel depends on it. Please make the output of the facts at least 700 words long. Thank you.</t>
         </is>
       </c>
     </row>
@@ -8895,12 +8947,12 @@
       </c>
       <c r="B178" t="inlineStr">
         <is>
-          <t>Funmilayo Ransome-Kuti</t>
+          <t>Noureddine Morceli</t>
         </is>
       </c>
       <c r="C178" t="inlineStr">
         <is>
-          <t>Nigerian women's rights advocate and activist.</t>
+          <t>Algerian middle-distance runner, Olympic gold medalist.</t>
         </is>
       </c>
       <c r="D178" t="inlineStr">
@@ -8931,7 +8983,7 @@
       <c r="I178" t="inlineStr"/>
       <c r="J178" t="inlineStr">
         <is>
-          <t>Generate 10 pretty long and interesting facts about Funmilayo Ransome-Kuti</t>
+          <t>Please provide me with 10 long and interesting facts about Noureddine Morceli. I have a youtube channel based on influential figures so this information must be accurate as my channel depends on it. Please make the output of the facts at least 700 words long. Thank you.</t>
         </is>
       </c>
     </row>
@@ -8941,12 +8993,12 @@
       </c>
       <c r="B179" t="inlineStr">
         <is>
-          <t>Salvador Dalí</t>
+          <t>Al-Maʿarri</t>
         </is>
       </c>
       <c r="C179" t="inlineStr">
         <is>
-          <t>Spanish Surrealist artist, known for his bizarre and dreamlike imagery.</t>
+          <t>Arabian philosopher and poet in the 11th century, known for his skepticism and critical views on religious and societal norms.</t>
         </is>
       </c>
       <c r="D179" t="inlineStr">
@@ -8977,7 +9029,7 @@
       <c r="I179" t="inlineStr"/>
       <c r="J179" t="inlineStr">
         <is>
-          <t>Generate 10 pretty long and interesting facts about Salvador Dalí</t>
+          <t>Please provide me with 10 long and interesting facts about Al-Maʿarri. I have a youtube channel based on influential figures so this information must be accurate as my channel depends on it. Please make the output of the facts at least 700 words long. Thank you.</t>
         </is>
       </c>
     </row>
@@ -8987,12 +9039,12 @@
       </c>
       <c r="B180" t="inlineStr">
         <is>
-          <t>Queen Nzinga</t>
+          <t>Yayoi Kusama</t>
         </is>
       </c>
       <c r="C180" t="inlineStr">
         <is>
-          <t>Queen of Ndongo and Matamba, skilled diplomat.</t>
+          <t>Japanese contemporary artist, known for her immersive installations and polka dot motifs.</t>
         </is>
       </c>
       <c r="D180" t="inlineStr">
@@ -9023,7 +9075,7 @@
       <c r="I180" t="inlineStr"/>
       <c r="J180" t="inlineStr">
         <is>
-          <t>Generate 10 pretty long and interesting facts about Queen Nzinga</t>
+          <t>Please provide me with 10 long and interesting facts about Yayoi Kusama. I have a youtube channel based on influential figures so this information must be accurate as my channel depends on it. Please make the output of the facts at least 700 words long. Thank you.</t>
         </is>
       </c>
     </row>
@@ -9033,12 +9085,12 @@
       </c>
       <c r="B181" t="inlineStr">
         <is>
-          <t>Antonio Vivaldi</t>
+          <t>Bob Marley</t>
         </is>
       </c>
       <c r="C181" t="inlineStr">
         <is>
-          <t>Italian composer, famous for "The Four Seasons."</t>
+          <t>Jamaican reggae icon, known for his messages of unity and peace.</t>
         </is>
       </c>
       <c r="D181" t="inlineStr">
@@ -9069,7 +9121,7 @@
       <c r="I181" t="inlineStr"/>
       <c r="J181" t="inlineStr">
         <is>
-          <t>Generate 10 pretty long and interesting facts about Antonio Vivaldi</t>
+          <t>Please provide me with 10 long and interesting facts about Bob Marley. I have a youtube channel based on influential figures so this information must be accurate as my channel depends on it. Please make the output of the facts at least 700 words long. Thank you.</t>
         </is>
       </c>
     </row>
@@ -9079,12 +9131,12 @@
       </c>
       <c r="B182" t="inlineStr">
         <is>
-          <t>Jawaharlal Nehru</t>
+          <t>Jomo Kenyatta</t>
         </is>
       </c>
       <c r="C182" t="inlineStr">
         <is>
-          <t>Indian independence leader and the first Prime Minister of India.</t>
+          <t>Founding father and first president of Kenya.</t>
         </is>
       </c>
       <c r="D182" t="inlineStr">
@@ -9115,7 +9167,7 @@
       <c r="I182" t="inlineStr"/>
       <c r="J182" t="inlineStr">
         <is>
-          <t>Generate 10 pretty long and interesting facts about Jawaharlal Nehru</t>
+          <t>Please provide me with 10 long and interesting facts about Jomo Kenyatta. I have a youtube channel based on influential figures so this information must be accurate as my channel depends on it. Please make the output of the facts at least 700 words long. Thank you.</t>
         </is>
       </c>
     </row>
@@ -9125,12 +9177,12 @@
       </c>
       <c r="B183" t="inlineStr">
         <is>
-          <t>Queen Ranavalona III</t>
+          <t>Mao Zedong</t>
         </is>
       </c>
       <c r="C183" t="inlineStr">
         <is>
-          <t>Last sovereign of the Kingdom of Madagascar.</t>
+          <t>Chinese communist revolutionary and founding father of the People's Republic of China.</t>
         </is>
       </c>
       <c r="D183" t="inlineStr">
@@ -9161,7 +9213,7 @@
       <c r="I183" t="inlineStr"/>
       <c r="J183" t="inlineStr">
         <is>
-          <t>Generate 10 pretty long and interesting facts about Queen Ranavalona III</t>
+          <t>Please provide me with 10 long and interesting facts about Mao Zedong. I have a youtube channel based on influential figures so this information must be accurate as my channel depends on it. Please make the output of the facts at least 700 words long. Thank you.</t>
         </is>
       </c>
     </row>
@@ -9171,12 +9223,12 @@
       </c>
       <c r="B184" t="inlineStr">
         <is>
-          <t>Yayoi Kusama</t>
+          <t>Ahmed Sékou Touré</t>
         </is>
       </c>
       <c r="C184" t="inlineStr">
         <is>
-          <t>Japanese contemporary artist, known for her immersive installations and polka dot motifs.</t>
+          <t>Guinea's first president and anti-colonial leader.</t>
         </is>
       </c>
       <c r="D184" t="inlineStr">
@@ -9207,7 +9259,7 @@
       <c r="I184" t="inlineStr"/>
       <c r="J184" t="inlineStr">
         <is>
-          <t>Generate 10 pretty long and interesting facts about Yayoi Kusama</t>
+          <t>Please provide me with 10 long and interesting facts about Ahmed Sékou Touré. I have a youtube channel based on influential figures so this information must be accurate as my channel depends on it. Please make the output of the facts at least 700 words long. Thank you.</t>
         </is>
       </c>
     </row>
@@ -9217,12 +9269,12 @@
       </c>
       <c r="B185" t="inlineStr">
         <is>
-          <t>Thomas Sankara</t>
+          <t>Jim Henson</t>
         </is>
       </c>
       <c r="C185" t="inlineStr">
         <is>
-          <t>Burkina Faso's revolutionary leader and president.</t>
+          <t>One of the most influential puppeteers of all time, he created some of the most beloved characters in television history.</t>
         </is>
       </c>
       <c r="D185" t="inlineStr">
@@ -9253,7 +9305,7 @@
       <c r="I185" t="inlineStr"/>
       <c r="J185" t="inlineStr">
         <is>
-          <t>Generate 10 pretty long and interesting facts about Thomas Sankara</t>
+          <t>Please provide me with 10 long and interesting facts about Jim Henson. I have a youtube channel based on influential figures so this information must be accurate as my channel depends on it. Please make the output of the facts at least 700 words long. Thank you.</t>
         </is>
       </c>
     </row>
@@ -9263,12 +9315,12 @@
       </c>
       <c r="B186" t="inlineStr">
         <is>
-          <t>Jim Thorpe</t>
+          <t>Chen Guangcheng</t>
         </is>
       </c>
       <c r="C186" t="inlineStr">
         <is>
-          <t>American multi-sport athlete, Olympic gold medalist and football legend.</t>
+          <t>Fought for the rights of people with disabilities in China and was imprisoned for his activism.</t>
         </is>
       </c>
       <c r="D186" t="inlineStr">
@@ -9299,7 +9351,7 @@
       <c r="I186" t="inlineStr"/>
       <c r="J186" t="inlineStr">
         <is>
-          <t>Generate 10 pretty long and interesting facts about Jim Thorpe</t>
+          <t>Please provide me with 10 long and interesting facts about Chen Guangcheng. I have a youtube channel based on influential figures so this information must be accurate as my channel depends on it. Please make the output of the facts at least 700 words long. Thank you.</t>
         </is>
       </c>
     </row>
@@ -9309,12 +9361,12 @@
       </c>
       <c r="B187" t="inlineStr">
         <is>
-          <t>Elvis Presley</t>
+          <t>Jacqueline Kennedy Onassis</t>
         </is>
       </c>
       <c r="C187" t="inlineStr">
         <is>
-          <t>American rock 'n' roll legend, the "King of Rock and Roll."</t>
+          <t>One of the most popular First Ladies of the 20th century, she was also a successful author.</t>
         </is>
       </c>
       <c r="D187" t="inlineStr">
@@ -9345,7 +9397,7 @@
       <c r="I187" t="inlineStr"/>
       <c r="J187" t="inlineStr">
         <is>
-          <t>Generate 10 pretty long and interesting facts about Elvis Presley</t>
+          <t>Please provide me with 10 long and interesting facts about Jacqueline Kennedy Onassis. I have a youtube channel based on influential figures so this information must be accurate as my channel depends on it. Please make the output of the facts at least 700 words long. Thank you.</t>
         </is>
       </c>
     </row>
@@ -9355,12 +9407,12 @@
       </c>
       <c r="B188" t="inlineStr">
         <is>
-          <t>Guru Nanak</t>
+          <t>Didier Drogba</t>
         </is>
       </c>
       <c r="C188" t="inlineStr">
         <is>
-          <t>Founder of Sikhism in the 15th century, revered as the first Sikh guru and promoting the principles of equality and social justice.</t>
+          <t>Ivorian footballer and humanitarian.</t>
         </is>
       </c>
       <c r="D188" t="inlineStr">
@@ -9391,7 +9443,7 @@
       <c r="I188" t="inlineStr"/>
       <c r="J188" t="inlineStr">
         <is>
-          <t>Generate 10 pretty long and interesting facts about Guru Nanak</t>
+          <t>Please provide me with 10 long and interesting facts about Didier Drogba. I have a youtube channel based on influential figures so this information must be accurate as my channel depends on it. Please make the output of the facts at least 700 words long. Thank you.</t>
         </is>
       </c>
     </row>
@@ -9401,12 +9453,12 @@
       </c>
       <c r="B189" t="inlineStr">
         <is>
-          <t>Ahmed Sékou Touré</t>
+          <t>Henri Cartier-Bresson</t>
         </is>
       </c>
       <c r="C189" t="inlineStr">
         <is>
-          <t>Guinea's first president and anti-colonial leader.</t>
+          <t>French photographer, considered the father of modern photojournalism.</t>
         </is>
       </c>
       <c r="D189" t="inlineStr">
@@ -9437,7 +9489,7 @@
       <c r="I189" t="inlineStr"/>
       <c r="J189" t="inlineStr">
         <is>
-          <t>Generate 10 pretty long and interesting facts about Ahmed Sékou Touré</t>
+          <t>Please provide me with 10 long and interesting facts about Henri Cartier-Bresson. I have a youtube channel based on influential figures so this information must be accurate as my channel depends on it. Please make the output of the facts at least 700 words long. Thank you.</t>
         </is>
       </c>
     </row>
@@ -9447,12 +9499,12 @@
       </c>
       <c r="B190" t="inlineStr">
         <is>
-          <t>Henri Cartier-Bresson</t>
+          <t>Ibn Battuta</t>
         </is>
       </c>
       <c r="C190" t="inlineStr">
         <is>
-          <t>French photographer, considered the father of modern photojournalism.</t>
+          <t>Moroccan explorer and scholar who embarked on extensive travels throughout the Islamic world, chronicling his journeys in his renowned travelogue.</t>
         </is>
       </c>
       <c r="D190" t="inlineStr">
@@ -9483,7 +9535,7 @@
       <c r="I190" t="inlineStr"/>
       <c r="J190" t="inlineStr">
         <is>
-          <t>Generate 10 pretty long and interesting facts about Henri Cartier-Bresson</t>
+          <t>Please provide me with 10 long and interesting facts about Ibn Battuta. I have a youtube channel based on influential figures so this information must be accurate as my channel depends on it. Please make the output of the facts at least 700 words long. Thank you.</t>
         </is>
       </c>
     </row>
@@ -9493,12 +9545,12 @@
       </c>
       <c r="B191" t="inlineStr">
         <is>
-          <t>Maria Mutola</t>
+          <t>Vivian Cheruiyot</t>
         </is>
       </c>
       <c r="C191" t="inlineStr">
         <is>
-          <t>Mozambican middle-distance runner, Olympic gold medalist.</t>
+          <t>Kenyan long-distance runner, Olympic gold medalist.</t>
         </is>
       </c>
       <c r="D191" t="inlineStr">
@@ -9529,7 +9581,7 @@
       <c r="I191" t="inlineStr"/>
       <c r="J191" t="inlineStr">
         <is>
-          <t>Generate 10 pretty long and interesting facts about Maria Mutola</t>
+          <t>Please provide me with 10 long and interesting facts about Vivian Cheruiyot. I have a youtube channel based on influential figures so this information must be accurate as my channel depends on it. Please make the output of the facts at least 700 words long. Thank you.</t>
         </is>
       </c>
     </row>
@@ -9539,12 +9591,12 @@
       </c>
       <c r="B192" t="inlineStr">
         <is>
-          <t>Hypatia of Alexandria</t>
+          <t>Martina Navratilova</t>
         </is>
       </c>
       <c r="C192" t="inlineStr">
         <is>
-          <t>Greek mathematician, astronomer, and philosopher in the 4th century CE, known for her contributions to mathematics and astronomy.</t>
+          <t>Czech-American tennis player, considered one of the greatest female players.</t>
         </is>
       </c>
       <c r="D192" t="inlineStr">
@@ -9575,7 +9627,7 @@
       <c r="I192" t="inlineStr"/>
       <c r="J192" t="inlineStr">
         <is>
-          <t>Generate 10 pretty long and interesting facts about Hypatia of Alexandria</t>
+          <t>Please provide me with 10 long and interesting facts about Martina Navratilova. I have a youtube channel based on influential figures so this information must be accurate as my channel depends on it. Please make the output of the facts at least 700 words long. Thank you.</t>
         </is>
       </c>
     </row>
@@ -9585,12 +9637,12 @@
       </c>
       <c r="B193" t="inlineStr">
         <is>
-          <t>Wilhelmina Drucker</t>
+          <t>Jim Thorpe</t>
         </is>
       </c>
       <c r="C193" t="inlineStr">
         <is>
-          <t>One of the first women to be elected to the German parliament, she was a leading figure in the women's suffrage movement.</t>
+          <t>American multi-sport athlete, Olympic gold medalist and football legend.</t>
         </is>
       </c>
       <c r="D193" t="inlineStr">
@@ -9621,7 +9673,7 @@
       <c r="I193" t="inlineStr"/>
       <c r="J193" t="inlineStr">
         <is>
-          <t>Generate 10 pretty long and interesting facts about Wilhelmina Drucker</t>
+          <t>Please provide me with 10 long and interesting facts about Jim Thorpe. I have a youtube channel based on influential figures so this information must be accurate as my channel depends on it. Please make the output of the facts at least 700 words long. Thank you.</t>
         </is>
       </c>
     </row>
@@ -9631,12 +9683,12 @@
       </c>
       <c r="B194" t="inlineStr">
         <is>
-          <t>Jackson Pollock</t>
+          <t>Henri Matisse</t>
         </is>
       </c>
       <c r="C194" t="inlineStr">
         <is>
-          <t>American abstract expressionist painter, known for his unique drip painting technique.</t>
+          <t>French artist, known for his colorful and innovative use of shapes and patterns.</t>
         </is>
       </c>
       <c r="D194" t="inlineStr">
@@ -9667,7 +9719,7 @@
       <c r="I194" t="inlineStr"/>
       <c r="J194" t="inlineStr">
         <is>
-          <t>Generate 10 pretty long and interesting facts about Jackson Pollock</t>
+          <t>Please provide me with 10 long and interesting facts about Henri Matisse. I have a youtube channel based on influential figures so this information must be accurate as my channel depends on it. Please make the output of the facts at least 700 words long. Thank you.</t>
         </is>
       </c>
     </row>
@@ -9677,12 +9729,12 @@
       </c>
       <c r="B195" t="inlineStr">
         <is>
-          <t>John Lennon</t>
+          <t>Al-Kindi</t>
         </is>
       </c>
       <c r="C195" t="inlineStr">
         <is>
-          <t>British singer, songwriter, and member of The Beatles.</t>
+          <t>Arab philosopher and polymath in the 9th century, making significant contributions to mathematics, astronomy, and philosophy.</t>
         </is>
       </c>
       <c r="D195" t="inlineStr">
@@ -9713,7 +9765,7 @@
       <c r="I195" t="inlineStr"/>
       <c r="J195" t="inlineStr">
         <is>
-          <t>Generate 10 pretty long and interesting facts about John Lennon</t>
+          <t>Please provide me with 10 long and interesting facts about Al-Kindi. I have a youtube channel based on influential figures so this information must be accurate as my channel depends on it. Please make the output of the facts at least 700 words long. Thank you.</t>
         </is>
       </c>
     </row>
@@ -9723,12 +9775,12 @@
       </c>
       <c r="B196" t="inlineStr">
         <is>
-          <t>Blessing Okagbare</t>
+          <t>Johann Sebastian Bach</t>
         </is>
       </c>
       <c r="C196" t="inlineStr">
         <is>
-          <t>Nigerian track and field athlete, Olympic medalist.</t>
+          <t>German composer and musician, a Baroque music master.</t>
         </is>
       </c>
       <c r="D196" t="inlineStr">
@@ -9759,7 +9811,7 @@
       <c r="I196" t="inlineStr"/>
       <c r="J196" t="inlineStr">
         <is>
-          <t>Generate 10 pretty long and interesting facts about Blessing Okagbare</t>
+          <t>Please provide me with 10 long and interesting facts about Johann Sebastian Bach. I have a youtube channel based on influential figures so this information must be accurate as my channel depends on it. Please make the output of the facts at least 700 words long. Thank you.</t>
         </is>
       </c>
     </row>
@@ -9769,12 +9821,12 @@
       </c>
       <c r="B197" t="inlineStr">
         <is>
-          <t>Caster Semenya</t>
+          <t>Martina Hingis</t>
         </is>
       </c>
       <c r="C197" t="inlineStr">
         <is>
-          <t>South African middle-distance runner and Olympic gold medalist.</t>
+          <t>Swiss tennis player, former world No. 1 and multiple Grand Slam winner.</t>
         </is>
       </c>
       <c r="D197" t="inlineStr">
@@ -9805,7 +9857,7 @@
       <c r="I197" t="inlineStr"/>
       <c r="J197" t="inlineStr">
         <is>
-          <t>Generate 10 pretty long and interesting facts about Caster Semenya</t>
+          <t>Please provide me with 10 long and interesting facts about Martina Hingis. I have a youtube channel based on influential figures so this information must be accurate as my channel depends on it. Please make the output of the facts at least 700 words long. Thank you.</t>
         </is>
       </c>
     </row>
@@ -9815,12 +9867,12 @@
       </c>
       <c r="B198" t="inlineStr">
         <is>
-          <t>Golda Meir</t>
+          <t>Ellen Johnson Sirleaf</t>
         </is>
       </c>
       <c r="C198" t="inlineStr">
         <is>
-          <t>Israeli Prime Minister and one of the world's first female heads of government.</t>
+          <t>First female president in Africa and Nobel laureate.</t>
         </is>
       </c>
       <c r="D198" t="inlineStr">
@@ -9851,7 +9903,7 @@
       <c r="I198" t="inlineStr"/>
       <c r="J198" t="inlineStr">
         <is>
-          <t>Generate 10 pretty long and interesting facts about Golda Meir</t>
+          <t>Please provide me with 10 long and interesting facts about Ellen Johnson Sirleaf. I have a youtube channel based on influential figures so this information must be accurate as my channel depends on it. Please make the output of the facts at least 700 words long. Thank you.</t>
         </is>
       </c>
     </row>
@@ -9861,12 +9913,12 @@
       </c>
       <c r="B199" t="inlineStr">
         <is>
-          <t>Bob Marley</t>
+          <t>Edvard Munch</t>
         </is>
       </c>
       <c r="C199" t="inlineStr">
         <is>
-          <t>Jamaican reggae icon, known for his messages of unity and peace.</t>
+          <t>Norwegian painter, known for "The Scream" and other emotionally charged works.</t>
         </is>
       </c>
       <c r="D199" t="inlineStr">
@@ -9897,7 +9949,7 @@
       <c r="I199" t="inlineStr"/>
       <c r="J199" t="inlineStr">
         <is>
-          <t>Generate 10 pretty long and interesting facts about Bob Marley</t>
+          <t>Please provide me with 10 long and interesting facts about Edvard Munch. I have a youtube channel based on influential figures so this information must be accurate as my channel depends on it. Please make the output of the facts at least 700 words long. Thank you.</t>
         </is>
       </c>
     </row>
@@ -9907,12 +9959,12 @@
       </c>
       <c r="B200" t="inlineStr">
         <is>
-          <t>Noureddine Morceli</t>
+          <t>Hakeem Olajuwon</t>
         </is>
       </c>
       <c r="C200" t="inlineStr">
         <is>
-          <t>Algerian middle-distance runner, Olympic gold medalist.</t>
+          <t>Nigerian-American basketball player, NBA legend.</t>
         </is>
       </c>
       <c r="D200" t="inlineStr">
@@ -9943,7 +9995,7 @@
       <c r="I200" t="inlineStr"/>
       <c r="J200" t="inlineStr">
         <is>
-          <t>Generate 10 pretty long and interesting facts about Noureddine Morceli</t>
+          <t>Please provide me with 10 long and interesting facts about Hakeem Olajuwon. I have a youtube channel based on influential figures so this information must be accurate as my channel depends on it. Please make the output of the facts at least 700 words long. Thank you.</t>
         </is>
       </c>
     </row>
@@ -9953,12 +10005,12 @@
       </c>
       <c r="B201" t="inlineStr">
         <is>
-          <t>Georgia O'Keeffe</t>
+          <t>Harvey Milk</t>
         </is>
       </c>
       <c r="C201" t="inlineStr">
         <is>
-          <t>American painter, known for her large-scale flower paintings.</t>
+          <t>One of the first openly gay elected officials in the United States, he was a leading figure in the gay rights movement.</t>
         </is>
       </c>
       <c r="D201" t="inlineStr">
@@ -9989,7 +10041,7 @@
       <c r="I201" t="inlineStr"/>
       <c r="J201" t="inlineStr">
         <is>
-          <t>Generate 10 pretty long and interesting facts about Georgia O'Keeffe</t>
+          <t>Please provide me with 10 long and interesting facts about Harvey Milk. I have a youtube channel based on influential figures so this information must be accurate as my channel depends on it. Please make the output of the facts at least 700 words long. Thank you.</t>
         </is>
       </c>
     </row>
@@ -9999,12 +10051,12 @@
       </c>
       <c r="B202" t="inlineStr">
         <is>
-          <t>Ho Chi Minh</t>
+          <t>Guru Nanak</t>
         </is>
       </c>
       <c r="C202" t="inlineStr">
         <is>
-          <t>Vietnamese communist revolutionary and President of North Vietnam.</t>
+          <t>Founder of Sikhism in the 15th century, revered as the first Sikh guru and promoting the principles of equality and social justice.</t>
         </is>
       </c>
       <c r="D202" t="inlineStr">
@@ -10035,7 +10087,7 @@
       <c r="I202" t="inlineStr"/>
       <c r="J202" t="inlineStr">
         <is>
-          <t>Generate 10 pretty long and interesting facts about Ho Chi Minh</t>
+          <t>Please provide me with 10 long and interesting facts about Guru Nanak. I have a youtube channel based on influential figures so this information must be accurate as my channel depends on it. Please make the output of the facts at least 700 words long. Thank you.</t>
         </is>
       </c>
     </row>
@@ -10045,12 +10097,12 @@
       </c>
       <c r="B203" t="inlineStr">
         <is>
-          <t>Andy Warhol</t>
+          <t>Ono no Komachi</t>
         </is>
       </c>
       <c r="C203" t="inlineStr">
         <is>
-          <t>American pop art pioneer, known for his iconic portraits and prints.</t>
+          <t>Japanese poet in the 9th century, one of the "Six Immortals of Poetry" known for her lyrical and emotional verses.</t>
         </is>
       </c>
       <c r="D203" t="inlineStr">
@@ -10081,7 +10133,7 @@
       <c r="I203" t="inlineStr"/>
       <c r="J203" t="inlineStr">
         <is>
-          <t>Generate 10 pretty long and interesting facts about Andy Warhol</t>
+          <t>Please provide me with 10 long and interesting facts about Ono no Komachi. I have a youtube channel based on influential figures so this information must be accurate as my channel depends on it. Please make the output of the facts at least 700 words long. Thank you.</t>
         </is>
       </c>
     </row>
@@ -10091,12 +10143,12 @@
       </c>
       <c r="B204" t="inlineStr">
         <is>
-          <t>Henri Matisse</t>
+          <t>Michael Jordan</t>
         </is>
       </c>
       <c r="C204" t="inlineStr">
         <is>
-          <t>French artist, known for his colorful and innovative use of shapes and patterns.</t>
+          <t>American basketball player, NBA legend.</t>
         </is>
       </c>
       <c r="D204" t="inlineStr">
@@ -10127,7 +10179,145 @@
       <c r="I204" t="inlineStr"/>
       <c r="J204" t="inlineStr">
         <is>
-          <t>Generate 10 pretty long and interesting facts about Henri Matisse</t>
+          <t>Please provide me with 10 long and interesting facts about Michael Jordan. I have a youtube channel based on influential figures so this information must be accurate as my channel depends on it. Please make the output of the facts at least 700 words long. Thank you.</t>
+        </is>
+      </c>
+    </row>
+    <row r="205">
+      <c r="A205" t="n">
+        <v>204</v>
+      </c>
+      <c r="B205" t="inlineStr">
+        <is>
+          <t>Greg Lemond</t>
+        </is>
+      </c>
+      <c r="C205" t="inlineStr">
+        <is>
+          <t>American cyclist, three-time Tour de France winner.</t>
+        </is>
+      </c>
+      <c r="D205" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="E205" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="F205" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="G205" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="H205" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="I205" t="inlineStr"/>
+      <c r="J205" t="inlineStr">
+        <is>
+          <t>Please provide me with 10 long and interesting facts about Greg Lemond. I have a youtube channel based on influential figures so this information must be accurate as my channel depends on it. Please make the output of the facts at least 700 words long. Thank you.</t>
+        </is>
+      </c>
+    </row>
+    <row r="206">
+      <c r="A206" t="n">
+        <v>205</v>
+      </c>
+      <c r="B206" t="inlineStr">
+        <is>
+          <t>Bjorn Borg</t>
+        </is>
+      </c>
+      <c r="C206" t="inlineStr">
+        <is>
+          <t>Swedish tennis legend, dominated the tennis world in the late 1970s.</t>
+        </is>
+      </c>
+      <c r="D206" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="E206" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="F206" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="G206" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="H206" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="I206" t="inlineStr"/>
+      <c r="J206" t="inlineStr">
+        <is>
+          <t>Please provide me with 10 long and interesting facts about Bjorn Borg. I have a youtube channel based on influential figures so this information must be accurate as my channel depends on it. Please make the output of the facts at least 700 words long. Thank you.</t>
+        </is>
+      </c>
+    </row>
+    <row r="207">
+      <c r="A207" t="n">
+        <v>206</v>
+      </c>
+      <c r="B207" t="inlineStr">
+        <is>
+          <t>Kwame Nkrumah</t>
+        </is>
+      </c>
+      <c r="C207" t="inlineStr">
+        <is>
+          <t>Pan-Africanist leader and Ghana's first president.</t>
+        </is>
+      </c>
+      <c r="D207" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="E207" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="F207" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="G207" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="H207" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="I207" t="inlineStr"/>
+      <c r="J207" t="inlineStr">
+        <is>
+          <t>Please provide me with 10 long and interesting facts about Kwame Nkrumah. I have a youtube channel based on influential figures so this information must be accurate as my channel depends on it. Please make the output of the facts at least 700 words long. Thank you.</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
Major updates, OpenAI interaction and YouTube API
</commit_message>
<xml_diff>
--- a/Historical Figures List.xlsx
+++ b/Historical Figures List.xlsx
@@ -5037,12 +5037,12 @@
       </c>
       <c r="B93" t="inlineStr">
         <is>
-          <t>Ella Fitzgerald</t>
+          <t>George Orwell</t>
         </is>
       </c>
       <c r="C93" t="inlineStr">
         <is>
-          <t>American jazz singer, known for her pure and versatile voice.</t>
+          <t>American singer, songwriter, and multi-instrumentalist.</t>
         </is>
       </c>
       <c r="D93" t="inlineStr">
@@ -5073,7 +5073,7 @@
       <c r="I93" t="inlineStr"/>
       <c r="J93" t="inlineStr">
         <is>
-          <t>Please provide me with 10 long and interesting facts about Ella Fitzgerald. I have a youtube channel based on influential figures so this information must be accurate as my channel depends on it. Please make the output of the facts at least 700 words long. Thank you.</t>
+          <t>Please provide me with 10 long and interesting facts about George Orwell. I have a youtube channel based on influential figures so this information must be accurate as my channel depends on it. Please make the output of the facts at least 700 words long. Thank you.</t>
         </is>
       </c>
     </row>
@@ -5083,12 +5083,12 @@
       </c>
       <c r="B94" t="inlineStr">
         <is>
-          <t>Charles Dickens</t>
+          <t>Ella Fitzgerald</t>
         </is>
       </c>
       <c r="C94" t="inlineStr">
         <is>
-          <t>One of the most popular novelists of the 19th century, he wrote about the lives of the poor and working class.</t>
+          <t>American jazz singer, known for her pure and versatile voice.</t>
         </is>
       </c>
       <c r="D94" t="inlineStr">
@@ -5119,7 +5119,7 @@
       <c r="I94" t="inlineStr"/>
       <c r="J94" t="inlineStr">
         <is>
-          <t>Please provide me with 10 long and interesting facts about Charles Dickens. I have a youtube channel based on influential figures so this information must be accurate as my channel depends on it. Please make the output of the facts at least 700 words long. Thank you.</t>
+          <t>Please provide me with 10 long and interesting facts about Ella Fitzgerald. I have a youtube channel based on influential figures so this information must be accurate as my channel depends on it. Please make the output of the facts at least 700 words long. Thank you.</t>
         </is>
       </c>
     </row>
@@ -5129,12 +5129,12 @@
       </c>
       <c r="B95" t="inlineStr">
         <is>
-          <t>Elvis Presley</t>
+          <t>Charles Dickens</t>
         </is>
       </c>
       <c r="C95" t="inlineStr">
         <is>
-          <t>American rock 'n' roll legend, the "King of Rock and Roll."</t>
+          <t>One of the most popular novelists of the 19th century, he wrote about the lives of the poor and working class.</t>
         </is>
       </c>
       <c r="D95" t="inlineStr">
@@ -5165,7 +5165,7 @@
       <c r="I95" t="inlineStr"/>
       <c r="J95" t="inlineStr">
         <is>
-          <t>Please provide me with 10 long and interesting facts about Elvis Presley. I have a youtube channel based on influential figures so this information must be accurate as my channel depends on it. Please make the output of the facts at least 700 words long. Thank you.</t>
+          <t>Please provide me with 10 long and interesting facts about Charles Dickens. I have a youtube channel based on influential figures so this information must be accurate as my channel depends on it. Please make the output of the facts at least 700 words long. Thank you.</t>
         </is>
       </c>
     </row>
@@ -5175,12 +5175,12 @@
       </c>
       <c r="B96" t="inlineStr">
         <is>
-          <t>Salvador Dali</t>
+          <t>Elvis Presley</t>
         </is>
       </c>
       <c r="C96" t="inlineStr">
         <is>
-          <t>Spanish Surrealist artist, known for his bizarre and dreamlike imagery.</t>
+          <t>American rock 'n' roll legend, the "King of Rock and Roll."</t>
         </is>
       </c>
       <c r="D96" t="inlineStr">
@@ -5211,7 +5211,7 @@
       <c r="I96" t="inlineStr"/>
       <c r="J96" t="inlineStr">
         <is>
-          <t>Please provide me with 10 long and interesting facts about Salvador Dali. I have a youtube channel based on influential figures so this information must be accurate as my channel depends on it. Please make the output of the facts at least 700 words long. Thank you.</t>
+          <t>Please provide me with 10 long and interesting facts about Elvis Presley. I have a youtube channel based on influential figures so this information must be accurate as my channel depends on it. Please make the output of the facts at least 700 words long. Thank you.</t>
         </is>
       </c>
     </row>
@@ -5221,12 +5221,12 @@
       </c>
       <c r="B97" t="inlineStr">
         <is>
-          <t>Jay-Jay Okocha</t>
+          <t>Salvador Dali</t>
         </is>
       </c>
       <c r="C97" t="inlineStr">
         <is>
-          <t>Nigerian footballer, known for his flair and creativity.</t>
+          <t>Spanish Surrealist artist, known for his bizarre and dreamlike imagery.</t>
         </is>
       </c>
       <c r="D97" t="inlineStr">
@@ -5257,7 +5257,7 @@
       <c r="I97" t="inlineStr"/>
       <c r="J97" t="inlineStr">
         <is>
-          <t>Please provide me with 10 long and interesting facts about Jay-Jay Okocha. I have a youtube channel based on influential figures so this information must be accurate as my channel depends on it. Please make the output of the facts at least 700 words long. Thank you.</t>
+          <t>Please provide me with 10 long and interesting facts about Salvador Dali. I have a youtube channel based on influential figures so this information must be accurate as my channel depends on it. Please make the output of the facts at least 700 words long. Thank you.</t>
         </is>
       </c>
     </row>
@@ -5267,12 +5267,12 @@
       </c>
       <c r="B98" t="inlineStr">
         <is>
-          <t>Nadia Comaneci</t>
+          <t>Jay-Jay Okocha</t>
         </is>
       </c>
       <c r="C98" t="inlineStr">
         <is>
-          <t>Romanian gymnast, first to score a perfect 10 in Olympic gymnastics.</t>
+          <t>Nigerian footballer, known for his flair and creativity.</t>
         </is>
       </c>
       <c r="D98" t="inlineStr">
@@ -5303,7 +5303,7 @@
       <c r="I98" t="inlineStr"/>
       <c r="J98" t="inlineStr">
         <is>
-          <t>Please provide me with 10 long and interesting facts about Nadia Comaneci. I have a youtube channel based on influential figures so this information must be accurate as my channel depends on it. Please make the output of the facts at least 700 words long. Thank you.</t>
+          <t>Please provide me with 10 long and interesting facts about Jay-Jay Okocha. I have a youtube channel based on influential figures so this information must be accurate as my channel depends on it. Please make the output of the facts at least 700 words long. Thank you.</t>
         </is>
       </c>
     </row>
@@ -5313,12 +5313,12 @@
       </c>
       <c r="B99" t="inlineStr">
         <is>
-          <t>Mansa Musa</t>
+          <t>Nadia Comaneci</t>
         </is>
       </c>
       <c r="C99" t="inlineStr">
         <is>
-          <t>Mali's wealthiest ruler, a great patron of art and education.</t>
+          <t>Romanian gymnast, first to score a perfect 10 in Olympic gymnastics.</t>
         </is>
       </c>
       <c r="D99" t="inlineStr">
@@ -5333,23 +5333,23 @@
       </c>
       <c r="F99" t="inlineStr">
         <is>
-          <t>No</t>
+          <t>Yes</t>
         </is>
       </c>
       <c r="G99" t="inlineStr">
         <is>
-          <t>No</t>
+          <t>Yes</t>
         </is>
       </c>
       <c r="H99" t="inlineStr">
         <is>
-          <t>No</t>
+          <t>Yes</t>
         </is>
       </c>
       <c r="I99" t="inlineStr"/>
       <c r="J99" t="inlineStr">
         <is>
-          <t>Please provide me with 10 long and interesting facts about Mansa Musa. I have a youtube channel based on influential figures so this information must be accurate as my channel depends on it. Please make the output of the facts at least 700 words long. Thank you.</t>
+          <t>Please provide me with 10 long and interesting facts about Nadia Comaneci. I have a youtube channel based on influential figures so this information must be accurate as my channel depends on it. Please make the output of the facts at least 700 words long. Thank you.</t>
         </is>
       </c>
     </row>
@@ -5359,12 +5359,12 @@
       </c>
       <c r="B100" t="inlineStr">
         <is>
-          <t>Hypatia of Alexandria</t>
+          <t>Banksy</t>
         </is>
       </c>
       <c r="C100" t="inlineStr">
         <is>
-          <t>Greek mathematician, astronomer, and philosopher in the 4th century CE, known for her contributions to mathematics and astronomy.</t>
+          <t>Romanian gymnast, first to score a perfect 10 in Olympic gymnastics.</t>
         </is>
       </c>
       <c r="D100" t="inlineStr">
@@ -5379,12 +5379,12 @@
       </c>
       <c r="F100" t="inlineStr">
         <is>
-          <t>No</t>
+          <t>Yes</t>
         </is>
       </c>
       <c r="G100" t="inlineStr">
         <is>
-          <t>No</t>
+          <t>Yes</t>
         </is>
       </c>
       <c r="H100" t="inlineStr">
@@ -5395,7 +5395,7 @@
       <c r="I100" t="inlineStr"/>
       <c r="J100" t="inlineStr">
         <is>
-          <t>Please provide me with 10 long and interesting facts about Hypatia of Alexandria. I have a youtube channel based on influential figures so this information must be accurate as my channel depends on it. Please make the output of the facts at least 700 words long. Thank you.</t>
+          <t>Please provide me with 10 long and interesting facts about Banksy. I have a youtube channel based on influential figures so this information must be accurate as my channel depends on it. Please make the output of the facts at least 700 words long. Thank you.</t>
         </is>
       </c>
     </row>
@@ -5405,12 +5405,12 @@
       </c>
       <c r="B101" t="inlineStr">
         <is>
-          <t>Bob Dylan</t>
+          <t>Diego Maradona</t>
         </is>
       </c>
       <c r="C101" t="inlineStr">
         <is>
-          <t>American singer-songwriter, Nobel laureate for literature.</t>
+          <t>Argentine football legend, known for his "Hand of God" goal.</t>
         </is>
       </c>
       <c r="D101" t="inlineStr">
@@ -5441,7 +5441,7 @@
       <c r="I101" t="inlineStr"/>
       <c r="J101" t="inlineStr">
         <is>
-          <t>Please provide me with 10 long and interesting facts about Bob Dylan. I have a youtube channel based on influential figures so this information must be accurate as my channel depends on it. Please make the output of the facts at least 700 words long. Thank you.</t>
+          <t>Please provide me with 10 long and interesting facts about Diego Maradona. I have a youtube channel based on influential figures so this information must be accurate as my channel depends on it. Please make the output of the facts at least 700 words long. Thank you.</t>
         </is>
       </c>
     </row>
@@ -5451,12 +5451,12 @@
       </c>
       <c r="B102" t="inlineStr">
         <is>
-          <t>Enheduanna</t>
+          <t>Aretha Franklin</t>
         </is>
       </c>
       <c r="C102" t="inlineStr">
         <is>
-          <t>High priestess of the moon god Nanna in ancient Sumer, credited as one of the earliest known authors and poets in history.</t>
+          <t>American singer and "Queen of Soul."</t>
         </is>
       </c>
       <c r="D102" t="inlineStr">
@@ -5487,7 +5487,7 @@
       <c r="I102" t="inlineStr"/>
       <c r="J102" t="inlineStr">
         <is>
-          <t>Please provide me with 10 long and interesting facts about Enheduanna. I have a youtube channel based on influential figures so this information must be accurate as my channel depends on it. Please make the output of the facts at least 700 words long. Thank you.</t>
+          <t>Please provide me with 10 long and interesting facts about Aretha Franklin. I have a youtube channel based on influential figures so this information must be accurate as my channel depends on it. Please make the output of the facts at least 700 words long. Thank you.</t>
         </is>
       </c>
     </row>
@@ -5497,12 +5497,12 @@
       </c>
       <c r="B103" t="inlineStr">
         <is>
-          <t>Antonio Vivaldi</t>
+          <t>Henri Cartier-Bresson</t>
         </is>
       </c>
       <c r="C103" t="inlineStr">
         <is>
-          <t>Italian composer, famous for "The Four Seasons."</t>
+          <t>French photographer, considered the father of modern photojournalism.</t>
         </is>
       </c>
       <c r="D103" t="inlineStr">
@@ -5533,7 +5533,7 @@
       <c r="I103" t="inlineStr"/>
       <c r="J103" t="inlineStr">
         <is>
-          <t>Please provide me with 10 long and interesting facts about Antonio Vivaldi. I have a youtube channel based on influential figures so this information must be accurate as my channel depends on it. Please make the output of the facts at least 700 words long. Thank you.</t>
+          <t>Please provide me with 10 long and interesting facts about Henri Cartier-Bresson. I have a youtube channel based on influential figures so this information must be accurate as my channel depends on it. Please make the output of the facts at least 700 words long. Thank you.</t>
         </is>
       </c>
     </row>
@@ -5543,12 +5543,12 @@
       </c>
       <c r="B104" t="inlineStr">
         <is>
-          <t>Frantz Fanon</t>
+          <t>Ibn Battuta</t>
         </is>
       </c>
       <c r="C104" t="inlineStr">
         <is>
-          <t>Philosopher, revolutionary, and anti-colonial theorist.</t>
+          <t>Moroccan explorer and scholar who embarked on extensive travels throughout the Islamic world, chronicling his journeys in his renowned travelogue.</t>
         </is>
       </c>
       <c r="D104" t="inlineStr">
@@ -5579,7 +5579,7 @@
       <c r="I104" t="inlineStr"/>
       <c r="J104" t="inlineStr">
         <is>
-          <t>Please provide me with 10 long and interesting facts about Frantz Fanon. I have a youtube channel based on influential figures so this information must be accurate as my channel depends on it. Please make the output of the facts at least 700 words long. Thank you.</t>
+          <t>Please provide me with 10 long and interesting facts about Ibn Battuta. I have a youtube channel based on influential figures so this information must be accurate as my channel depends on it. Please make the output of the facts at least 700 words long. Thank you.</t>
         </is>
       </c>
     </row>
@@ -5589,12 +5589,12 @@
       </c>
       <c r="B105" t="inlineStr">
         <is>
-          <t>Benito Mussolini</t>
+          <t>Daenerys Targaryen</t>
         </is>
       </c>
       <c r="C105" t="inlineStr">
         <is>
-          <t>Italian fascist dictator during the 1920s and 1930s.</t>
+          <t>A fictional character in the "Game of Thrones" series, she is a powerful and inspiring leader.</t>
         </is>
       </c>
       <c r="D105" t="inlineStr">
@@ -5625,7 +5625,7 @@
       <c r="I105" t="inlineStr"/>
       <c r="J105" t="inlineStr">
         <is>
-          <t>Please provide me with 10 long and interesting facts about Benito Mussolini. I have a youtube channel based on influential figures so this information must be accurate as my channel depends on it. Please make the output of the facts at least 700 words long. Thank you.</t>
+          <t>Please provide me with 10 long and interesting facts about Daenerys Targaryen. I have a youtube channel based on influential figures so this information must be accurate as my channel depends on it. Please make the output of the facts at least 700 words long. Thank you.</t>
         </is>
       </c>
     </row>
@@ -5635,12 +5635,12 @@
       </c>
       <c r="B106" t="inlineStr">
         <is>
-          <t>Susan B. Anthony</t>
+          <t>Noureddine Morceli</t>
         </is>
       </c>
       <c r="C106" t="inlineStr">
         <is>
-          <t>Fought for women's suffrage and other women's rights.</t>
+          <t>Algerian middle-distance runner, Olympic gold medalist.</t>
         </is>
       </c>
       <c r="D106" t="inlineStr">
@@ -5671,7 +5671,7 @@
       <c r="I106" t="inlineStr"/>
       <c r="J106" t="inlineStr">
         <is>
-          <t>Please provide me with 10 long and interesting facts about Susan B. Anthony. I have a youtube channel based on influential figures so this information must be accurate as my channel depends on it. Please make the output of the facts at least 700 words long. Thank you.</t>
+          <t>Please provide me with 10 long and interesting facts about Noureddine Morceli. I have a youtube channel based on influential figures so this information must be accurate as my channel depends on it. Please make the output of the facts at least 700 words long. Thank you.</t>
         </is>
       </c>
     </row>
@@ -5681,12 +5681,12 @@
       </c>
       <c r="B107" t="inlineStr">
         <is>
-          <t>Franklin D. Roosevelt</t>
+          <t>Kwame Nkrumah</t>
         </is>
       </c>
       <c r="C107" t="inlineStr">
         <is>
-          <t>32nd President of the United States, led the nation through the Great Depression and World War II.</t>
+          <t>Pan-Africanist leader and Ghana's first president.</t>
         </is>
       </c>
       <c r="D107" t="inlineStr">
@@ -5717,7 +5717,7 @@
       <c r="I107" t="inlineStr"/>
       <c r="J107" t="inlineStr">
         <is>
-          <t>Please provide me with 10 long and interesting facts about Franklin D. Roosevelt. I have a youtube channel based on influential figures so this information must be accurate as my channel depends on it. Please make the output of the facts at least 700 words long. Thank you.</t>
+          <t>Please provide me with 10 long and interesting facts about Kwame Nkrumah. I have a youtube channel based on influential figures so this information must be accurate as my channel depends on it. Please make the output of the facts at least 700 words long. Thank you.</t>
         </is>
       </c>
     </row>
@@ -5727,12 +5727,12 @@
       </c>
       <c r="B108" t="inlineStr">
         <is>
-          <t>Qutb-ud-din Aybak</t>
+          <t>Claude Monet</t>
         </is>
       </c>
       <c r="C108" t="inlineStr">
         <is>
-          <t>Slave-turned-sultan who founded the Delhi Sultanate in medieval India, establishing the Mamluk dynasty and ruling over a vast empire.</t>
+          <t>French Impressionist painter, famous for his "Water Lilies" series.</t>
         </is>
       </c>
       <c r="D108" t="inlineStr">
@@ -5763,7 +5763,7 @@
       <c r="I108" t="inlineStr"/>
       <c r="J108" t="inlineStr">
         <is>
-          <t>Please provide me with 10 long and interesting facts about Qutb-ud-din Aybak. I have a youtube channel based on influential figures so this information must be accurate as my channel depends on it. Please make the output of the facts at least 700 words long. Thank you.</t>
+          <t>Please provide me with 10 long and interesting facts about Claude Monet. I have a youtube channel based on influential figures so this information must be accurate as my channel depends on it. Please make the output of the facts at least 700 words long. Thank you.</t>
         </is>
       </c>
     </row>
@@ -5773,12 +5773,12 @@
       </c>
       <c r="B109" t="inlineStr">
         <is>
-          <t>Aretha Franklin</t>
+          <t>Frantz Fanon</t>
         </is>
       </c>
       <c r="C109" t="inlineStr">
         <is>
-          <t>American singer and "Queen of Soul."</t>
+          <t>Philosopher, revolutionary, and anti-colonial theorist.</t>
         </is>
       </c>
       <c r="D109" t="inlineStr">
@@ -5809,7 +5809,7 @@
       <c r="I109" t="inlineStr"/>
       <c r="J109" t="inlineStr">
         <is>
-          <t>Please provide me with 10 long and interesting facts about Aretha Franklin. I have a youtube channel based on influential figures so this information must be accurate as my channel depends on it. Please make the output of the facts at least 700 words long. Thank you.</t>
+          <t>Please provide me with 10 long and interesting facts about Frantz Fanon. I have a youtube channel based on influential figures so this information must be accurate as my channel depends on it. Please make the output of the facts at least 700 words long. Thank you.</t>
         </is>
       </c>
     </row>
@@ -5819,12 +5819,12 @@
       </c>
       <c r="B110" t="inlineStr">
         <is>
-          <t>Miriam Makeba</t>
+          <t>Andy Warhol</t>
         </is>
       </c>
       <c r="C110" t="inlineStr">
         <is>
-          <t>South African singer and civil rights activist.</t>
+          <t>American pop art pioneer, known for his iconic portraits and prints.</t>
         </is>
       </c>
       <c r="D110" t="inlineStr">
@@ -5855,7 +5855,7 @@
       <c r="I110" t="inlineStr"/>
       <c r="J110" t="inlineStr">
         <is>
-          <t>Please provide me with 10 long and interesting facts about Miriam Makeba. I have a youtube channel based on influential figures so this information must be accurate as my channel depends on it. Please make the output of the facts at least 700 words long. Thank you.</t>
+          <t>Please provide me with 10 long and interesting facts about Andy Warhol. I have a youtube channel based on influential figures so this information must be accurate as my channel depends on it. Please make the output of the facts at least 700 words long. Thank you.</t>
         </is>
       </c>
     </row>
@@ -5911,12 +5911,12 @@
       </c>
       <c r="B112" t="inlineStr">
         <is>
-          <t>Banksy</t>
+          <t>Theodore Roosevelt</t>
         </is>
       </c>
       <c r="C112" t="inlineStr">
         <is>
-          <t>Anonymous British street artist, famous for his politically charged graffiti art.</t>
+          <t>26th President of the United States, he was a leading advocate for environmental protection.</t>
         </is>
       </c>
       <c r="D112" t="inlineStr">
@@ -5947,7 +5947,7 @@
       <c r="I112" t="inlineStr"/>
       <c r="J112" t="inlineStr">
         <is>
-          <t>Please provide me with 10 long and interesting facts about Banksy. I have a youtube channel based on influential figures so this information must be accurate as my channel depends on it. Please make the output of the facts at least 700 words long. Thank you.</t>
+          <t>Please provide me with 10 long and interesting facts about Theodore Roosevelt. I have a youtube channel based on influential figures so this information must be accurate as my channel depends on it. Please make the output of the facts at least 700 words long. Thank you.</t>
         </is>
       </c>
     </row>
@@ -5957,12 +5957,12 @@
       </c>
       <c r="B113" t="inlineStr">
         <is>
-          <t>Yaa Asantewaa</t>
+          <t>Hypatia of Alexandria</t>
         </is>
       </c>
       <c r="C113" t="inlineStr">
         <is>
-          <t>Ashanti queen mother, led an anti-colonial rebellion.</t>
+          <t>Greek mathematician, astronomer, and philosopher in the 4th century CE, known for her contributions to mathematics and astronomy.</t>
         </is>
       </c>
       <c r="D113" t="inlineStr">
@@ -5993,7 +5993,7 @@
       <c r="I113" t="inlineStr"/>
       <c r="J113" t="inlineStr">
         <is>
-          <t>Please provide me with 10 long and interesting facts about Yaa Asantewaa. I have a youtube channel based on influential figures so this information must be accurate as my channel depends on it. Please make the output of the facts at least 700 words long. Thank you.</t>
+          <t>Please provide me with 10 long and interesting facts about Hypatia of Alexandria. I have a youtube channel based on influential figures so this information must be accurate as my channel depends on it. Please make the output of the facts at least 700 words long. Thank you.</t>
         </is>
       </c>
     </row>
@@ -6003,12 +6003,12 @@
       </c>
       <c r="B114" t="inlineStr">
         <is>
-          <t>Seondeok of Silla</t>
+          <t>Oprah Winfrey</t>
         </is>
       </c>
       <c r="C114" t="inlineStr">
         <is>
-          <t>Queen of the Silla Kingdom in ancient Korea during the 7th century CE, remembered for her strong leadership and advancements in science and culture.</t>
+          <t>One of the most successful talk show hosts of all time, she is also a successful actress and producer.</t>
         </is>
       </c>
       <c r="D114" t="inlineStr">
@@ -6039,7 +6039,7 @@
       <c r="I114" t="inlineStr"/>
       <c r="J114" t="inlineStr">
         <is>
-          <t>Please provide me with 10 long and interesting facts about Seondeok of Silla. I have a youtube channel based on influential figures so this information must be accurate as my channel depends on it. Please make the output of the facts at least 700 words long. Thank you.</t>
+          <t>Please provide me with 10 long and interesting facts about Oprah Winfrey. I have a youtube channel based on influential figures so this information must be accurate as my channel depends on it. Please make the output of the facts at least 700 words long. Thank you.</t>
         </is>
       </c>
     </row>
@@ -6049,12 +6049,12 @@
       </c>
       <c r="B115" t="inlineStr">
         <is>
-          <t>Oprah Winfrey</t>
+          <t>Kofi Annan</t>
         </is>
       </c>
       <c r="C115" t="inlineStr">
         <is>
-          <t>One of the most successful talk show hosts of all time, she is also a successful actress and producer.</t>
+          <t>Ghanaian diplomat, UN Secretary-General, Nobel laureate.</t>
         </is>
       </c>
       <c r="D115" t="inlineStr">
@@ -6085,7 +6085,7 @@
       <c r="I115" t="inlineStr"/>
       <c r="J115" t="inlineStr">
         <is>
-          <t>Please provide me with 10 long and interesting facts about Oprah Winfrey. I have a youtube channel based on influential figures so this information must be accurate as my channel depends on it. Please make the output of the facts at least 700 words long. Thank you.</t>
+          <t>Please provide me with 10 long and interesting facts about Kofi Annan. I have a youtube channel based on influential figures so this information must be accurate as my channel depends on it. Please make the output of the facts at least 700 words long. Thank you.</t>
         </is>
       </c>
     </row>
@@ -6095,12 +6095,12 @@
       </c>
       <c r="B116" t="inlineStr">
         <is>
-          <t>David Bowie</t>
+          <t>Bjorn Borg</t>
         </is>
       </c>
       <c r="C116" t="inlineStr">
         <is>
-          <t>British singer and musician, known for his innovation and artistic style.</t>
+          <t>Swedish tennis legend, dominated the tennis world in the late 1970s.</t>
         </is>
       </c>
       <c r="D116" t="inlineStr">
@@ -6131,7 +6131,7 @@
       <c r="I116" t="inlineStr"/>
       <c r="J116" t="inlineStr">
         <is>
-          <t>Please provide me with 10 long and interesting facts about David Bowie. I have a youtube channel based on influential figures so this information must be accurate as my channel depends on it. Please make the output of the facts at least 700 words long. Thank you.</t>
+          <t>Please provide me with 10 long and interesting facts about Bjorn Borg. I have a youtube channel based on influential figures so this information must be accurate as my channel depends on it. Please make the output of the facts at least 700 words long. Thank you.</t>
         </is>
       </c>
     </row>
@@ -6141,12 +6141,12 @@
       </c>
       <c r="B117" t="inlineStr">
         <is>
-          <t>Diego Maradona</t>
+          <t>Edvard Munch</t>
         </is>
       </c>
       <c r="C117" t="inlineStr">
         <is>
-          <t>Argentine football legend, known for his "Hand of God" goal.</t>
+          <t>Norwegian painter, known for "The Scream" and other emotionally charged works.</t>
         </is>
       </c>
       <c r="D117" t="inlineStr">
@@ -6177,7 +6177,7 @@
       <c r="I117" t="inlineStr"/>
       <c r="J117" t="inlineStr">
         <is>
-          <t>Please provide me with 10 long and interesting facts about Diego Maradona. I have a youtube channel based on influential figures so this information must be accurate as my channel depends on it. Please make the output of the facts at least 700 words long. Thank you.</t>
+          <t>Please provide me with 10 long and interesting facts about Edvard Munch. I have a youtube channel based on influential figures so this information must be accurate as my channel depends on it. Please make the output of the facts at least 700 words long. Thank you.</t>
         </is>
       </c>
     </row>
@@ -6187,12 +6187,12 @@
       </c>
       <c r="B118" t="inlineStr">
         <is>
-          <t>Queen Nzinga</t>
+          <t>Rani Padmini</t>
         </is>
       </c>
       <c r="C118" t="inlineStr">
         <is>
-          <t>Queen of Ndongo and Matamba, skilled diplomat.</t>
+          <t>Queen of Mewar in medieval India, renowned for her beauty and bravery during the siege of Chittorgarh by Alauddin Khilji.</t>
         </is>
       </c>
       <c r="D118" t="inlineStr">
@@ -6223,7 +6223,7 @@
       <c r="I118" t="inlineStr"/>
       <c r="J118" t="inlineStr">
         <is>
-          <t>Please provide me with 10 long and interesting facts about Queen Nzinga. I have a youtube channel based on influential figures so this information must be accurate as my channel depends on it. Please make the output of the facts at least 700 words long. Thank you.</t>
+          <t>Please provide me with 10 long and interesting facts about Rani Padmini. I have a youtube channel based on influential figures so this information must be accurate as my channel depends on it. Please make the output of the facts at least 700 words long. Thank you.</t>
         </is>
       </c>
     </row>
@@ -6233,12 +6233,12 @@
       </c>
       <c r="B119" t="inlineStr">
         <is>
-          <t>Kipchoge Keino</t>
+          <t>Samuel Eto'o</t>
         </is>
       </c>
       <c r="C119" t="inlineStr">
         <is>
-          <t>Kenyan middle-distance runner, Olympic gold medalist.</t>
+          <t>Cameroonian footballer and African legend.</t>
         </is>
       </c>
       <c r="D119" t="inlineStr">
@@ -6269,7 +6269,7 @@
       <c r="I119" t="inlineStr"/>
       <c r="J119" t="inlineStr">
         <is>
-          <t>Please provide me with 10 long and interesting facts about Kipchoge Keino. I have a youtube channel based on influential figures so this information must be accurate as my channel depends on it. Please make the output of the facts at least 700 words long. Thank you.</t>
+          <t>Please provide me with 10 long and interesting facts about Samuel Eto'o. I have a youtube channel based on influential figures so this information must be accurate as my channel depends on it. Please make the output of the facts at least 700 words long. Thank you.</t>
         </is>
       </c>
     </row>
@@ -6279,12 +6279,12 @@
       </c>
       <c r="B120" t="inlineStr">
         <is>
-          <t>Al-Khansa</t>
+          <t>Bob Dylan</t>
         </is>
       </c>
       <c r="C120" t="inlineStr">
         <is>
-          <t>Arabic poetess in the 7th century CE, recognized for her elegies and poems commemorating fallen warriors.</t>
+          <t>American singer-songwriter, Nobel laureate for literature.</t>
         </is>
       </c>
       <c r="D120" t="inlineStr">
@@ -6315,7 +6315,7 @@
       <c r="I120" t="inlineStr"/>
       <c r="J120" t="inlineStr">
         <is>
-          <t>Please provide me with 10 long and interesting facts about Al-Khansa. I have a youtube channel based on influential figures so this information must be accurate as my channel depends on it. Please make the output of the facts at least 700 words long. Thank you.</t>
+          <t>Please provide me with 10 long and interesting facts about Bob Dylan. I have a youtube channel based on influential figures so this information must be accurate as my channel depends on it. Please make the output of the facts at least 700 words long. Thank you.</t>
         </is>
       </c>
     </row>
@@ -6325,12 +6325,12 @@
       </c>
       <c r="B121" t="inlineStr">
         <is>
-          <t>Pele</t>
+          <t>Funmilayo Ransome-Kuti</t>
         </is>
       </c>
       <c r="C121" t="inlineStr">
         <is>
-          <t>Brazilian football legend, three-time World Cup winner.</t>
+          <t>Nigerian women's rights advocate and activist.</t>
         </is>
       </c>
       <c r="D121" t="inlineStr">
@@ -6361,7 +6361,7 @@
       <c r="I121" t="inlineStr"/>
       <c r="J121" t="inlineStr">
         <is>
-          <t>Please provide me with 10 long and interesting facts about Pele. I have a youtube channel based on influential figures so this information must be accurate as my channel depends on it. Please make the output of the facts at least 700 words long. Thank you.</t>
+          <t>Please provide me with 10 long and interesting facts about Funmilayo Ransome-Kuti. I have a youtube channel based on influential figures so this information must be accurate as my channel depends on it. Please make the output of the facts at least 700 words long. Thank you.</t>
         </is>
       </c>
     </row>
@@ -6371,12 +6371,12 @@
       </c>
       <c r="B122" t="inlineStr">
         <is>
-          <t>George Orwell</t>
+          <t>Martina Hingis</t>
         </is>
       </c>
       <c r="C122" t="inlineStr">
         <is>
-          <t>One of the most important writers of the 20th century, he wrote about the dangers of totalitarianism.</t>
+          <t>Swiss tennis player, former world No. 1 and multiple Grand Slam winner.</t>
         </is>
       </c>
       <c r="D122" t="inlineStr">
@@ -6407,7 +6407,7 @@
       <c r="I122" t="inlineStr"/>
       <c r="J122" t="inlineStr">
         <is>
-          <t>Please provide me with 10 long and interesting facts about George Orwell. I have a youtube channel based on influential figures so this information must be accurate as my channel depends on it. Please make the output of the facts at least 700 words long. Thank you.</t>
+          <t>Please provide me with 10 long and interesting facts about Martina Hingis. I have a youtube channel based on influential figures so this information must be accurate as my channel depends on it. Please make the output of the facts at least 700 words long. Thank you.</t>
         </is>
       </c>
     </row>
@@ -6417,12 +6417,12 @@
       </c>
       <c r="B123" t="inlineStr">
         <is>
-          <t>Khutulun</t>
+          <t>Pele</t>
         </is>
       </c>
       <c r="C123" t="inlineStr">
         <is>
-          <t>Mongol princess and skilled warrior in the 13th century, renowned for her wrestling abilities and her requirement that potential suitors defeat her in combat.</t>
+          <t>Brazilian football legend, three-time World Cup winner.</t>
         </is>
       </c>
       <c r="D123" t="inlineStr">
@@ -6453,7 +6453,7 @@
       <c r="I123" t="inlineStr"/>
       <c r="J123" t="inlineStr">
         <is>
-          <t>Please provide me with 10 long and interesting facts about Khutulun. I have a youtube channel based on influential figures so this information must be accurate as my channel depends on it. Please make the output of the facts at least 700 words long. Thank you.</t>
+          <t>Please provide me with 10 long and interesting facts about Pele. I have a youtube channel based on influential figures so this information must be accurate as my channel depends on it. Please make the output of the facts at least 700 words long. Thank you.</t>
         </is>
       </c>
     </row>
@@ -6463,12 +6463,12 @@
       </c>
       <c r="B124" t="inlineStr">
         <is>
-          <t>Voltaire</t>
+          <t>Jawaharlal Nehru</t>
         </is>
       </c>
       <c r="C124" t="inlineStr">
         <is>
-          <t>One of the most important Enlightenment thinkers, he was a leading advocate for freedom of speech and religious tolerance.</t>
+          <t>Indian independence leader and the first Prime Minister of India.</t>
         </is>
       </c>
       <c r="D124" t="inlineStr">
@@ -6499,7 +6499,7 @@
       <c r="I124" t="inlineStr"/>
       <c r="J124" t="inlineStr">
         <is>
-          <t>Please provide me with 10 long and interesting facts about Voltaire. I have a youtube channel based on influential figures so this information must be accurate as my channel depends on it. Please make the output of the facts at least 700 words long. Thank you.</t>
+          <t>Please provide me with 10 long and interesting facts about Jawaharlal Nehru. I have a youtube channel based on influential figures so this information must be accurate as my channel depends on it. Please make the output of the facts at least 700 words long. Thank you.</t>
         </is>
       </c>
     </row>
@@ -6509,12 +6509,12 @@
       </c>
       <c r="B125" t="inlineStr">
         <is>
-          <t>Ching Shih</t>
+          <t>Jomo Kenyatta</t>
         </is>
       </c>
       <c r="C125" t="inlineStr">
         <is>
-          <t>Chinese pirate leader during the early 19th century, who commanded a vast fleet and became one of the most successful pirates in history.</t>
+          <t>Founding father and first president of Kenya.</t>
         </is>
       </c>
       <c r="D125" t="inlineStr">
@@ -6545,7 +6545,7 @@
       <c r="I125" t="inlineStr"/>
       <c r="J125" t="inlineStr">
         <is>
-          <t>Please provide me with 10 long and interesting facts about Ching Shih. I have a youtube channel based on influential figures so this information must be accurate as my channel depends on it. Please make the output of the facts at least 700 words long. Thank you.</t>
+          <t>Please provide me with 10 long and interesting facts about Jomo Kenyatta. I have a youtube channel based on influential figures so this information must be accurate as my channel depends on it. Please make the output of the facts at least 700 words long. Thank you.</t>
         </is>
       </c>
     </row>
@@ -6555,12 +6555,12 @@
       </c>
       <c r="B126" t="inlineStr">
         <is>
-          <t>Michelangelo</t>
+          <t>Harvey Milk</t>
         </is>
       </c>
       <c r="C126" t="inlineStr">
         <is>
-          <t>Italian sculptor, painter, and architect, known for works like the Sistine Chapel ceiling.</t>
+          <t>One of the first openly gay elected officials in the United States, he was a leading figure in the gay rights movement.</t>
         </is>
       </c>
       <c r="D126" t="inlineStr">
@@ -6591,7 +6591,7 @@
       <c r="I126" t="inlineStr"/>
       <c r="J126" t="inlineStr">
         <is>
-          <t>Please provide me with 10 long and interesting facts about Michelangelo. I have a youtube channel based on influential figures so this information must be accurate as my channel depends on it. Please make the output of the facts at least 700 words long. Thank you.</t>
+          <t>Please provide me with 10 long and interesting facts about Harvey Milk. I have a youtube channel based on influential figures so this information must be accurate as my channel depends on it. Please make the output of the facts at least 700 words long. Thank you.</t>
         </is>
       </c>
     </row>
@@ -6601,12 +6601,12 @@
       </c>
       <c r="B127" t="inlineStr">
         <is>
-          <t>Samuel Eto'o</t>
+          <t>Voltaire</t>
         </is>
       </c>
       <c r="C127" t="inlineStr">
         <is>
-          <t>Cameroonian footballer and African legend.</t>
+          <t>One of the most important Enlightenment thinkers, he was a leading advocate for freedom of speech and religious tolerance.</t>
         </is>
       </c>
       <c r="D127" t="inlineStr">
@@ -6637,7 +6637,7 @@
       <c r="I127" t="inlineStr"/>
       <c r="J127" t="inlineStr">
         <is>
-          <t>Please provide me with 10 long and interesting facts about Samuel Eto'o. I have a youtube channel based on influential figures so this information must be accurate as my channel depends on it. Please make the output of the facts at least 700 words long. Thank you.</t>
+          <t>Please provide me with 10 long and interesting facts about Voltaire. I have a youtube channel based on influential figures so this information must be accurate as my channel depends on it. Please make the output of the facts at least 700 words long. Thank you.</t>
         </is>
       </c>
     </row>
@@ -6647,12 +6647,12 @@
       </c>
       <c r="B128" t="inlineStr">
         <is>
-          <t>George Best</t>
+          <t>Queen Makeda (Queen of Sheba)</t>
         </is>
       </c>
       <c r="C128" t="inlineStr">
         <is>
-          <t>Northern Irish footballer, known for his incredible skill.</t>
+          <t>Legendary queen who visited King Solomon.</t>
         </is>
       </c>
       <c r="D128" t="inlineStr">
@@ -6683,7 +6683,7 @@
       <c r="I128" t="inlineStr"/>
       <c r="J128" t="inlineStr">
         <is>
-          <t>Please provide me with 10 long and interesting facts about George Best. I have a youtube channel based on influential figures so this information must be accurate as my channel depends on it. Please make the output of the facts at least 700 words long. Thank you.</t>
+          <t>Please provide me with 10 long and interesting facts about Queen Makeda (Queen of Sheba). I have a youtube channel based on influential figures so this information must be accurate as my channel depends on it. Please make the output of the facts at least 700 words long. Thank you.</t>
         </is>
       </c>
     </row>
@@ -6693,12 +6693,12 @@
       </c>
       <c r="B129" t="inlineStr">
         <is>
-          <t>Claude Monet</t>
+          <t>Ayrton Senna</t>
         </is>
       </c>
       <c r="C129" t="inlineStr">
         <is>
-          <t>French Impressionist painter, famous for his "Water Lilies" series.</t>
+          <t>Brazilian racing driver, considered one of the greatest Formula 1 drivers.</t>
         </is>
       </c>
       <c r="D129" t="inlineStr">
@@ -6729,7 +6729,7 @@
       <c r="I129" t="inlineStr"/>
       <c r="J129" t="inlineStr">
         <is>
-          <t>Please provide me with 10 long and interesting facts about Claude Monet. I have a youtube channel based on influential figures so this information must be accurate as my channel depends on it. Please make the output of the facts at least 700 words long. Thank you.</t>
+          <t>Please provide me with 10 long and interesting facts about Ayrton Senna. I have a youtube channel based on influential figures so this information must be accurate as my channel depends on it. Please make the output of the facts at least 700 words long. Thank you.</t>
         </is>
       </c>
     </row>
@@ -6739,12 +6739,12 @@
       </c>
       <c r="B130" t="inlineStr">
         <is>
-          <t>Theodore Roosevelt</t>
+          <t>Frank Sinatra</t>
         </is>
       </c>
       <c r="C130" t="inlineStr">
         <is>
-          <t>26th President of the United States, he was a leading advocate for environmental protection.</t>
+          <t>American singer and actor, known for his timeless classics.</t>
         </is>
       </c>
       <c r="D130" t="inlineStr">
@@ -6775,7 +6775,7 @@
       <c r="I130" t="inlineStr"/>
       <c r="J130" t="inlineStr">
         <is>
-          <t>Please provide me with 10 long and interesting facts about Theodore Roosevelt. I have a youtube channel based on influential figures so this information must be accurate as my channel depends on it. Please make the output of the facts at least 700 words long. Thank you.</t>
+          <t>Please provide me with 10 long and interesting facts about Frank Sinatra. I have a youtube channel based on influential figures so this information must be accurate as my channel depends on it. Please make the output of the facts at least 700 words long. Thank you.</t>
         </is>
       </c>
     </row>
@@ -6785,22 +6785,22 @@
       </c>
       <c r="B131" t="inlineStr">
         <is>
-          <t>Benazir Bhutto</t>
+          <t>Didier Drogba</t>
         </is>
       </c>
       <c r="C131" t="inlineStr">
         <is>
-          <t>Prime Minister of Pakistan from 1988 to 1990 and again from 1993 to 1996, she was the first woman to be elected prime minister of a Muslim-majority country.</t>
+          <t>Ivorian footballer and humanitarian.</t>
         </is>
       </c>
       <c r="D131" t="inlineStr">
         <is>
-          <t>No</t>
+          <t>Yes</t>
         </is>
       </c>
       <c r="E131" t="inlineStr">
         <is>
-          <t>No</t>
+          <t>Yes</t>
         </is>
       </c>
       <c r="F131" t="inlineStr">
@@ -6821,7 +6821,7 @@
       <c r="I131" t="inlineStr"/>
       <c r="J131" t="inlineStr">
         <is>
-          <t>Please provide me with 10 long and interesting facts about Benazir Bhutto. I have a youtube channel based on influential figures so this information must be accurate as my channel depends on it. Please make the output of the facts at least 700 words long. Thank you.</t>
+          <t>Please provide me with 10 long and interesting facts about Didier Drogba. I have a youtube channel based on influential figures so this information must be accurate as my channel depends on it. Please make the output of the facts at least 700 words long. Thank you.</t>
         </is>
       </c>
     </row>
@@ -6831,22 +6831,22 @@
       </c>
       <c r="B132" t="inlineStr">
         <is>
-          <t>Stephen Keshi</t>
+          <t>Caster Semenya</t>
         </is>
       </c>
       <c r="C132" t="inlineStr">
         <is>
-          <t>Nigerian footballer and coach, led Nigeria to AFCON victory.</t>
+          <t>South African middle-distance runner and Olympic gold medalist.</t>
         </is>
       </c>
       <c r="D132" t="inlineStr">
         <is>
-          <t>No</t>
+          <t>Yes</t>
         </is>
       </c>
       <c r="E132" t="inlineStr">
         <is>
-          <t>No</t>
+          <t>Yes</t>
         </is>
       </c>
       <c r="F132" t="inlineStr">
@@ -6867,7 +6867,7 @@
       <c r="I132" t="inlineStr"/>
       <c r="J132" t="inlineStr">
         <is>
-          <t>Please provide me with 10 long and interesting facts about Stephen Keshi. I have a youtube channel based on influential figures so this information must be accurate as my channel depends on it. Please make the output of the facts at least 700 words long. Thank you.</t>
+          <t>Please provide me with 10 long and interesting facts about Caster Semenya. I have a youtube channel based on influential figures so this information must be accurate as my channel depends on it. Please make the output of the facts at least 700 words long. Thank you.</t>
         </is>
       </c>
     </row>
@@ -6877,22 +6877,22 @@
       </c>
       <c r="B133" t="inlineStr">
         <is>
-          <t>Funmilayo Ransome-Kuti</t>
+          <t>Miriam Makeba</t>
         </is>
       </c>
       <c r="C133" t="inlineStr">
         <is>
-          <t>Nigerian women's rights advocate and activist.</t>
+          <t>South African singer and civil rights activist.</t>
         </is>
       </c>
       <c r="D133" t="inlineStr">
         <is>
-          <t>No</t>
+          <t>Yes</t>
         </is>
       </c>
       <c r="E133" t="inlineStr">
         <is>
-          <t>No</t>
+          <t>Yes</t>
         </is>
       </c>
       <c r="F133" t="inlineStr">
@@ -6913,7 +6913,7 @@
       <c r="I133" t="inlineStr"/>
       <c r="J133" t="inlineStr">
         <is>
-          <t>Please provide me with 10 long and interesting facts about Funmilayo Ransome-Kuti. I have a youtube channel based on influential figures so this information must be accurate as my channel depends on it. Please make the output of the facts at least 700 words long. Thank you.</t>
+          <t>Please provide me with 10 long and interesting facts about Miriam Makeba. I have a youtube channel based on influential figures so this information must be accurate as my channel depends on it. Please make the output of the facts at least 700 words long. Thank you.</t>
         </is>
       </c>
     </row>
@@ -6923,22 +6923,22 @@
       </c>
       <c r="B134" t="inlineStr">
         <is>
-          <t>Ayrton Senna</t>
+          <t>Betty Friedan</t>
         </is>
       </c>
       <c r="C134" t="inlineStr">
         <is>
-          <t>Brazilian racing driver, considered one of the greatest Formula 1 drivers.</t>
+          <t>Author of the book "The Feminine Mystique," which helped to spark the second wave of the feminist movement.</t>
         </is>
       </c>
       <c r="D134" t="inlineStr">
         <is>
-          <t>No</t>
+          <t>Yes</t>
         </is>
       </c>
       <c r="E134" t="inlineStr">
         <is>
-          <t>No</t>
+          <t>Yes</t>
         </is>
       </c>
       <c r="F134" t="inlineStr">
@@ -6959,7 +6959,7 @@
       <c r="I134" t="inlineStr"/>
       <c r="J134" t="inlineStr">
         <is>
-          <t>Please provide me with 10 long and interesting facts about Ayrton Senna. I have a youtube channel based on influential figures so this information must be accurate as my channel depends on it. Please make the output of the facts at least 700 words long. Thank you.</t>
+          <t>Please provide me with 10 long and interesting facts about Betty Friedan. I have a youtube channel based on influential figures so this information must be accurate as my channel depends on it. Please make the output of the facts at least 700 words long. Thank you.</t>
         </is>
       </c>
     </row>
@@ -6969,22 +6969,22 @@
       </c>
       <c r="B135" t="inlineStr">
         <is>
-          <t>Georgia O'Keeffe</t>
+          <t>Emperor Wu of Liang</t>
         </is>
       </c>
       <c r="C135" t="inlineStr">
         <is>
-          <t>American painter, known for her large-scale flower paintings.</t>
+          <t>Ruler of the Liang Dynasty in China during the 6th century CE, famous for his support of Buddhism and patronage of the arts.</t>
         </is>
       </c>
       <c r="D135" t="inlineStr">
         <is>
-          <t>No</t>
+          <t>Yes</t>
         </is>
       </c>
       <c r="E135" t="inlineStr">
         <is>
-          <t>No</t>
+          <t>Yes</t>
         </is>
       </c>
       <c r="F135" t="inlineStr">
@@ -7005,7 +7005,7 @@
       <c r="I135" t="inlineStr"/>
       <c r="J135" t="inlineStr">
         <is>
-          <t>Please provide me with 10 long and interesting facts about Georgia O'Keeffe. I have a youtube channel based on influential figures so this information must be accurate as my channel depends on it. Please make the output of the facts at least 700 words long. Thank you.</t>
+          <t>Please provide me with 10 long and interesting facts about Emperor Wu of Liang. I have a youtube channel based on influential figures so this information must be accurate as my channel depends on it. Please make the output of the facts at least 700 words long. Thank you.</t>
         </is>
       </c>
     </row>
@@ -7015,22 +7015,22 @@
       </c>
       <c r="B136" t="inlineStr">
         <is>
-          <t>Caster Semenya</t>
+          <t>Martina Navratilova</t>
         </is>
       </c>
       <c r="C136" t="inlineStr">
         <is>
-          <t>South African middle-distance runner and Olympic gold medalist.</t>
+          <t>Czech-American tennis player, considered one of the greatest female players.</t>
         </is>
       </c>
       <c r="D136" t="inlineStr">
         <is>
-          <t>No</t>
+          <t>Yes</t>
         </is>
       </c>
       <c r="E136" t="inlineStr">
         <is>
-          <t>No</t>
+          <t>Yes</t>
         </is>
       </c>
       <c r="F136" t="inlineStr">
@@ -7051,7 +7051,7 @@
       <c r="I136" t="inlineStr"/>
       <c r="J136" t="inlineStr">
         <is>
-          <t>Please provide me with 10 long and interesting facts about Caster Semenya. I have a youtube channel based on influential figures so this information must be accurate as my channel depends on it. Please make the output of the facts at least 700 words long. Thank you.</t>
+          <t>Please provide me with 10 long and interesting facts about Martina Navratilova. I have a youtube channel based on influential figures so this information must be accurate as my channel depends on it. Please make the output of the facts at least 700 words long. Thank you.</t>
         </is>
       </c>
     </row>
@@ -7061,22 +7061,22 @@
       </c>
       <c r="B137" t="inlineStr">
         <is>
-          <t>Wassily Kandinsky</t>
+          <t>Benazir Bhutto</t>
         </is>
       </c>
       <c r="C137" t="inlineStr">
         <is>
-          <t>Russian abstract painter, one of the pioneers of abstract art.</t>
+          <t>Prime Minister of Pakistan from 1988 to 1990 and again from 1993 to 1996, she was the first woman to be elected prime minister of a Muslim-majority country.</t>
         </is>
       </c>
       <c r="D137" t="inlineStr">
         <is>
-          <t>No</t>
+          <t>Yes</t>
         </is>
       </c>
       <c r="E137" t="inlineStr">
         <is>
-          <t>No</t>
+          <t>Yes</t>
         </is>
       </c>
       <c r="F137" t="inlineStr">
@@ -7097,7 +7097,7 @@
       <c r="I137" t="inlineStr"/>
       <c r="J137" t="inlineStr">
         <is>
-          <t>Please provide me with 10 long and interesting facts about Wassily Kandinsky. I have a youtube channel based on influential figures so this information must be accurate as my channel depends on it. Please make the output of the facts at least 700 words long. Thank you.</t>
+          <t>Please provide me with 10 long and interesting facts about Benazir Bhutto. I have a youtube channel based on influential figures so this information must be accurate as my channel depends on it. Please make the output of the facts at least 700 words long. Thank you.</t>
         </is>
       </c>
     </row>
@@ -7107,22 +7107,22 @@
       </c>
       <c r="B138" t="inlineStr">
         <is>
-          <t>Queen Makeda (Queen of Sheba)</t>
+          <t>Greg Lemond</t>
         </is>
       </c>
       <c r="C138" t="inlineStr">
         <is>
-          <t>Legendary queen who visited King Solomon.</t>
+          <t>American cyclist, three-time Tour de France winner.</t>
         </is>
       </c>
       <c r="D138" t="inlineStr">
         <is>
-          <t>No</t>
+          <t>Yes</t>
         </is>
       </c>
       <c r="E138" t="inlineStr">
         <is>
-          <t>No</t>
+          <t>Yes</t>
         </is>
       </c>
       <c r="F138" t="inlineStr">
@@ -7143,7 +7143,7 @@
       <c r="I138" t="inlineStr"/>
       <c r="J138" t="inlineStr">
         <is>
-          <t>Please provide me with 10 long and interesting facts about Queen Makeda (Queen of Sheba). I have a youtube channel based on influential figures so this information must be accurate as my channel depends on it. Please make the output of the facts at least 700 words long. Thank you.</t>
+          <t>Please provide me with 10 long and interesting facts about Greg Lemond. I have a youtube channel based on influential figures so this information must be accurate as my channel depends on it. Please make the output of the facts at least 700 words long. Thank you.</t>
         </is>
       </c>
     </row>
@@ -7153,22 +7153,22 @@
       </c>
       <c r="B139" t="inlineStr">
         <is>
-          <t>Emperor Wu of Liang</t>
+          <t>Xenophon</t>
         </is>
       </c>
       <c r="C139" t="inlineStr">
         <is>
-          <t>Ruler of the Liang Dynasty in China during the 6th century CE, famous for his support of Buddhism and patronage of the arts.</t>
+          <t>A Greek historian and soldier, he wrote about the Peloponnesian War and the Anabasis.</t>
         </is>
       </c>
       <c r="D139" t="inlineStr">
         <is>
-          <t>No</t>
+          <t>Yes</t>
         </is>
       </c>
       <c r="E139" t="inlineStr">
         <is>
-          <t>No</t>
+          <t>Yes</t>
         </is>
       </c>
       <c r="F139" t="inlineStr">
@@ -7189,7 +7189,7 @@
       <c r="I139" t="inlineStr"/>
       <c r="J139" t="inlineStr">
         <is>
-          <t>Please provide me with 10 long and interesting facts about Emperor Wu of Liang. I have a youtube channel based on influential figures so this information must be accurate as my channel depends on it. Please make the output of the facts at least 700 words long. Thank you.</t>
+          <t>Please provide me with 10 long and interesting facts about Xenophon. I have a youtube channel based on influential figures so this information must be accurate as my channel depends on it. Please make the output of the facts at least 700 words long. Thank you.</t>
         </is>
       </c>
     </row>
@@ -7199,22 +7199,22 @@
       </c>
       <c r="B140" t="inlineStr">
         <is>
-          <t>Abu al-Qasim al-Zahrawi</t>
+          <t>Ching Shih</t>
         </is>
       </c>
       <c r="C140" t="inlineStr">
         <is>
-          <t>Medieval Andalusian surgeon and polymath who wrote extensively on medicine, surgery, and pharmacology, influencing medical practices for centuries.</t>
+          <t>Chinese pirate leader during the early 19th century, who commanded a vast fleet and became one of the most successful pirates in history.</t>
         </is>
       </c>
       <c r="D140" t="inlineStr">
         <is>
-          <t>No</t>
+          <t>Yes</t>
         </is>
       </c>
       <c r="E140" t="inlineStr">
         <is>
-          <t>No</t>
+          <t>Yes</t>
         </is>
       </c>
       <c r="F140" t="inlineStr">
@@ -7235,7 +7235,7 @@
       <c r="I140" t="inlineStr"/>
       <c r="J140" t="inlineStr">
         <is>
-          <t>Please provide me with 10 long and interesting facts about Abu al-Qasim al-Zahrawi. I have a youtube channel based on influential figures so this information must be accurate as my channel depends on it. Please make the output of the facts at least 700 words long. Thank you.</t>
+          <t>Please provide me with 10 long and interesting facts about Ching Shih. I have a youtube channel based on influential figures so this information must be accurate as my channel depends on it. Please make the output of the facts at least 700 words long. Thank you.</t>
         </is>
       </c>
     </row>
@@ -7245,22 +7245,22 @@
       </c>
       <c r="B141" t="inlineStr">
         <is>
-          <t>Haile Selassie</t>
+          <t>Patrice Lumumba</t>
         </is>
       </c>
       <c r="C141" t="inlineStr">
         <is>
-          <t>Emperor of Ethiopia and African unity advocate.</t>
+          <t>Independence leader, first PM of the Congo.</t>
         </is>
       </c>
       <c r="D141" t="inlineStr">
         <is>
-          <t>No</t>
+          <t>Yes</t>
         </is>
       </c>
       <c r="E141" t="inlineStr">
         <is>
-          <t>No</t>
+          <t>Yes</t>
         </is>
       </c>
       <c r="F141" t="inlineStr">
@@ -7281,7 +7281,7 @@
       <c r="I141" t="inlineStr"/>
       <c r="J141" t="inlineStr">
         <is>
-          <t>Please provide me with 10 long and interesting facts about Haile Selassie. I have a youtube channel based on influential figures so this information must be accurate as my channel depends on it. Please make the output of the facts at least 700 words long. Thank you.</t>
+          <t>Please provide me with 10 long and interesting facts about Patrice Lumumba. I have a youtube channel based on influential figures so this information must be accurate as my channel depends on it. Please make the output of the facts at least 700 words long. Thank you.</t>
         </is>
       </c>
     </row>
@@ -7291,22 +7291,22 @@
       </c>
       <c r="B142" t="inlineStr">
         <is>
-          <t>W.E.B. Du Bois</t>
+          <t>Haile Selassie</t>
         </is>
       </c>
       <c r="C142" t="inlineStr">
         <is>
-          <t>One of the most important figures in the American civil rights movement, he was a scholar, writer, and activist.</t>
+          <t>Emperor of Ethiopia and African unity advocate.</t>
         </is>
       </c>
       <c r="D142" t="inlineStr">
         <is>
-          <t>No</t>
+          <t>Yes</t>
         </is>
       </c>
       <c r="E142" t="inlineStr">
         <is>
-          <t>No</t>
+          <t>Yes</t>
         </is>
       </c>
       <c r="F142" t="inlineStr">
@@ -7327,7 +7327,7 @@
       <c r="I142" t="inlineStr"/>
       <c r="J142" t="inlineStr">
         <is>
-          <t>Please provide me with 10 long and interesting facts about W.E.B. Du Bois. I have a youtube channel based on influential figures so this information must be accurate as my channel depends on it. Please make the output of the facts at least 700 words long. Thank you.</t>
+          <t>Please provide me with 10 long and interesting facts about Haile Selassie. I have a youtube channel based on influential figures so this information must be accurate as my channel depends on it. Please make the output of the facts at least 700 words long. Thank you.</t>
         </is>
       </c>
     </row>
@@ -7337,22 +7337,22 @@
       </c>
       <c r="B143" t="inlineStr">
         <is>
-          <t>Kofi Annan</t>
+          <t>Elon Musk</t>
         </is>
       </c>
       <c r="C143" t="inlineStr">
         <is>
-          <t>Ghanaian diplomat, UN Secretary-General, Nobel laureate.</t>
+          <t>Co-founder of Tesla and SpaceX, he is one of the most innovative entrepreneurs of our time.</t>
         </is>
       </c>
       <c r="D143" t="inlineStr">
         <is>
-          <t>No</t>
+          <t>Yes</t>
         </is>
       </c>
       <c r="E143" t="inlineStr">
         <is>
-          <t>No</t>
+          <t>Yes</t>
         </is>
       </c>
       <c r="F143" t="inlineStr">
@@ -7373,7 +7373,7 @@
       <c r="I143" t="inlineStr"/>
       <c r="J143" t="inlineStr">
         <is>
-          <t>Please provide me with 10 long and interesting facts about Kofi Annan. I have a youtube channel based on influential figures so this information must be accurate as my channel depends on it. Please make the output of the facts at least 700 words long. Thank you.</t>
+          <t>Please provide me with 10 long and interesting facts about Elon Musk. I have a youtube channel based on influential figures so this information must be accurate as my channel depends on it. Please make the output of the facts at least 700 words long. Thank you.</t>
         </is>
       </c>
     </row>
@@ -7383,22 +7383,22 @@
       </c>
       <c r="B144" t="inlineStr">
         <is>
-          <t>Maria Mutola</t>
+          <t>Chen Guangcheng</t>
         </is>
       </c>
       <c r="C144" t="inlineStr">
         <is>
-          <t>Mozambican middle-distance runner, Olympic gold medalist.</t>
+          <t>Fought for the rights of people with disabilities in China and was imprisoned for his activism.</t>
         </is>
       </c>
       <c r="D144" t="inlineStr">
         <is>
-          <t>No</t>
+          <t>Yes</t>
         </is>
       </c>
       <c r="E144" t="inlineStr">
         <is>
-          <t>No</t>
+          <t>Yes</t>
         </is>
       </c>
       <c r="F144" t="inlineStr">
@@ -7419,7 +7419,7 @@
       <c r="I144" t="inlineStr"/>
       <c r="J144" t="inlineStr">
         <is>
-          <t>Please provide me with 10 long and interesting facts about Maria Mutola. I have a youtube channel based on influential figures so this information must be accurate as my channel depends on it. Please make the output of the facts at least 700 words long. Thank you.</t>
+          <t>Please provide me with 10 long and interesting facts about Chen Guangcheng. I have a youtube channel based on influential figures so this information must be accurate as my channel depends on it. Please make the output of the facts at least 700 words long. Thank you.</t>
         </is>
       </c>
     </row>
@@ -7429,22 +7429,22 @@
       </c>
       <c r="B145" t="inlineStr">
         <is>
-          <t>Wilhelmina Drucker</t>
+          <t>Jean-Claude Killy</t>
         </is>
       </c>
       <c r="C145" t="inlineStr">
         <is>
-          <t>One of the first women to be elected to the German parliament, she was a leading figure in the women's suffrage movement.</t>
+          <t>French alpine ski racer, triple Olympic gold medalist.</t>
         </is>
       </c>
       <c r="D145" t="inlineStr">
         <is>
-          <t>No</t>
+          <t>Yes</t>
         </is>
       </c>
       <c r="E145" t="inlineStr">
         <is>
-          <t>No</t>
+          <t>Yes</t>
         </is>
       </c>
       <c r="F145" t="inlineStr">
@@ -7465,7 +7465,7 @@
       <c r="I145" t="inlineStr"/>
       <c r="J145" t="inlineStr">
         <is>
-          <t>Please provide me with 10 long and interesting facts about Wilhelmina Drucker. I have a youtube channel based on influential figures so this information must be accurate as my channel depends on it. Please make the output of the facts at least 700 words long. Thank you.</t>
+          <t>Please provide me with 10 long and interesting facts about Jean-Claude Killy. I have a youtube channel based on influential figures so this information must be accurate as my channel depends on it. Please make the output of the facts at least 700 words long. Thank you.</t>
         </is>
       </c>
     </row>
@@ -7475,22 +7475,22 @@
       </c>
       <c r="B146" t="inlineStr">
         <is>
-          <t>Golda Meir</t>
+          <t>Mikhail Gorbachev</t>
         </is>
       </c>
       <c r="C146" t="inlineStr">
         <is>
-          <t>Israeli Prime Minister and one of the world's first female heads of government.</t>
+          <t>Soviet statesman, implemented reforms leading to the end of the Cold War.</t>
         </is>
       </c>
       <c r="D146" t="inlineStr">
         <is>
-          <t>No</t>
+          <t>Yes</t>
         </is>
       </c>
       <c r="E146" t="inlineStr">
         <is>
-          <t>No</t>
+          <t>Yes</t>
         </is>
       </c>
       <c r="F146" t="inlineStr">
@@ -7511,7 +7511,7 @@
       <c r="I146" t="inlineStr"/>
       <c r="J146" t="inlineStr">
         <is>
-          <t>Please provide me with 10 long and interesting facts about Golda Meir. I have a youtube channel based on influential figures so this information must be accurate as my channel depends on it. Please make the output of the facts at least 700 words long. Thank you.</t>
+          <t>Please provide me with 10 long and interesting facts about Mikhail Gorbachev. I have a youtube channel based on influential figures so this information must be accurate as my channel depends on it. Please make the output of the facts at least 700 words long. Thank you.</t>
         </is>
       </c>
     </row>
@@ -7521,22 +7521,22 @@
       </c>
       <c r="B147" t="inlineStr">
         <is>
-          <t>Hicham El Guerrouj</t>
+          <t>Vivian Cheruiyot</t>
         </is>
       </c>
       <c r="C147" t="inlineStr">
         <is>
-          <t>Moroccan middle-distance runner, Olympic gold medalist.</t>
+          <t>Kenyan long-distance runner, Olympic gold medalist.</t>
         </is>
       </c>
       <c r="D147" t="inlineStr">
         <is>
-          <t>No</t>
+          <t>Yes</t>
         </is>
       </c>
       <c r="E147" t="inlineStr">
         <is>
-          <t>No</t>
+          <t>Yes</t>
         </is>
       </c>
       <c r="F147" t="inlineStr">
@@ -7557,7 +7557,7 @@
       <c r="I147" t="inlineStr"/>
       <c r="J147" t="inlineStr">
         <is>
-          <t>Please provide me with 10 long and interesting facts about Hicham El Guerrouj. I have a youtube channel based on influential figures so this information must be accurate as my channel depends on it. Please make the output of the facts at least 700 words long. Thank you.</t>
+          <t>Please provide me with 10 long and interesting facts about Vivian Cheruiyot. I have a youtube channel based on influential figures so this information must be accurate as my channel depends on it. Please make the output of the facts at least 700 words long. Thank you.</t>
         </is>
       </c>
     </row>
@@ -7567,22 +7567,22 @@
       </c>
       <c r="B148" t="inlineStr">
         <is>
-          <t>Elon Musk</t>
+          <t>Yayoi Kusama</t>
         </is>
       </c>
       <c r="C148" t="inlineStr">
         <is>
-          <t>Co-founder of Tesla and SpaceX, he is one of the most innovative entrepreneurs of our time.</t>
+          <t>Japanese contemporary artist, known for her immersive installations and polka dot motifs.</t>
         </is>
       </c>
       <c r="D148" t="inlineStr">
         <is>
-          <t>No</t>
+          <t>Yes</t>
         </is>
       </c>
       <c r="E148" t="inlineStr">
         <is>
-          <t>No</t>
+          <t>Yes</t>
         </is>
       </c>
       <c r="F148" t="inlineStr">
@@ -7603,7 +7603,7 @@
       <c r="I148" t="inlineStr"/>
       <c r="J148" t="inlineStr">
         <is>
-          <t>Please provide me with 10 long and interesting facts about Elon Musk. I have a youtube channel based on influential figures so this information must be accurate as my channel depends on it. Please make the output of the facts at least 700 words long. Thank you.</t>
+          <t>Please provide me with 10 long and interesting facts about Yayoi Kusama. I have a youtube channel based on influential figures so this information must be accurate as my channel depends on it. Please make the output of the facts at least 700 words long. Thank you.</t>
         </is>
       </c>
     </row>
@@ -7613,22 +7613,22 @@
       </c>
       <c r="B149" t="inlineStr">
         <is>
-          <t>Michael Essien</t>
+          <t>Guru Nanak</t>
         </is>
       </c>
       <c r="C149" t="inlineStr">
         <is>
-          <t>Ghanaian footballer, known for his versatility.</t>
+          <t>Founder of Sikhism in the 15th century, revered as the first Sikh guru and promoting the principles of equality and social justice.</t>
         </is>
       </c>
       <c r="D149" t="inlineStr">
         <is>
-          <t>No</t>
+          <t>Yes</t>
         </is>
       </c>
       <c r="E149" t="inlineStr">
         <is>
-          <t>No</t>
+          <t>Yes</t>
         </is>
       </c>
       <c r="F149" t="inlineStr">
@@ -7649,7 +7649,7 @@
       <c r="I149" t="inlineStr"/>
       <c r="J149" t="inlineStr">
         <is>
-          <t>Please provide me with 10 long and interesting facts about Michael Essien. I have a youtube channel based on influential figures so this information must be accurate as my channel depends on it. Please make the output of the facts at least 700 words long. Thank you.</t>
+          <t>Please provide me with 10 long and interesting facts about Guru Nanak. I have a youtube channel based on influential figures so this information must be accurate as my channel depends on it. Please make the output of the facts at least 700 words long. Thank you.</t>
         </is>
       </c>
     </row>
@@ -7659,22 +7659,22 @@
       </c>
       <c r="B150" t="inlineStr">
         <is>
-          <t>Mikhail Gorbachev</t>
+          <t>Michael Essien</t>
         </is>
       </c>
       <c r="C150" t="inlineStr">
         <is>
-          <t>Soviet statesman, implemented reforms leading to the end of the Cold War.</t>
+          <t>Ghanaian footballer, known for his versatility.</t>
         </is>
       </c>
       <c r="D150" t="inlineStr">
         <is>
-          <t>No</t>
+          <t>Yes</t>
         </is>
       </c>
       <c r="E150" t="inlineStr">
         <is>
-          <t>No</t>
+          <t>Yes</t>
         </is>
       </c>
       <c r="F150" t="inlineStr">
@@ -7695,7 +7695,7 @@
       <c r="I150" t="inlineStr"/>
       <c r="J150" t="inlineStr">
         <is>
-          <t>Please provide me with 10 long and interesting facts about Mikhail Gorbachev. I have a youtube channel based on influential figures so this information must be accurate as my channel depends on it. Please make the output of the facts at least 700 words long. Thank you.</t>
+          <t>Please provide me with 10 long and interesting facts about Michael Essien. I have a youtube channel based on influential figures so this information must be accurate as my channel depends on it. Please make the output of the facts at least 700 words long. Thank you.</t>
         </is>
       </c>
     </row>
@@ -7705,22 +7705,22 @@
       </c>
       <c r="B151" t="inlineStr">
         <is>
-          <t>Blessing Okagbare</t>
+          <t>Al-Khansa</t>
         </is>
       </c>
       <c r="C151" t="inlineStr">
         <is>
-          <t>Nigerian track and field athlete, Olympic medalist.</t>
+          <t>Arabic poetess in the 7th century CE, recognized for her elegies and poems commemorating fallen warriors.</t>
         </is>
       </c>
       <c r="D151" t="inlineStr">
         <is>
-          <t>No</t>
+          <t>Yes</t>
         </is>
       </c>
       <c r="E151" t="inlineStr">
         <is>
-          <t>No</t>
+          <t>Yes</t>
         </is>
       </c>
       <c r="F151" t="inlineStr">
@@ -7741,7 +7741,7 @@
       <c r="I151" t="inlineStr"/>
       <c r="J151" t="inlineStr">
         <is>
-          <t>Please provide me with 10 long and interesting facts about Blessing Okagbare. I have a youtube channel based on influential figures so this information must be accurate as my channel depends on it. Please make the output of the facts at least 700 words long. Thank you.</t>
+          <t>Please provide me with 10 long and interesting facts about Al-Khansa. I have a youtube channel based on influential figures so this information must be accurate as my channel depends on it. Please make the output of the facts at least 700 words long. Thank you.</t>
         </is>
       </c>
     </row>
@@ -7751,22 +7751,22 @@
       </c>
       <c r="B152" t="inlineStr">
         <is>
-          <t>Tina Fey</t>
+          <t>Ellen Johnson Sirleaf</t>
         </is>
       </c>
       <c r="C152" t="inlineStr">
         <is>
-          <t>One of the most successful comedians of all time, she is also a successful actress and writer.</t>
+          <t>First female president in Africa and Nobel laureate.</t>
         </is>
       </c>
       <c r="D152" t="inlineStr">
         <is>
-          <t>No</t>
+          <t>Yes</t>
         </is>
       </c>
       <c r="E152" t="inlineStr">
         <is>
-          <t>No</t>
+          <t>Yes</t>
         </is>
       </c>
       <c r="F152" t="inlineStr">
@@ -7787,7 +7787,7 @@
       <c r="I152" t="inlineStr"/>
       <c r="J152" t="inlineStr">
         <is>
-          <t>Please provide me with 10 long and interesting facts about Tina Fey. I have a youtube channel based on influential figures so this information must be accurate as my channel depends on it. Please make the output of the facts at least 700 words long. Thank you.</t>
+          <t>Please provide me with 10 long and interesting facts about Ellen Johnson Sirleaf. I have a youtube channel based on influential figures so this information must be accurate as my channel depends on it. Please make the output of the facts at least 700 words long. Thank you.</t>
         </is>
       </c>
     </row>
@@ -7797,22 +7797,22 @@
       </c>
       <c r="B153" t="inlineStr">
         <is>
-          <t>John Lennon</t>
+          <t>Jacqueline Kennedy Onassis</t>
         </is>
       </c>
       <c r="C153" t="inlineStr">
         <is>
-          <t>British singer, songwriter, and member of The Beatles.</t>
+          <t>One of the most popular First Ladies of the 20th century, she was also a successful author.</t>
         </is>
       </c>
       <c r="D153" t="inlineStr">
         <is>
-          <t>No</t>
+          <t>Yes</t>
         </is>
       </c>
       <c r="E153" t="inlineStr">
         <is>
-          <t>No</t>
+          <t>Yes</t>
         </is>
       </c>
       <c r="F153" t="inlineStr">
@@ -7833,7 +7833,7 @@
       <c r="I153" t="inlineStr"/>
       <c r="J153" t="inlineStr">
         <is>
-          <t>Please provide me with 10 long and interesting facts about John Lennon. I have a youtube channel based on influential figures so this information must be accurate as my channel depends on it. Please make the output of the facts at least 700 words long. Thank you.</t>
+          <t>Please provide me with 10 long and interesting facts about Jacqueline Kennedy Onassis. I have a youtube channel based on influential figures so this information must be accurate as my channel depends on it. Please make the output of the facts at least 700 words long. Thank you.</t>
         </is>
       </c>
     </row>
@@ -7843,22 +7843,22 @@
       </c>
       <c r="B154" t="inlineStr">
         <is>
-          <t>Aung San Suu Kyi</t>
+          <t>Henri Matisse</t>
         </is>
       </c>
       <c r="C154" t="inlineStr">
         <is>
-          <t>Led the pro-democracy movement in Myanmar and was awarded the Nobel Peace Prize.</t>
+          <t>French artist, known for his colorful and innovative use of shapes and patterns.</t>
         </is>
       </c>
       <c r="D154" t="inlineStr">
         <is>
-          <t>No</t>
+          <t>Yes</t>
         </is>
       </c>
       <c r="E154" t="inlineStr">
         <is>
-          <t>No</t>
+          <t>Yes</t>
         </is>
       </c>
       <c r="F154" t="inlineStr">
@@ -7879,7 +7879,7 @@
       <c r="I154" t="inlineStr"/>
       <c r="J154" t="inlineStr">
         <is>
-          <t>Please provide me with 10 long and interesting facts about Aung San Suu Kyi. I have a youtube channel based on influential figures so this information must be accurate as my channel depends on it. Please make the output of the facts at least 700 words long. Thank you.</t>
+          <t>Please provide me with 10 long and interesting facts about Henri Matisse. I have a youtube channel based on influential figures so this information must be accurate as my channel depends on it. Please make the output of the facts at least 700 words long. Thank you.</t>
         </is>
       </c>
     </row>
@@ -7889,22 +7889,22 @@
       </c>
       <c r="B155" t="inlineStr">
         <is>
-          <t>Empress Jingu</t>
+          <t>Michael Jordan</t>
         </is>
       </c>
       <c r="C155" t="inlineStr">
         <is>
-          <t>Legendary Japanese empress who led successful military campaigns, including the conquest of Korea, during the 3rd century.</t>
+          <t>American basketball player, NBA legend.</t>
         </is>
       </c>
       <c r="D155" t="inlineStr">
         <is>
-          <t>No</t>
+          <t>Yes</t>
         </is>
       </c>
       <c r="E155" t="inlineStr">
         <is>
-          <t>No</t>
+          <t>Yes</t>
         </is>
       </c>
       <c r="F155" t="inlineStr">
@@ -7925,7 +7925,7 @@
       <c r="I155" t="inlineStr"/>
       <c r="J155" t="inlineStr">
         <is>
-          <t>Please provide me with 10 long and interesting facts about Empress Jingu. I have a youtube channel based on influential figures so this information must be accurate as my channel depends on it. Please make the output of the facts at least 700 words long. Thank you.</t>
+          <t>Please provide me with 10 long and interesting facts about Michael Jordan. I have a youtube channel based on influential figures so this information must be accurate as my channel depends on it. Please make the output of the facts at least 700 words long. Thank you.</t>
         </is>
       </c>
     </row>
@@ -7935,22 +7935,22 @@
       </c>
       <c r="B156" t="inlineStr">
         <is>
-          <t>Thomas Sankara</t>
+          <t>Al-Kindi</t>
         </is>
       </c>
       <c r="C156" t="inlineStr">
         <is>
-          <t>Burkina Faso's revolutionary leader and president.</t>
+          <t>Arab philosopher and polymath in the 9th century, making significant contributions to mathematics, astronomy, and philosophy.</t>
         </is>
       </c>
       <c r="D156" t="inlineStr">
         <is>
-          <t>No</t>
+          <t>Yes</t>
         </is>
       </c>
       <c r="E156" t="inlineStr">
         <is>
-          <t>No</t>
+          <t>Yes</t>
         </is>
       </c>
       <c r="F156" t="inlineStr">
@@ -7971,7 +7971,7 @@
       <c r="I156" t="inlineStr"/>
       <c r="J156" t="inlineStr">
         <is>
-          <t>Please provide me with 10 long and interesting facts about Thomas Sankara. I have a youtube channel based on influential figures so this information must be accurate as my channel depends on it. Please make the output of the facts at least 700 words long. Thank you.</t>
+          <t>Please provide me with 10 long and interesting facts about Al-Kindi. I have a youtube channel based on influential figures so this information must be accurate as my channel depends on it. Please make the output of the facts at least 700 words long. Thank you.</t>
         </is>
       </c>
     </row>
@@ -7981,22 +7981,22 @@
       </c>
       <c r="B157" t="inlineStr">
         <is>
-          <t>Mustafa Kemal Atatürk</t>
+          <t>Abebe Bikila</t>
         </is>
       </c>
       <c r="C157" t="inlineStr">
         <is>
-          <t>Founder and first President of Turkey, known for modernizing reforms.</t>
+          <t>Ethiopian marathon runner and Olympic champion.</t>
         </is>
       </c>
       <c r="D157" t="inlineStr">
         <is>
-          <t>No</t>
+          <t>Yes</t>
         </is>
       </c>
       <c r="E157" t="inlineStr">
         <is>
-          <t>No</t>
+          <t>Yes</t>
         </is>
       </c>
       <c r="F157" t="inlineStr">
@@ -8017,7 +8017,7 @@
       <c r="I157" t="inlineStr"/>
       <c r="J157" t="inlineStr">
         <is>
-          <t>Please provide me with 10 long and interesting facts about Mustafa Kemal Atatürk. I have a youtube channel based on influential figures so this information must be accurate as my channel depends on it. Please make the output of the facts at least 700 words long. Thank you.</t>
+          <t>Please provide me with 10 long and interesting facts about Abebe Bikila. I have a youtube channel based on influential figures so this information must be accurate as my channel depends on it. Please make the output of the facts at least 700 words long. Thank you.</t>
         </is>
       </c>
     </row>
@@ -8027,22 +8027,22 @@
       </c>
       <c r="B158" t="inlineStr">
         <is>
-          <t>Blessing Awodibu</t>
+          <t>Jim Henson</t>
         </is>
       </c>
       <c r="C158" t="inlineStr">
         <is>
-          <t>South African bodybuilder and social media influencer.</t>
+          <t>One of the most influential puppeteers of all time, he created some of the most beloved characters in television history.</t>
         </is>
       </c>
       <c r="D158" t="inlineStr">
         <is>
-          <t>No</t>
+          <t>Yes</t>
         </is>
       </c>
       <c r="E158" t="inlineStr">
         <is>
-          <t>No</t>
+          <t>Yes</t>
         </is>
       </c>
       <c r="F158" t="inlineStr">
@@ -8063,7 +8063,7 @@
       <c r="I158" t="inlineStr"/>
       <c r="J158" t="inlineStr">
         <is>
-          <t>Please provide me with 10 long and interesting facts about Blessing Awodibu. I have a youtube channel based on influential figures so this information must be accurate as my channel depends on it. Please make the output of the facts at least 700 words long. Thank you.</t>
+          <t>Please provide me with 10 long and interesting facts about Jim Henson. I have a youtube channel based on influential figures so this information must be accurate as my channel depends on it. Please make the output of the facts at least 700 words long. Thank you.</t>
         </is>
       </c>
     </row>
@@ -8073,22 +8073,22 @@
       </c>
       <c r="B159" t="inlineStr">
         <is>
-          <t>Rani Padmini</t>
+          <t>Maria Mutola</t>
         </is>
       </c>
       <c r="C159" t="inlineStr">
         <is>
-          <t>Queen of Mewar in medieval India, renowned for her beauty and bravery during the siege of Chittorgarh by Alauddin Khilji.</t>
+          <t>Mozambican middle-distance runner, Olympic gold medalist.</t>
         </is>
       </c>
       <c r="D159" t="inlineStr">
         <is>
-          <t>No</t>
+          <t>Yes</t>
         </is>
       </c>
       <c r="E159" t="inlineStr">
         <is>
-          <t>No</t>
+          <t>Yes</t>
         </is>
       </c>
       <c r="F159" t="inlineStr">
@@ -8109,7 +8109,7 @@
       <c r="I159" t="inlineStr"/>
       <c r="J159" t="inlineStr">
         <is>
-          <t>Please provide me with 10 long and interesting facts about Rani Padmini. I have a youtube channel based on influential figures so this information must be accurate as my channel depends on it. Please make the output of the facts at least 700 words long. Thank you.</t>
+          <t>Please provide me with 10 long and interesting facts about Maria Mutola. I have a youtube channel based on influential figures so this information must be accurate as my channel depends on it. Please make the output of the facts at least 700 words long. Thank you.</t>
         </is>
       </c>
     </row>
@@ -8119,22 +8119,22 @@
       </c>
       <c r="B160" t="inlineStr">
         <is>
-          <t>Xenophon</t>
+          <t>Tomoe Gozen</t>
         </is>
       </c>
       <c r="C160" t="inlineStr">
         <is>
-          <t>A Greek historian and soldier, he wrote about the Peloponnesian War and the Anabasis.</t>
+          <t>Female samurai warrior during the 12th century in Japan, renowned for her combat skills and bravery on the battlefield.</t>
         </is>
       </c>
       <c r="D160" t="inlineStr">
         <is>
-          <t>No</t>
+          <t>Yes</t>
         </is>
       </c>
       <c r="E160" t="inlineStr">
         <is>
-          <t>No</t>
+          <t>Yes</t>
         </is>
       </c>
       <c r="F160" t="inlineStr">
@@ -8155,7 +8155,7 @@
       <c r="I160" t="inlineStr"/>
       <c r="J160" t="inlineStr">
         <is>
-          <t>Please provide me with 10 long and interesting facts about Xenophon. I have a youtube channel based on influential figures so this information must be accurate as my channel depends on it. Please make the output of the facts at least 700 words long. Thank you.</t>
+          <t>Please provide me with 10 long and interesting facts about Tomoe Gozen. I have a youtube channel based on influential figures so this information must be accurate as my channel depends on it. Please make the output of the facts at least 700 words long. Thank you.</t>
         </is>
       </c>
     </row>
@@ -8165,22 +8165,22 @@
       </c>
       <c r="B161" t="inlineStr">
         <is>
-          <t>Jean-Claude Killy</t>
+          <t>Tina Fey</t>
         </is>
       </c>
       <c r="C161" t="inlineStr">
         <is>
-          <t>French alpine ski racer, triple Olympic gold medalist.</t>
+          <t>One of the most successful comedians of all time, she is also a successful actress and writer.</t>
         </is>
       </c>
       <c r="D161" t="inlineStr">
         <is>
-          <t>No</t>
+          <t>Yes</t>
         </is>
       </c>
       <c r="E161" t="inlineStr">
         <is>
-          <t>No</t>
+          <t>Yes</t>
         </is>
       </c>
       <c r="F161" t="inlineStr">
@@ -8201,7 +8201,7 @@
       <c r="I161" t="inlineStr"/>
       <c r="J161" t="inlineStr">
         <is>
-          <t>Please provide me with 10 long and interesting facts about Jean-Claude Killy. I have a youtube channel based on influential figures so this information must be accurate as my channel depends on it. Please make the output of the facts at least 700 words long. Thank you.</t>
+          <t>Please provide me with 10 long and interesting facts about Tina Fey. I have a youtube channel based on influential figures so this information must be accurate as my channel depends on it. Please make the output of the facts at least 700 words long. Thank you.</t>
         </is>
       </c>
     </row>
@@ -8211,22 +8211,22 @@
       </c>
       <c r="B162" t="inlineStr">
         <is>
-          <t>Roy Lichtenstein</t>
+          <t>Aung San Suu Kyi</t>
         </is>
       </c>
       <c r="C162" t="inlineStr">
         <is>
-          <t>American pop artist, known for his comic book-style artwork.</t>
+          <t>Led the pro-democracy movement in Myanmar and was awarded the Nobel Peace Prize.</t>
         </is>
       </c>
       <c r="D162" t="inlineStr">
         <is>
-          <t>No</t>
+          <t>Yes</t>
         </is>
       </c>
       <c r="E162" t="inlineStr">
         <is>
-          <t>No</t>
+          <t>Yes</t>
         </is>
       </c>
       <c r="F162" t="inlineStr">
@@ -8247,7 +8247,7 @@
       <c r="I162" t="inlineStr"/>
       <c r="J162" t="inlineStr">
         <is>
-          <t>Please provide me with 10 long and interesting facts about Roy Lichtenstein. I have a youtube channel based on influential figures so this information must be accurate as my channel depends on it. Please make the output of the facts at least 700 words long. Thank you.</t>
+          <t>Please provide me with 10 long and interesting facts about Aung San Suu Kyi. I have a youtube channel based on influential figures so this information must be accurate as my channel depends on it. Please make the output of the facts at least 700 words long. Thank you.</t>
         </is>
       </c>
     </row>
@@ -8257,22 +8257,22 @@
       </c>
       <c r="B163" t="inlineStr">
         <is>
-          <t>Jawaharlal Nehru</t>
+          <t>Georgia O'Keeffe</t>
         </is>
       </c>
       <c r="C163" t="inlineStr">
         <is>
-          <t>Indian independence leader and the first Prime Minister of India.</t>
+          <t>American painter, known for her large-scale flower paintings.</t>
         </is>
       </c>
       <c r="D163" t="inlineStr">
         <is>
-          <t>No</t>
+          <t>Yes</t>
         </is>
       </c>
       <c r="E163" t="inlineStr">
         <is>
-          <t>No</t>
+          <t>Yes</t>
         </is>
       </c>
       <c r="F163" t="inlineStr">
@@ -8293,7 +8293,7 @@
       <c r="I163" t="inlineStr"/>
       <c r="J163" t="inlineStr">
         <is>
-          <t>Please provide me with 10 long and interesting facts about Jawaharlal Nehru. I have a youtube channel based on influential figures so this information must be accurate as my channel depends on it. Please make the output of the facts at least 700 words long. Thank you.</t>
+          <t>Please provide me with 10 long and interesting facts about Georgia O'Keeffe. I have a youtube channel based on influential figures so this information must be accurate as my channel depends on it. Please make the output of the facts at least 700 words long. Thank you.</t>
         </is>
       </c>
     </row>
@@ -8303,22 +8303,22 @@
       </c>
       <c r="B164" t="inlineStr">
         <is>
-          <t>Ho Chi Minh</t>
+          <t>Abu al-Qasim al-Zahrawi</t>
         </is>
       </c>
       <c r="C164" t="inlineStr">
         <is>
-          <t>Vietnamese communist revolutionary and President of North Vietnam.</t>
+          <t>Medieval Andalusian surgeon and polymath who wrote extensively on medicine, surgery, and pharmacology, influencing medical practices for centuries.</t>
         </is>
       </c>
       <c r="D164" t="inlineStr">
         <is>
-          <t>No</t>
+          <t>Yes</t>
         </is>
       </c>
       <c r="E164" t="inlineStr">
         <is>
-          <t>No</t>
+          <t>Yes</t>
         </is>
       </c>
       <c r="F164" t="inlineStr">
@@ -8339,7 +8339,7 @@
       <c r="I164" t="inlineStr"/>
       <c r="J164" t="inlineStr">
         <is>
-          <t>Please provide me with 10 long and interesting facts about Ho Chi Minh. I have a youtube channel based on influential figures so this information must be accurate as my channel depends on it. Please make the output of the facts at least 700 words long. Thank you.</t>
+          <t>Please provide me with 10 long and interesting facts about Abu al-Qasim al-Zahrawi. I have a youtube channel based on influential figures so this information must be accurate as my channel depends on it. Please make the output of the facts at least 700 words long. Thank you.</t>
         </is>
       </c>
     </row>
@@ -8349,22 +8349,22 @@
       </c>
       <c r="B165" t="inlineStr">
         <is>
-          <t>Jelimo Pamela</t>
+          <t>Enheduanna</t>
         </is>
       </c>
       <c r="C165" t="inlineStr">
         <is>
-          <t>Kenyan middle-distance runner, Olympic gold medalist.</t>
+          <t>High priestess of the moon god Nanna in ancient Sumer, credited as one of the earliest known authors and poets in history.</t>
         </is>
       </c>
       <c r="D165" t="inlineStr">
         <is>
-          <t>No</t>
+          <t>Yes</t>
         </is>
       </c>
       <c r="E165" t="inlineStr">
         <is>
-          <t>No</t>
+          <t>Yes</t>
         </is>
       </c>
       <c r="F165" t="inlineStr">
@@ -8385,7 +8385,7 @@
       <c r="I165" t="inlineStr"/>
       <c r="J165" t="inlineStr">
         <is>
-          <t>Please provide me with 10 long and interesting facts about Jelimo Pamela. I have a youtube channel based on influential figures so this information must be accurate as my channel depends on it. Please make the output of the facts at least 700 words long. Thank you.</t>
+          <t>Please provide me with 10 long and interesting facts about Enheduanna. I have a youtube channel based on influential figures so this information must be accurate as my channel depends on it. Please make the output of the facts at least 700 words long. Thank you.</t>
         </is>
       </c>
     </row>
@@ -8395,22 +8395,22 @@
       </c>
       <c r="B166" t="inlineStr">
         <is>
-          <t>Andy Warhol</t>
+          <t>Blessing Okagbare</t>
         </is>
       </c>
       <c r="C166" t="inlineStr">
         <is>
-          <t>American pop art pioneer, known for his iconic portraits and prints.</t>
+          <t>Nigerian track and field athlete, Olympic medalist.</t>
         </is>
       </c>
       <c r="D166" t="inlineStr">
         <is>
-          <t>No</t>
+          <t>Yes</t>
         </is>
       </c>
       <c r="E166" t="inlineStr">
         <is>
-          <t>No</t>
+          <t>Yes</t>
         </is>
       </c>
       <c r="F166" t="inlineStr">
@@ -8431,7 +8431,7 @@
       <c r="I166" t="inlineStr"/>
       <c r="J166" t="inlineStr">
         <is>
-          <t>Please provide me with 10 long and interesting facts about Andy Warhol. I have a youtube channel based on influential figures so this information must be accurate as my channel depends on it. Please make the output of the facts at least 700 words long. Thank you.</t>
+          <t>Please provide me with 10 long and interesting facts about Blessing Okagbare. I have a youtube channel based on influential figures so this information must be accurate as my channel depends on it. Please make the output of the facts at least 700 words long. Thank you.</t>
         </is>
       </c>
     </row>
@@ -8441,22 +8441,22 @@
       </c>
       <c r="B167" t="inlineStr">
         <is>
-          <t>Jackson Pollock</t>
+          <t>Johann Sebastian Bach</t>
         </is>
       </c>
       <c r="C167" t="inlineStr">
         <is>
-          <t>American abstract expressionist painter, known for his unique drip painting technique.</t>
+          <t>German composer and musician, a Baroque music master.</t>
         </is>
       </c>
       <c r="D167" t="inlineStr">
         <is>
-          <t>No</t>
+          <t>Yes</t>
         </is>
       </c>
       <c r="E167" t="inlineStr">
         <is>
-          <t>No</t>
+          <t>Yes</t>
         </is>
       </c>
       <c r="F167" t="inlineStr">
@@ -8477,7 +8477,7 @@
       <c r="I167" t="inlineStr"/>
       <c r="J167" t="inlineStr">
         <is>
-          <t>Please provide me with 10 long and interesting facts about Jackson Pollock. I have a youtube channel based on influential figures so this information must be accurate as my channel depends on it. Please make the output of the facts at least 700 words long. Thank you.</t>
+          <t>Please provide me with 10 long and interesting facts about Johann Sebastian Bach. I have a youtube channel based on influential figures so this information must be accurate as my channel depends on it. Please make the output of the facts at least 700 words long. Thank you.</t>
         </is>
       </c>
     </row>
@@ -8487,22 +8487,22 @@
       </c>
       <c r="B168" t="inlineStr">
         <is>
-          <t>Betty Friedan</t>
+          <t>Mustafa Kemal Atatürk</t>
         </is>
       </c>
       <c r="C168" t="inlineStr">
         <is>
-          <t>Author of the book "The Feminine Mystique," which helped to spark the second wave of the feminist movement.</t>
+          <t>Founder and first President of Turkey, known for modernizing reforms.</t>
         </is>
       </c>
       <c r="D168" t="inlineStr">
         <is>
-          <t>No</t>
+          <t>Yes</t>
         </is>
       </c>
       <c r="E168" t="inlineStr">
         <is>
-          <t>No</t>
+          <t>Yes</t>
         </is>
       </c>
       <c r="F168" t="inlineStr">
@@ -8523,7 +8523,7 @@
       <c r="I168" t="inlineStr"/>
       <c r="J168" t="inlineStr">
         <is>
-          <t>Please provide me with 10 long and interesting facts about Betty Friedan. I have a youtube channel based on influential figures so this information must be accurate as my channel depends on it. Please make the output of the facts at least 700 words long. Thank you.</t>
+          <t>Please provide me with 10 long and interesting facts about Mustafa Kemal Atatürk. I have a youtube channel based on influential figures so this information must be accurate as my channel depends on it. Please make the output of the facts at least 700 words long. Thank you.</t>
         </is>
       </c>
     </row>
@@ -8533,22 +8533,22 @@
       </c>
       <c r="B169" t="inlineStr">
         <is>
-          <t>Blessing Oborududu</t>
+          <t>Al-Maʿarri</t>
         </is>
       </c>
       <c r="C169" t="inlineStr">
         <is>
-          <t>Nigerian wrestler, first African female wrestling Olympic medalist.</t>
+          <t>Arabian philosopher and poet in the 11th century, known for his skepticism and critical views on religious and societal norms.</t>
         </is>
       </c>
       <c r="D169" t="inlineStr">
         <is>
-          <t>No</t>
+          <t>Yes</t>
         </is>
       </c>
       <c r="E169" t="inlineStr">
         <is>
-          <t>No</t>
+          <t>Yes</t>
         </is>
       </c>
       <c r="F169" t="inlineStr">
@@ -8569,7 +8569,7 @@
       <c r="I169" t="inlineStr"/>
       <c r="J169" t="inlineStr">
         <is>
-          <t>Please provide me with 10 long and interesting facts about Blessing Oborududu. I have a youtube channel based on influential figures so this information must be accurate as my channel depends on it. Please make the output of the facts at least 700 words long. Thank you.</t>
+          <t>Please provide me with 10 long and interesting facts about Al-Maʿarri. I have a youtube channel based on influential figures so this information must be accurate as my channel depends on it. Please make the output of the facts at least 700 words long. Thank you.</t>
         </is>
       </c>
     </row>
@@ -8579,22 +8579,22 @@
       </c>
       <c r="B170" t="inlineStr">
         <is>
-          <t>Tomoe Gozen</t>
+          <t>Queen Nzinga</t>
         </is>
       </c>
       <c r="C170" t="inlineStr">
         <is>
-          <t>Female samurai warrior during the 12th century in Japan, renowned for her combat skills and bravery on the battlefield.</t>
+          <t>Queen of Ndongo and Matamba, skilled diplomat.</t>
         </is>
       </c>
       <c r="D170" t="inlineStr">
         <is>
-          <t>No</t>
+          <t>Yes</t>
         </is>
       </c>
       <c r="E170" t="inlineStr">
         <is>
-          <t>No</t>
+          <t>Yes</t>
         </is>
       </c>
       <c r="F170" t="inlineStr">
@@ -8615,7 +8615,7 @@
       <c r="I170" t="inlineStr"/>
       <c r="J170" t="inlineStr">
         <is>
-          <t>Please provide me with 10 long and interesting facts about Tomoe Gozen. I have a youtube channel based on influential figures so this information must be accurate as my channel depends on it. Please make the output of the facts at least 700 words long. Thank you.</t>
+          <t>Please provide me with 10 long and interesting facts about Queen Nzinga. I have a youtube channel based on influential figures so this information must be accurate as my channel depends on it. Please make the output of the facts at least 700 words long. Thank you.</t>
         </is>
       </c>
     </row>
@@ -8625,22 +8625,22 @@
       </c>
       <c r="B171" t="inlineStr">
         <is>
-          <t>Daenerys Targaryen</t>
+          <t>Jim Thorpe</t>
         </is>
       </c>
       <c r="C171" t="inlineStr">
         <is>
-          <t>A fictional character in the "Game of Thrones" series, she is a powerful and inspiring leader.</t>
+          <t>American multi-sport athlete, Olympic gold medalist and football legend.</t>
         </is>
       </c>
       <c r="D171" t="inlineStr">
         <is>
-          <t>No</t>
+          <t>Yes</t>
         </is>
       </c>
       <c r="E171" t="inlineStr">
         <is>
-          <t>No</t>
+          <t>Yes</t>
         </is>
       </c>
       <c r="F171" t="inlineStr">
@@ -8661,7 +8661,7 @@
       <c r="I171" t="inlineStr"/>
       <c r="J171" t="inlineStr">
         <is>
-          <t>Please provide me with 10 long and interesting facts about Daenerys Targaryen. I have a youtube channel based on influential figures so this information must be accurate as my channel depends on it. Please make the output of the facts at least 700 words long. Thank you.</t>
+          <t>Please provide me with 10 long and interesting facts about Jim Thorpe. I have a youtube channel based on influential figures so this information must be accurate as my channel depends on it. Please make the output of the facts at least 700 words long. Thank you.</t>
         </is>
       </c>
     </row>
@@ -8671,22 +8671,22 @@
       </c>
       <c r="B172" t="inlineStr">
         <is>
-          <t>Frank Sinatra</t>
+          <t>Wassily Kandinsky</t>
         </is>
       </c>
       <c r="C172" t="inlineStr">
         <is>
-          <t>American singer and actor, known for his timeless classics.</t>
+          <t>Russian abstract painter, one of the pioneers of abstract art.</t>
         </is>
       </c>
       <c r="D172" t="inlineStr">
         <is>
-          <t>No</t>
+          <t>Yes</t>
         </is>
       </c>
       <c r="E172" t="inlineStr">
         <is>
-          <t>No</t>
+          <t>Yes</t>
         </is>
       </c>
       <c r="F172" t="inlineStr">
@@ -8707,7 +8707,7 @@
       <c r="I172" t="inlineStr"/>
       <c r="J172" t="inlineStr">
         <is>
-          <t>Please provide me with 10 long and interesting facts about Frank Sinatra. I have a youtube channel based on influential figures so this information must be accurate as my channel depends on it. Please make the output of the facts at least 700 words long. Thank you.</t>
+          <t>Please provide me with 10 long and interesting facts about Wassily Kandinsky. I have a youtube channel based on influential figures so this information must be accurate as my channel depends on it. Please make the output of the facts at least 700 words long. Thank you.</t>
         </is>
       </c>
     </row>
@@ -8717,22 +8717,22 @@
       </c>
       <c r="B173" t="inlineStr">
         <is>
-          <t>Yaya Touré</t>
+          <t>Queen Ranavalona III</t>
         </is>
       </c>
       <c r="C173" t="inlineStr">
         <is>
-          <t>Ivorian footballer and four-time African Player of the Year.</t>
+          <t>Last sovereign of the Kingdom of Madagascar.</t>
         </is>
       </c>
       <c r="D173" t="inlineStr">
         <is>
-          <t>No</t>
+          <t>Yes</t>
         </is>
       </c>
       <c r="E173" t="inlineStr">
         <is>
-          <t>No</t>
+          <t>Yes</t>
         </is>
       </c>
       <c r="F173" t="inlineStr">
@@ -8753,7 +8753,7 @@
       <c r="I173" t="inlineStr"/>
       <c r="J173" t="inlineStr">
         <is>
-          <t>Please provide me with 10 long and interesting facts about Yaya Touré. I have a youtube channel based on influential figures so this information must be accurate as my channel depends on it. Please make the output of the facts at least 700 words long. Thank you.</t>
+          <t>Please provide me with 10 long and interesting facts about Queen Ranavalona III. I have a youtube channel based on influential figures so this information must be accurate as my channel depends on it. Please make the output of the facts at least 700 words long. Thank you.</t>
         </is>
       </c>
     </row>
@@ -8763,22 +8763,22 @@
       </c>
       <c r="B174" t="inlineStr">
         <is>
-          <t>Steve Biko</t>
+          <t>Ho Chi Minh</t>
         </is>
       </c>
       <c r="C174" t="inlineStr">
         <is>
-          <t>Black Consciousness Movement leader in South Africa.</t>
+          <t>Vietnamese communist revolutionary and President of North Vietnam.</t>
         </is>
       </c>
       <c r="D174" t="inlineStr">
         <is>
-          <t>No</t>
+          <t>Yes</t>
         </is>
       </c>
       <c r="E174" t="inlineStr">
         <is>
-          <t>No</t>
+          <t>Yes</t>
         </is>
       </c>
       <c r="F174" t="inlineStr">
@@ -8799,7 +8799,7 @@
       <c r="I174" t="inlineStr"/>
       <c r="J174" t="inlineStr">
         <is>
-          <t>Please provide me with 10 long and interesting facts about Steve Biko. I have a youtube channel based on influential figures so this information must be accurate as my channel depends on it. Please make the output of the facts at least 700 words long. Thank you.</t>
+          <t>Please provide me with 10 long and interesting facts about Ho Chi Minh. I have a youtube channel based on influential figures so this information must be accurate as my channel depends on it. Please make the output of the facts at least 700 words long. Thank you.</t>
         </is>
       </c>
     </row>
@@ -8809,22 +8809,22 @@
       </c>
       <c r="B175" t="inlineStr">
         <is>
-          <t>Queen Ranavalona III</t>
+          <t>Qutb-ud-din Aybak</t>
         </is>
       </c>
       <c r="C175" t="inlineStr">
         <is>
-          <t>Last sovereign of the Kingdom of Madagascar.</t>
+          <t>Slave-turned-sultan who founded the Delhi Sultanate in medieval India, establishing the Mamluk dynasty and ruling over a vast empire.</t>
         </is>
       </c>
       <c r="D175" t="inlineStr">
         <is>
-          <t>No</t>
+          <t>Yes</t>
         </is>
       </c>
       <c r="E175" t="inlineStr">
         <is>
-          <t>No</t>
+          <t>Yes</t>
         </is>
       </c>
       <c r="F175" t="inlineStr">
@@ -8845,7 +8845,7 @@
       <c r="I175" t="inlineStr"/>
       <c r="J175" t="inlineStr">
         <is>
-          <t>Please provide me with 10 long and interesting facts about Queen Ranavalona III. I have a youtube channel based on influential figures so this information must be accurate as my channel depends on it. Please make the output of the facts at least 700 words long. Thank you.</t>
+          <t>Please provide me with 10 long and interesting facts about Qutb-ud-din Aybak. I have a youtube channel based on influential figures so this information must be accurate as my channel depends on it. Please make the output of the facts at least 700 words long. Thank you.</t>
         </is>
       </c>
     </row>
@@ -8855,22 +8855,22 @@
       </c>
       <c r="B176" t="inlineStr">
         <is>
-          <t>Abebe Bikila</t>
+          <t>Michelangelo</t>
         </is>
       </c>
       <c r="C176" t="inlineStr">
         <is>
-          <t>Ethiopian marathon runner and Olympic champion.</t>
+          <t>Italian sculptor, painter, and architect, known for works like the Sistine Chapel ceiling.</t>
         </is>
       </c>
       <c r="D176" t="inlineStr">
         <is>
-          <t>No</t>
+          <t>Yes</t>
         </is>
       </c>
       <c r="E176" t="inlineStr">
         <is>
-          <t>No</t>
+          <t>Yes</t>
         </is>
       </c>
       <c r="F176" t="inlineStr">
@@ -8891,7 +8891,7 @@
       <c r="I176" t="inlineStr"/>
       <c r="J176" t="inlineStr">
         <is>
-          <t>Please provide me with 10 long and interesting facts about Abebe Bikila. I have a youtube channel based on influential figures so this information must be accurate as my channel depends on it. Please make the output of the facts at least 700 words long. Thank you.</t>
+          <t>Please provide me with 10 long and interesting facts about Michelangelo. I have a youtube channel based on influential figures so this information must be accurate as my channel depends on it. Please make the output of the facts at least 700 words long. Thank you.</t>
         </is>
       </c>
     </row>
@@ -8901,22 +8901,22 @@
       </c>
       <c r="B177" t="inlineStr">
         <is>
-          <t>Patrice Lumumba</t>
+          <t>Susan B. Anthony</t>
         </is>
       </c>
       <c r="C177" t="inlineStr">
         <is>
-          <t>Independence leader, first PM of the Congo.</t>
+          <t>Fought for women's suffrage and other women's rights.</t>
         </is>
       </c>
       <c r="D177" t="inlineStr">
         <is>
-          <t>No</t>
+          <t>Yes</t>
         </is>
       </c>
       <c r="E177" t="inlineStr">
         <is>
-          <t>No</t>
+          <t>Yes</t>
         </is>
       </c>
       <c r="F177" t="inlineStr">
@@ -8937,7 +8937,7 @@
       <c r="I177" t="inlineStr"/>
       <c r="J177" t="inlineStr">
         <is>
-          <t>Please provide me with 10 long and interesting facts about Patrice Lumumba. I have a youtube channel based on influential figures so this information must be accurate as my channel depends on it. Please make the output of the facts at least 700 words long. Thank you.</t>
+          <t>Please provide me with 10 long and interesting facts about Susan B. Anthony. I have a youtube channel based on influential figures so this information must be accurate as my channel depends on it. Please make the output of the facts at least 700 words long. Thank you.</t>
         </is>
       </c>
     </row>
@@ -8947,22 +8947,22 @@
       </c>
       <c r="B178" t="inlineStr">
         <is>
-          <t>Noureddine Morceli</t>
+          <t>Stephen Keshi</t>
         </is>
       </c>
       <c r="C178" t="inlineStr">
         <is>
-          <t>Algerian middle-distance runner, Olympic gold medalist.</t>
+          <t>Nigerian footballer and coach, led Nigeria to AFCON victory.</t>
         </is>
       </c>
       <c r="D178" t="inlineStr">
         <is>
-          <t>No</t>
+          <t>Yes</t>
         </is>
       </c>
       <c r="E178" t="inlineStr">
         <is>
-          <t>No</t>
+          <t>Yes</t>
         </is>
       </c>
       <c r="F178" t="inlineStr">
@@ -8983,7 +8983,7 @@
       <c r="I178" t="inlineStr"/>
       <c r="J178" t="inlineStr">
         <is>
-          <t>Please provide me with 10 long and interesting facts about Noureddine Morceli. I have a youtube channel based on influential figures so this information must be accurate as my channel depends on it. Please make the output of the facts at least 700 words long. Thank you.</t>
+          <t>Please provide me with 10 long and interesting facts about Stephen Keshi. I have a youtube channel based on influential figures so this information must be accurate as my channel depends on it. Please make the output of the facts at least 700 words long. Thank you.</t>
         </is>
       </c>
     </row>
@@ -8993,22 +8993,22 @@
       </c>
       <c r="B179" t="inlineStr">
         <is>
-          <t>Al-Maʿarri</t>
+          <t>Golda Meir</t>
         </is>
       </c>
       <c r="C179" t="inlineStr">
         <is>
-          <t>Arabian philosopher and poet in the 11th century, known for his skepticism and critical views on religious and societal norms.</t>
+          <t>Israeli Prime Minister and one of the world's first female heads of government.</t>
         </is>
       </c>
       <c r="D179" t="inlineStr">
         <is>
-          <t>No</t>
+          <t>Yes</t>
         </is>
       </c>
       <c r="E179" t="inlineStr">
         <is>
-          <t>No</t>
+          <t>Yes</t>
         </is>
       </c>
       <c r="F179" t="inlineStr">
@@ -9029,7 +9029,7 @@
       <c r="I179" t="inlineStr"/>
       <c r="J179" t="inlineStr">
         <is>
-          <t>Please provide me with 10 long and interesting facts about Al-Maʿarri. I have a youtube channel based on influential figures so this information must be accurate as my channel depends on it. Please make the output of the facts at least 700 words long. Thank you.</t>
+          <t>Please provide me with 10 long and interesting facts about Golda Meir. I have a youtube channel based on influential figures so this information must be accurate as my channel depends on it. Please make the output of the facts at least 700 words long. Thank you.</t>
         </is>
       </c>
     </row>
@@ -9039,22 +9039,22 @@
       </c>
       <c r="B180" t="inlineStr">
         <is>
-          <t>Yayoi Kusama</t>
+          <t>Seondeok of Silla</t>
         </is>
       </c>
       <c r="C180" t="inlineStr">
         <is>
-          <t>Japanese contemporary artist, known for her immersive installations and polka dot motifs.</t>
+          <t>Queen of the Silla Kingdom in ancient Korea during the 7th century CE, remembered for her strong leadership and advancements in science and culture.</t>
         </is>
       </c>
       <c r="D180" t="inlineStr">
         <is>
-          <t>No</t>
+          <t>Yes</t>
         </is>
       </c>
       <c r="E180" t="inlineStr">
         <is>
-          <t>No</t>
+          <t>Yes</t>
         </is>
       </c>
       <c r="F180" t="inlineStr">
@@ -9075,7 +9075,7 @@
       <c r="I180" t="inlineStr"/>
       <c r="J180" t="inlineStr">
         <is>
-          <t>Please provide me with 10 long and interesting facts about Yayoi Kusama. I have a youtube channel based on influential figures so this information must be accurate as my channel depends on it. Please make the output of the facts at least 700 words long. Thank you.</t>
+          <t>Please provide me with 10 long and interesting facts about Seondeok of Silla. I have a youtube channel based on influential figures so this information must be accurate as my channel depends on it. Please make the output of the facts at least 700 words long. Thank you.</t>
         </is>
       </c>
     </row>
@@ -9085,22 +9085,22 @@
       </c>
       <c r="B181" t="inlineStr">
         <is>
-          <t>Bob Marley</t>
+          <t>Mao Zedong</t>
         </is>
       </c>
       <c r="C181" t="inlineStr">
         <is>
-          <t>Jamaican reggae icon, known for his messages of unity and peace.</t>
+          <t>Chinese communist revolutionary and founding father of the People's Republic of China.</t>
         </is>
       </c>
       <c r="D181" t="inlineStr">
         <is>
-          <t>No</t>
+          <t>Yes</t>
         </is>
       </c>
       <c r="E181" t="inlineStr">
         <is>
-          <t>No</t>
+          <t>Yes</t>
         </is>
       </c>
       <c r="F181" t="inlineStr">
@@ -9121,7 +9121,7 @@
       <c r="I181" t="inlineStr"/>
       <c r="J181" t="inlineStr">
         <is>
-          <t>Please provide me with 10 long and interesting facts about Bob Marley. I have a youtube channel based on influential figures so this information must be accurate as my channel depends on it. Please make the output of the facts at least 700 words long. Thank you.</t>
+          <t>Please provide me with 10 long and interesting facts about Mao Zedong. I have a youtube channel based on influential figures so this information must be accurate as my channel depends on it. Please make the output of the facts at least 700 words long. Thank you.</t>
         </is>
       </c>
     </row>
@@ -9131,22 +9131,22 @@
       </c>
       <c r="B182" t="inlineStr">
         <is>
-          <t>Jomo Kenyatta</t>
+          <t>John Lennon</t>
         </is>
       </c>
       <c r="C182" t="inlineStr">
         <is>
-          <t>Founding father and first president of Kenya.</t>
+          <t>British singer, songwriter, and member of The Beatles.</t>
         </is>
       </c>
       <c r="D182" t="inlineStr">
         <is>
-          <t>No</t>
+          <t>Yes</t>
         </is>
       </c>
       <c r="E182" t="inlineStr">
         <is>
-          <t>No</t>
+          <t>Yes</t>
         </is>
       </c>
       <c r="F182" t="inlineStr">
@@ -9167,7 +9167,7 @@
       <c r="I182" t="inlineStr"/>
       <c r="J182" t="inlineStr">
         <is>
-          <t>Please provide me with 10 long and interesting facts about Jomo Kenyatta. I have a youtube channel based on influential figures so this information must be accurate as my channel depends on it. Please make the output of the facts at least 700 words long. Thank you.</t>
+          <t>Please provide me with 10 long and interesting facts about John Lennon. I have a youtube channel based on influential figures so this information must be accurate as my channel depends on it. Please make the output of the facts at least 700 words long. Thank you.</t>
         </is>
       </c>
     </row>
@@ -9177,22 +9177,22 @@
       </c>
       <c r="B183" t="inlineStr">
         <is>
-          <t>Mao Zedong</t>
+          <t>David Bowie</t>
         </is>
       </c>
       <c r="C183" t="inlineStr">
         <is>
-          <t>Chinese communist revolutionary and founding father of the People's Republic of China.</t>
+          <t>British singer and musician, known for his innovation and artistic style.</t>
         </is>
       </c>
       <c r="D183" t="inlineStr">
         <is>
-          <t>No</t>
+          <t>Yes</t>
         </is>
       </c>
       <c r="E183" t="inlineStr">
         <is>
-          <t>No</t>
+          <t>Yes</t>
         </is>
       </c>
       <c r="F183" t="inlineStr">
@@ -9213,7 +9213,7 @@
       <c r="I183" t="inlineStr"/>
       <c r="J183" t="inlineStr">
         <is>
-          <t>Please provide me with 10 long and interesting facts about Mao Zedong. I have a youtube channel based on influential figures so this information must be accurate as my channel depends on it. Please make the output of the facts at least 700 words long. Thank you.</t>
+          <t>Please provide me with 10 long and interesting facts about David Bowie. I have a youtube channel based on influential figures so this information must be accurate as my channel depends on it. Please make the output of the facts at least 700 words long. Thank you.</t>
         </is>
       </c>
     </row>
@@ -9223,22 +9223,22 @@
       </c>
       <c r="B184" t="inlineStr">
         <is>
-          <t>Ahmed Sékou Touré</t>
+          <t>Blessing Awodibu</t>
         </is>
       </c>
       <c r="C184" t="inlineStr">
         <is>
-          <t>Guinea's first president and anti-colonial leader.</t>
+          <t>South African bodybuilder and social media influencer.</t>
         </is>
       </c>
       <c r="D184" t="inlineStr">
         <is>
-          <t>No</t>
+          <t>Yes</t>
         </is>
       </c>
       <c r="E184" t="inlineStr">
         <is>
-          <t>No</t>
+          <t>Yes</t>
         </is>
       </c>
       <c r="F184" t="inlineStr">
@@ -9259,7 +9259,7 @@
       <c r="I184" t="inlineStr"/>
       <c r="J184" t="inlineStr">
         <is>
-          <t>Please provide me with 10 long and interesting facts about Ahmed Sékou Touré. I have a youtube channel based on influential figures so this information must be accurate as my channel depends on it. Please make the output of the facts at least 700 words long. Thank you.</t>
+          <t>Please provide me with 10 long and interesting facts about Blessing Awodibu. I have a youtube channel based on influential figures so this information must be accurate as my channel depends on it. Please make the output of the facts at least 700 words long. Thank you.</t>
         </is>
       </c>
     </row>
@@ -9269,22 +9269,22 @@
       </c>
       <c r="B185" t="inlineStr">
         <is>
-          <t>Jim Henson</t>
+          <t>Jelimo Pamela</t>
         </is>
       </c>
       <c r="C185" t="inlineStr">
         <is>
-          <t>One of the most influential puppeteers of all time, he created some of the most beloved characters in television history.</t>
+          <t>Kenyan middle-distance runner, Olympic gold medalist.</t>
         </is>
       </c>
       <c r="D185" t="inlineStr">
         <is>
-          <t>No</t>
+          <t>Yes</t>
         </is>
       </c>
       <c r="E185" t="inlineStr">
         <is>
-          <t>No</t>
+          <t>Yes</t>
         </is>
       </c>
       <c r="F185" t="inlineStr">
@@ -9305,7 +9305,7 @@
       <c r="I185" t="inlineStr"/>
       <c r="J185" t="inlineStr">
         <is>
-          <t>Please provide me with 10 long and interesting facts about Jim Henson. I have a youtube channel based on influential figures so this information must be accurate as my channel depends on it. Please make the output of the facts at least 700 words long. Thank you.</t>
+          <t>Please provide me with 10 long and interesting facts about Jelimo Pamela. I have a youtube channel based on influential figures so this information must be accurate as my channel depends on it. Please make the output of the facts at least 700 words long. Thank you.</t>
         </is>
       </c>
     </row>
@@ -9315,22 +9315,22 @@
       </c>
       <c r="B186" t="inlineStr">
         <is>
-          <t>Chen Guangcheng</t>
+          <t>Yaa Asantewaa</t>
         </is>
       </c>
       <c r="C186" t="inlineStr">
         <is>
-          <t>Fought for the rights of people with disabilities in China and was imprisoned for his activism.</t>
+          <t>Ashanti queen mother, led an anti-colonial rebellion.</t>
         </is>
       </c>
       <c r="D186" t="inlineStr">
         <is>
-          <t>No</t>
+          <t>Yes</t>
         </is>
       </c>
       <c r="E186" t="inlineStr">
         <is>
-          <t>No</t>
+          <t>Yes</t>
         </is>
       </c>
       <c r="F186" t="inlineStr">
@@ -9351,7 +9351,7 @@
       <c r="I186" t="inlineStr"/>
       <c r="J186" t="inlineStr">
         <is>
-          <t>Please provide me with 10 long and interesting facts about Chen Guangcheng. I have a youtube channel based on influential figures so this information must be accurate as my channel depends on it. Please make the output of the facts at least 700 words long. Thank you.</t>
+          <t>Please provide me with 10 long and interesting facts about Yaa Asantewaa. I have a youtube channel based on influential figures so this information must be accurate as my channel depends on it. Please make the output of the facts at least 700 words long. Thank you.</t>
         </is>
       </c>
     </row>
@@ -9361,22 +9361,22 @@
       </c>
       <c r="B187" t="inlineStr">
         <is>
-          <t>Jacqueline Kennedy Onassis</t>
+          <t>Ahmed Sékou Touré</t>
         </is>
       </c>
       <c r="C187" t="inlineStr">
         <is>
-          <t>One of the most popular First Ladies of the 20th century, she was also a successful author.</t>
+          <t>Guinea's first president and anti-colonial leader.</t>
         </is>
       </c>
       <c r="D187" t="inlineStr">
         <is>
-          <t>No</t>
+          <t>Yes</t>
         </is>
       </c>
       <c r="E187" t="inlineStr">
         <is>
-          <t>No</t>
+          <t>Yes</t>
         </is>
       </c>
       <c r="F187" t="inlineStr">
@@ -9397,7 +9397,7 @@
       <c r="I187" t="inlineStr"/>
       <c r="J187" t="inlineStr">
         <is>
-          <t>Please provide me with 10 long and interesting facts about Jacqueline Kennedy Onassis. I have a youtube channel based on influential figures so this information must be accurate as my channel depends on it. Please make the output of the facts at least 700 words long. Thank you.</t>
+          <t>Please provide me with 10 long and interesting facts about Ahmed Sékou Touré. I have a youtube channel based on influential figures so this information must be accurate as my channel depends on it. Please make the output of the facts at least 700 words long. Thank you.</t>
         </is>
       </c>
     </row>
@@ -9407,22 +9407,22 @@
       </c>
       <c r="B188" t="inlineStr">
         <is>
-          <t>Didier Drogba</t>
+          <t>Yaya Touré</t>
         </is>
       </c>
       <c r="C188" t="inlineStr">
         <is>
-          <t>Ivorian footballer and humanitarian.</t>
+          <t>Ivorian footballer and four-time African Player of the Year.</t>
         </is>
       </c>
       <c r="D188" t="inlineStr">
         <is>
-          <t>No</t>
+          <t>Yes</t>
         </is>
       </c>
       <c r="E188" t="inlineStr">
         <is>
-          <t>No</t>
+          <t>Yes</t>
         </is>
       </c>
       <c r="F188" t="inlineStr">
@@ -9443,7 +9443,7 @@
       <c r="I188" t="inlineStr"/>
       <c r="J188" t="inlineStr">
         <is>
-          <t>Please provide me with 10 long and interesting facts about Didier Drogba. I have a youtube channel based on influential figures so this information must be accurate as my channel depends on it. Please make the output of the facts at least 700 words long. Thank you.</t>
+          <t>Please provide me with 10 long and interesting facts about Yaya Touré. I have a youtube channel based on influential figures so this information must be accurate as my channel depends on it. Please make the output of the facts at least 700 words long. Thank you.</t>
         </is>
       </c>
     </row>
@@ -9453,22 +9453,22 @@
       </c>
       <c r="B189" t="inlineStr">
         <is>
-          <t>Henri Cartier-Bresson</t>
+          <t>Ono no Komachi</t>
         </is>
       </c>
       <c r="C189" t="inlineStr">
         <is>
-          <t>French photographer, considered the father of modern photojournalism.</t>
+          <t>Japanese poet in the 9th century, one of the "Six Immortals of Poetry" known for her lyrical and emotional verses.</t>
         </is>
       </c>
       <c r="D189" t="inlineStr">
         <is>
-          <t>No</t>
+          <t>Yes</t>
         </is>
       </c>
       <c r="E189" t="inlineStr">
         <is>
-          <t>No</t>
+          <t>Yes</t>
         </is>
       </c>
       <c r="F189" t="inlineStr">
@@ -9489,7 +9489,7 @@
       <c r="I189" t="inlineStr"/>
       <c r="J189" t="inlineStr">
         <is>
-          <t>Please provide me with 10 long and interesting facts about Henri Cartier-Bresson. I have a youtube channel based on influential figures so this information must be accurate as my channel depends on it. Please make the output of the facts at least 700 words long. Thank you.</t>
+          <t>Please provide me with 10 long and interesting facts about Ono no Komachi. I have a youtube channel based on influential figures so this information must be accurate as my channel depends on it. Please make the output of the facts at least 700 words long. Thank you.</t>
         </is>
       </c>
     </row>
@@ -9499,22 +9499,22 @@
       </c>
       <c r="B190" t="inlineStr">
         <is>
-          <t>Ibn Battuta</t>
+          <t>Khutulun</t>
         </is>
       </c>
       <c r="C190" t="inlineStr">
         <is>
-          <t>Moroccan explorer and scholar who embarked on extensive travels throughout the Islamic world, chronicling his journeys in his renowned travelogue.</t>
+          <t>Mongol princess and skilled warrior in the 13th century, renowned for her wrestling abilities and her requirement that potential suitors defeat her in combat.</t>
         </is>
       </c>
       <c r="D190" t="inlineStr">
         <is>
-          <t>No</t>
+          <t>Yes</t>
         </is>
       </c>
       <c r="E190" t="inlineStr">
         <is>
-          <t>No</t>
+          <t>Yes</t>
         </is>
       </c>
       <c r="F190" t="inlineStr">
@@ -9535,7 +9535,7 @@
       <c r="I190" t="inlineStr"/>
       <c r="J190" t="inlineStr">
         <is>
-          <t>Please provide me with 10 long and interesting facts about Ibn Battuta. I have a youtube channel based on influential figures so this information must be accurate as my channel depends on it. Please make the output of the facts at least 700 words long. Thank you.</t>
+          <t>Please provide me with 10 long and interesting facts about Khutulun. I have a youtube channel based on influential figures so this information must be accurate as my channel depends on it. Please make the output of the facts at least 700 words long. Thank you.</t>
         </is>
       </c>
     </row>
@@ -9545,22 +9545,22 @@
       </c>
       <c r="B191" t="inlineStr">
         <is>
-          <t>Vivian Cheruiyot</t>
+          <t>Antonio Vivaldi</t>
         </is>
       </c>
       <c r="C191" t="inlineStr">
         <is>
-          <t>Kenyan long-distance runner, Olympic gold medalist.</t>
+          <t>Italian composer, famous for "The Four Seasons."</t>
         </is>
       </c>
       <c r="D191" t="inlineStr">
         <is>
-          <t>No</t>
+          <t>Yes</t>
         </is>
       </c>
       <c r="E191" t="inlineStr">
         <is>
-          <t>No</t>
+          <t>Yes</t>
         </is>
       </c>
       <c r="F191" t="inlineStr">
@@ -9581,7 +9581,7 @@
       <c r="I191" t="inlineStr"/>
       <c r="J191" t="inlineStr">
         <is>
-          <t>Please provide me with 10 long and interesting facts about Vivian Cheruiyot. I have a youtube channel based on influential figures so this information must be accurate as my channel depends on it. Please make the output of the facts at least 700 words long. Thank you.</t>
+          <t>Please provide me with 10 long and interesting facts about Antonio Vivaldi. I have a youtube channel based on influential figures so this information must be accurate as my channel depends on it. Please make the output of the facts at least 700 words long. Thank you.</t>
         </is>
       </c>
     </row>
@@ -9591,22 +9591,22 @@
       </c>
       <c r="B192" t="inlineStr">
         <is>
-          <t>Martina Navratilova</t>
+          <t>Hicham El Guerrouj</t>
         </is>
       </c>
       <c r="C192" t="inlineStr">
         <is>
-          <t>Czech-American tennis player, considered one of the greatest female players.</t>
+          <t>Moroccan middle-distance runner, Olympic gold medalist.</t>
         </is>
       </c>
       <c r="D192" t="inlineStr">
         <is>
-          <t>No</t>
+          <t>Yes</t>
         </is>
       </c>
       <c r="E192" t="inlineStr">
         <is>
-          <t>No</t>
+          <t>Yes</t>
         </is>
       </c>
       <c r="F192" t="inlineStr">
@@ -9627,7 +9627,7 @@
       <c r="I192" t="inlineStr"/>
       <c r="J192" t="inlineStr">
         <is>
-          <t>Please provide me with 10 long and interesting facts about Martina Navratilova. I have a youtube channel based on influential figures so this information must be accurate as my channel depends on it. Please make the output of the facts at least 700 words long. Thank you.</t>
+          <t>Please provide me with 10 long and interesting facts about Hicham El Guerrouj. I have a youtube channel based on influential figures so this information must be accurate as my channel depends on it. Please make the output of the facts at least 700 words long. Thank you.</t>
         </is>
       </c>
     </row>
@@ -9637,22 +9637,22 @@
       </c>
       <c r="B193" t="inlineStr">
         <is>
-          <t>Jim Thorpe</t>
+          <t>Kipchoge Keino</t>
         </is>
       </c>
       <c r="C193" t="inlineStr">
         <is>
-          <t>American multi-sport athlete, Olympic gold medalist and football legend.</t>
+          <t>Kenyan middle-distance runner, Olympic gold medalist.</t>
         </is>
       </c>
       <c r="D193" t="inlineStr">
         <is>
-          <t>No</t>
+          <t>Yes</t>
         </is>
       </c>
       <c r="E193" t="inlineStr">
         <is>
-          <t>No</t>
+          <t>Yes</t>
         </is>
       </c>
       <c r="F193" t="inlineStr">
@@ -9673,7 +9673,7 @@
       <c r="I193" t="inlineStr"/>
       <c r="J193" t="inlineStr">
         <is>
-          <t>Please provide me with 10 long and interesting facts about Jim Thorpe. I have a youtube channel based on influential figures so this information must be accurate as my channel depends on it. Please make the output of the facts at least 700 words long. Thank you.</t>
+          <t>Please provide me with 10 long and interesting facts about Kipchoge Keino. I have a youtube channel based on influential figures so this information must be accurate as my channel depends on it. Please make the output of the facts at least 700 words long. Thank you.</t>
         </is>
       </c>
     </row>
@@ -9683,22 +9683,22 @@
       </c>
       <c r="B194" t="inlineStr">
         <is>
-          <t>Henri Matisse</t>
+          <t>W.E.B. Du Bois</t>
         </is>
       </c>
       <c r="C194" t="inlineStr">
         <is>
-          <t>French artist, known for his colorful and innovative use of shapes and patterns.</t>
+          <t>One of the most important figures in the American civil rights movement, he was a scholar, writer, and activist.</t>
         </is>
       </c>
       <c r="D194" t="inlineStr">
         <is>
-          <t>No</t>
+          <t>Yes</t>
         </is>
       </c>
       <c r="E194" t="inlineStr">
         <is>
-          <t>No</t>
+          <t>Yes</t>
         </is>
       </c>
       <c r="F194" t="inlineStr">
@@ -9719,7 +9719,7 @@
       <c r="I194" t="inlineStr"/>
       <c r="J194" t="inlineStr">
         <is>
-          <t>Please provide me with 10 long and interesting facts about Henri Matisse. I have a youtube channel based on influential figures so this information must be accurate as my channel depends on it. Please make the output of the facts at least 700 words long. Thank you.</t>
+          <t>Please provide me with 10 long and interesting facts about W.E.B. Du Bois. I have a youtube channel based on influential figures so this information must be accurate as my channel depends on it. Please make the output of the facts at least 700 words long. Thank you.</t>
         </is>
       </c>
     </row>
@@ -9729,22 +9729,22 @@
       </c>
       <c r="B195" t="inlineStr">
         <is>
-          <t>Al-Kindi</t>
+          <t>George Best</t>
         </is>
       </c>
       <c r="C195" t="inlineStr">
         <is>
-          <t>Arab philosopher and polymath in the 9th century, making significant contributions to mathematics, astronomy, and philosophy.</t>
+          <t>Northern Irish footballer, known for his incredible skill.</t>
         </is>
       </c>
       <c r="D195" t="inlineStr">
         <is>
-          <t>No</t>
+          <t>Yes</t>
         </is>
       </c>
       <c r="E195" t="inlineStr">
         <is>
-          <t>No</t>
+          <t>Yes</t>
         </is>
       </c>
       <c r="F195" t="inlineStr">
@@ -9765,7 +9765,7 @@
       <c r="I195" t="inlineStr"/>
       <c r="J195" t="inlineStr">
         <is>
-          <t>Please provide me with 10 long and interesting facts about Al-Kindi. I have a youtube channel based on influential figures so this information must be accurate as my channel depends on it. Please make the output of the facts at least 700 words long. Thank you.</t>
+          <t>Please provide me with 10 long and interesting facts about George Best. I have a youtube channel based on influential figures so this information must be accurate as my channel depends on it. Please make the output of the facts at least 700 words long. Thank you.</t>
         </is>
       </c>
     </row>
@@ -9775,22 +9775,22 @@
       </c>
       <c r="B196" t="inlineStr">
         <is>
-          <t>Johann Sebastian Bach</t>
+          <t>Steve Biko</t>
         </is>
       </c>
       <c r="C196" t="inlineStr">
         <is>
-          <t>German composer and musician, a Baroque music master.</t>
+          <t>Black Consciousness Movement leader in South Africa.</t>
         </is>
       </c>
       <c r="D196" t="inlineStr">
         <is>
-          <t>No</t>
+          <t>Yes</t>
         </is>
       </c>
       <c r="E196" t="inlineStr">
         <is>
-          <t>No</t>
+          <t>Yes</t>
         </is>
       </c>
       <c r="F196" t="inlineStr">
@@ -9811,7 +9811,7 @@
       <c r="I196" t="inlineStr"/>
       <c r="J196" t="inlineStr">
         <is>
-          <t>Please provide me with 10 long and interesting facts about Johann Sebastian Bach. I have a youtube channel based on influential figures so this information must be accurate as my channel depends on it. Please make the output of the facts at least 700 words long. Thank you.</t>
+          <t>Please provide me with 10 long and interesting facts about Steve Biko. I have a youtube channel based on influential figures so this information must be accurate as my channel depends on it. Please make the output of the facts at least 700 words long. Thank you.</t>
         </is>
       </c>
     </row>
@@ -9821,22 +9821,22 @@
       </c>
       <c r="B197" t="inlineStr">
         <is>
-          <t>Martina Hingis</t>
+          <t>Blessing Oborududu</t>
         </is>
       </c>
       <c r="C197" t="inlineStr">
         <is>
-          <t>Swiss tennis player, former world No. 1 and multiple Grand Slam winner.</t>
+          <t>Nigerian wrestler, first African female wrestling Olympic medalist.</t>
         </is>
       </c>
       <c r="D197" t="inlineStr">
         <is>
-          <t>No</t>
+          <t>Yes</t>
         </is>
       </c>
       <c r="E197" t="inlineStr">
         <is>
-          <t>No</t>
+          <t>Yes</t>
         </is>
       </c>
       <c r="F197" t="inlineStr">
@@ -9857,7 +9857,7 @@
       <c r="I197" t="inlineStr"/>
       <c r="J197" t="inlineStr">
         <is>
-          <t>Please provide me with 10 long and interesting facts about Martina Hingis. I have a youtube channel based on influential figures so this information must be accurate as my channel depends on it. Please make the output of the facts at least 700 words long. Thank you.</t>
+          <t>Please provide me with 10 long and interesting facts about Blessing Oborududu. I have a youtube channel based on influential figures so this information must be accurate as my channel depends on it. Please make the output of the facts at least 700 words long. Thank you.</t>
         </is>
       </c>
     </row>
@@ -9867,22 +9867,22 @@
       </c>
       <c r="B198" t="inlineStr">
         <is>
-          <t>Ellen Johnson Sirleaf</t>
+          <t>Franklin D. Roosevelt</t>
         </is>
       </c>
       <c r="C198" t="inlineStr">
         <is>
-          <t>First female president in Africa and Nobel laureate.</t>
+          <t>32nd President of the United States, led the nation through the Great Depression and World War II.</t>
         </is>
       </c>
       <c r="D198" t="inlineStr">
         <is>
-          <t>No</t>
+          <t>Yes</t>
         </is>
       </c>
       <c r="E198" t="inlineStr">
         <is>
-          <t>No</t>
+          <t>Yes</t>
         </is>
       </c>
       <c r="F198" t="inlineStr">
@@ -9903,7 +9903,7 @@
       <c r="I198" t="inlineStr"/>
       <c r="J198" t="inlineStr">
         <is>
-          <t>Please provide me with 10 long and interesting facts about Ellen Johnson Sirleaf. I have a youtube channel based on influential figures so this information must be accurate as my channel depends on it. Please make the output of the facts at least 700 words long. Thank you.</t>
+          <t>Please provide me with 10 long and interesting facts about Franklin D. Roosevelt. I have a youtube channel based on influential figures so this information must be accurate as my channel depends on it. Please make the output of the facts at least 700 words long. Thank you.</t>
         </is>
       </c>
     </row>
@@ -9913,22 +9913,22 @@
       </c>
       <c r="B199" t="inlineStr">
         <is>
-          <t>Edvard Munch</t>
+          <t>Empress Jingu</t>
         </is>
       </c>
       <c r="C199" t="inlineStr">
         <is>
-          <t>Norwegian painter, known for "The Scream" and other emotionally charged works.</t>
+          <t>Legendary Japanese empress who led successful military campaigns, including the conquest of Korea, during the 3rd century.</t>
         </is>
       </c>
       <c r="D199" t="inlineStr">
         <is>
-          <t>No</t>
+          <t>Yes</t>
         </is>
       </c>
       <c r="E199" t="inlineStr">
         <is>
-          <t>No</t>
+          <t>Yes</t>
         </is>
       </c>
       <c r="F199" t="inlineStr">
@@ -9949,7 +9949,7 @@
       <c r="I199" t="inlineStr"/>
       <c r="J199" t="inlineStr">
         <is>
-          <t>Please provide me with 10 long and interesting facts about Edvard Munch. I have a youtube channel based on influential figures so this information must be accurate as my channel depends on it. Please make the output of the facts at least 700 words long. Thank you.</t>
+          <t>Please provide me with 10 long and interesting facts about Empress Jingu. I have a youtube channel based on influential figures so this information must be accurate as my channel depends on it. Please make the output of the facts at least 700 words long. Thank you.</t>
         </is>
       </c>
     </row>
@@ -9959,22 +9959,22 @@
       </c>
       <c r="B200" t="inlineStr">
         <is>
-          <t>Hakeem Olajuwon</t>
+          <t>Jackson Pollock</t>
         </is>
       </c>
       <c r="C200" t="inlineStr">
         <is>
-          <t>Nigerian-American basketball player, NBA legend.</t>
+          <t>American abstract expressionist painter, known for his unique drip painting technique.</t>
         </is>
       </c>
       <c r="D200" t="inlineStr">
         <is>
-          <t>No</t>
+          <t>Yes</t>
         </is>
       </c>
       <c r="E200" t="inlineStr">
         <is>
-          <t>No</t>
+          <t>Yes</t>
         </is>
       </c>
       <c r="F200" t="inlineStr">
@@ -9995,7 +9995,7 @@
       <c r="I200" t="inlineStr"/>
       <c r="J200" t="inlineStr">
         <is>
-          <t>Please provide me with 10 long and interesting facts about Hakeem Olajuwon. I have a youtube channel based on influential figures so this information must be accurate as my channel depends on it. Please make the output of the facts at least 700 words long. Thank you.</t>
+          <t>Please provide me with 10 long and interesting facts about Jackson Pollock. I have a youtube channel based on influential figures so this information must be accurate as my channel depends on it. Please make the output of the facts at least 700 words long. Thank you.</t>
         </is>
       </c>
     </row>
@@ -10005,22 +10005,22 @@
       </c>
       <c r="B201" t="inlineStr">
         <is>
-          <t>Harvey Milk</t>
+          <t>Mansa Musa</t>
         </is>
       </c>
       <c r="C201" t="inlineStr">
         <is>
-          <t>One of the first openly gay elected officials in the United States, he was a leading figure in the gay rights movement.</t>
+          <t>Mali's wealthiest ruler, a great patron of art and education.</t>
         </is>
       </c>
       <c r="D201" t="inlineStr">
         <is>
-          <t>No</t>
+          <t>Yes</t>
         </is>
       </c>
       <c r="E201" t="inlineStr">
         <is>
-          <t>No</t>
+          <t>Yes</t>
         </is>
       </c>
       <c r="F201" t="inlineStr">
@@ -10041,7 +10041,7 @@
       <c r="I201" t="inlineStr"/>
       <c r="J201" t="inlineStr">
         <is>
-          <t>Please provide me with 10 long and interesting facts about Harvey Milk. I have a youtube channel based on influential figures so this information must be accurate as my channel depends on it. Please make the output of the facts at least 700 words long. Thank you.</t>
+          <t>Please provide me with 10 long and interesting facts about Mansa Musa. I have a youtube channel based on influential figures so this information must be accurate as my channel depends on it. Please make the output of the facts at least 700 words long. Thank you.</t>
         </is>
       </c>
     </row>
@@ -10051,22 +10051,22 @@
       </c>
       <c r="B202" t="inlineStr">
         <is>
-          <t>Guru Nanak</t>
+          <t>Wilhelmina Drucker</t>
         </is>
       </c>
       <c r="C202" t="inlineStr">
         <is>
-          <t>Founder of Sikhism in the 15th century, revered as the first Sikh guru and promoting the principles of equality and social justice.</t>
+          <t>One of the first women to be elected to the German parliament, she was a leading figure in the women's suffrage movement.</t>
         </is>
       </c>
       <c r="D202" t="inlineStr">
         <is>
-          <t>No</t>
+          <t>Yes</t>
         </is>
       </c>
       <c r="E202" t="inlineStr">
         <is>
-          <t>No</t>
+          <t>Yes</t>
         </is>
       </c>
       <c r="F202" t="inlineStr">
@@ -10087,7 +10087,7 @@
       <c r="I202" t="inlineStr"/>
       <c r="J202" t="inlineStr">
         <is>
-          <t>Please provide me with 10 long and interesting facts about Guru Nanak. I have a youtube channel based on influential figures so this information must be accurate as my channel depends on it. Please make the output of the facts at least 700 words long. Thank you.</t>
+          <t>Please provide me with 10 long and interesting facts about Wilhelmina Drucker. I have a youtube channel based on influential figures so this information must be accurate as my channel depends on it. Please make the output of the facts at least 700 words long. Thank you.</t>
         </is>
       </c>
     </row>
@@ -10097,22 +10097,22 @@
       </c>
       <c r="B203" t="inlineStr">
         <is>
-          <t>Ono no Komachi</t>
+          <t>Thomas Sankara</t>
         </is>
       </c>
       <c r="C203" t="inlineStr">
         <is>
-          <t>Japanese poet in the 9th century, one of the "Six Immortals of Poetry" known for her lyrical and emotional verses.</t>
+          <t>Burkina Faso's revolutionary leader and president.</t>
         </is>
       </c>
       <c r="D203" t="inlineStr">
         <is>
-          <t>No</t>
+          <t>Yes</t>
         </is>
       </c>
       <c r="E203" t="inlineStr">
         <is>
-          <t>No</t>
+          <t>Yes</t>
         </is>
       </c>
       <c r="F203" t="inlineStr">
@@ -10133,7 +10133,7 @@
       <c r="I203" t="inlineStr"/>
       <c r="J203" t="inlineStr">
         <is>
-          <t>Please provide me with 10 long and interesting facts about Ono no Komachi. I have a youtube channel based on influential figures so this information must be accurate as my channel depends on it. Please make the output of the facts at least 700 words long. Thank you.</t>
+          <t>Please provide me with 10 long and interesting facts about Thomas Sankara. I have a youtube channel based on influential figures so this information must be accurate as my channel depends on it. Please make the output of the facts at least 700 words long. Thank you.</t>
         </is>
       </c>
     </row>
@@ -10143,22 +10143,22 @@
       </c>
       <c r="B204" t="inlineStr">
         <is>
-          <t>Michael Jordan</t>
+          <t>Bob Marley</t>
         </is>
       </c>
       <c r="C204" t="inlineStr">
         <is>
-          <t>American basketball player, NBA legend.</t>
+          <t>Jamaican reggae icon, known for his messages of unity and peace.</t>
         </is>
       </c>
       <c r="D204" t="inlineStr">
         <is>
-          <t>No</t>
+          <t>Yes</t>
         </is>
       </c>
       <c r="E204" t="inlineStr">
         <is>
-          <t>No</t>
+          <t>Yes</t>
         </is>
       </c>
       <c r="F204" t="inlineStr">
@@ -10179,7 +10179,7 @@
       <c r="I204" t="inlineStr"/>
       <c r="J204" t="inlineStr">
         <is>
-          <t>Please provide me with 10 long and interesting facts about Michael Jordan. I have a youtube channel based on influential figures so this information must be accurate as my channel depends on it. Please make the output of the facts at least 700 words long. Thank you.</t>
+          <t>Please provide me with 10 long and interesting facts about Bob Marley. I have a youtube channel based on influential figures so this information must be accurate as my channel depends on it. Please make the output of the facts at least 700 words long. Thank you.</t>
         </is>
       </c>
     </row>
@@ -10189,22 +10189,22 @@
       </c>
       <c r="B205" t="inlineStr">
         <is>
-          <t>Greg Lemond</t>
+          <t>Hakeem Olajuwon</t>
         </is>
       </c>
       <c r="C205" t="inlineStr">
         <is>
-          <t>American cyclist, three-time Tour de France winner.</t>
+          <t>Nigerian-American basketball player, NBA legend.</t>
         </is>
       </c>
       <c r="D205" t="inlineStr">
         <is>
-          <t>No</t>
+          <t>Yes</t>
         </is>
       </c>
       <c r="E205" t="inlineStr">
         <is>
-          <t>No</t>
+          <t>Yes</t>
         </is>
       </c>
       <c r="F205" t="inlineStr">
@@ -10225,7 +10225,7 @@
       <c r="I205" t="inlineStr"/>
       <c r="J205" t="inlineStr">
         <is>
-          <t>Please provide me with 10 long and interesting facts about Greg Lemond. I have a youtube channel based on influential figures so this information must be accurate as my channel depends on it. Please make the output of the facts at least 700 words long. Thank you.</t>
+          <t>Please provide me with 10 long and interesting facts about Hakeem Olajuwon. I have a youtube channel based on influential figures so this information must be accurate as my channel depends on it. Please make the output of the facts at least 700 words long. Thank you.</t>
         </is>
       </c>
     </row>
@@ -10235,22 +10235,22 @@
       </c>
       <c r="B206" t="inlineStr">
         <is>
-          <t>Bjorn Borg</t>
+          <t>Benito Mussolini</t>
         </is>
       </c>
       <c r="C206" t="inlineStr">
         <is>
-          <t>Swedish tennis legend, dominated the tennis world in the late 1970s.</t>
+          <t>Italian fascist dictator during the 1920s and 1930s.</t>
         </is>
       </c>
       <c r="D206" t="inlineStr">
         <is>
-          <t>No</t>
+          <t>Yes</t>
         </is>
       </c>
       <c r="E206" t="inlineStr">
         <is>
-          <t>No</t>
+          <t>Yes</t>
         </is>
       </c>
       <c r="F206" t="inlineStr">
@@ -10271,7 +10271,7 @@
       <c r="I206" t="inlineStr"/>
       <c r="J206" t="inlineStr">
         <is>
-          <t>Please provide me with 10 long and interesting facts about Bjorn Borg. I have a youtube channel based on influential figures so this information must be accurate as my channel depends on it. Please make the output of the facts at least 700 words long. Thank you.</t>
+          <t>Please provide me with 10 long and interesting facts about Benito Mussolini. I have a youtube channel based on influential figures so this information must be accurate as my channel depends on it. Please make the output of the facts at least 700 words long. Thank you.</t>
         </is>
       </c>
     </row>
@@ -10281,22 +10281,22 @@
       </c>
       <c r="B207" t="inlineStr">
         <is>
-          <t>Kwame Nkrumah</t>
+          <t>Roy Lichtenstein</t>
         </is>
       </c>
       <c r="C207" t="inlineStr">
         <is>
-          <t>Pan-Africanist leader and Ghana's first president.</t>
+          <t>American pop artist, known for his comic book-style artwork.</t>
         </is>
       </c>
       <c r="D207" t="inlineStr">
         <is>
-          <t>No</t>
+          <t>Yes</t>
         </is>
       </c>
       <c r="E207" t="inlineStr">
         <is>
-          <t>No</t>
+          <t>Yes</t>
         </is>
       </c>
       <c r="F207" t="inlineStr">
@@ -10317,7 +10317,7 @@
       <c r="I207" t="inlineStr"/>
       <c r="J207" t="inlineStr">
         <is>
-          <t>Please provide me with 10 long and interesting facts about Kwame Nkrumah. I have a youtube channel based on influential figures so this information must be accurate as my channel depends on it. Please make the output of the facts at least 700 words long. Thank you.</t>
+          <t>Please provide me with 10 long and interesting facts about Roy Lichtenstein. I have a youtube channel based on influential figures so this information must be accurate as my channel depends on it. Please make the output of the facts at least 700 words long. Thank you.</t>
         </is>
       </c>
     </row>

</xml_diff>